<commit_message>
database + stoplist 6.6
</commit_message>
<xml_diff>
--- a/excel/DATABASE_MENU_VENDITA.xlsx
+++ b/excel/DATABASE_MENU_VENDITA.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="491"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="491" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LE NOSTRE BIRRE" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="567">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="574">
   <si>
     <t>macro-category:</t>
   </si>
@@ -1695,9 +1695,6 @@
     <t>Salmone affumicato, insalata, cetrioli freschi, verdurine miste fresche, salsa tzatsiki. Servita con focaccia ai pomodorini e origano**.</t>
   </si>
   <si>
-    <t>Bocconcini di pollo alla griglia, formaggio di fossa di Sogliano DOP, insalata, verdurine miste fresche, pera a pezzetti, miele. Servita con focaccia ai pomodorini e origano**.</t>
-  </si>
-  <si>
     <t>soft drinks</t>
   </si>
   <si>
@@ -1729,6 +1726,30 @@
   </si>
   <si>
     <t xml:space="preserve">limited </t>
+  </si>
+  <si>
+    <t>Bocconcini di pollo, formaggio di fossa di Sogliano DOP, insalata, verdurine miste fresche, pera a pezzetti, miele. Servita con focaccia ai pomodorini e origano**.</t>
+  </si>
+  <si>
+    <t>wauwau</t>
+  </si>
+  <si>
+    <t>rouk</t>
+  </si>
+  <si>
+    <t>keepit</t>
+  </si>
+  <si>
+    <t>baconbbq</t>
+  </si>
+  <si>
+    <t>crispychick</t>
+  </si>
+  <si>
+    <t>johnbarley</t>
+  </si>
+  <si>
+    <t>jimmymc</t>
   </si>
 </sst>
 </file>
@@ -2904,27 +2925,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="9" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2985,6 +2985,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3340,8 +3361,8 @@
   </sheetPr>
   <dimension ref="A1:AG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView topLeftCell="L19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AC17" sqref="AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3781,7 +3802,7 @@
         <v>51</v>
       </c>
       <c r="F8" s="68" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>52</v>
@@ -3842,7 +3863,7 @@
         <v>56</v>
       </c>
       <c r="F9" s="68" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="G9" s="70" t="s">
         <v>57</v>
@@ -4090,31 +4111,31 @@
       <c r="V13" s="71"/>
       <c r="W13" s="71"/>
       <c r="X13" s="45"/>
-      <c r="Y13" s="311" t="s">
-        <v>559</v>
+      <c r="Y13" s="304" t="s">
+        <v>558</v>
       </c>
       <c r="Z13" s="288" t="s">
         <v>64</v>
       </c>
-      <c r="AA13" s="317">
+      <c r="AA13" s="310">
         <v>3.5</v>
       </c>
-      <c r="AB13" s="318" t="s">
-        <v>560</v>
+      <c r="AB13" s="311" t="s">
+        <v>559</v>
       </c>
       <c r="AC13" s="288" t="s">
         <v>60</v>
       </c>
-      <c r="AD13" s="319">
+      <c r="AD13" s="312">
         <v>6</v>
       </c>
-      <c r="AE13" s="311" t="s">
-        <v>561</v>
-      </c>
-      <c r="AF13" s="320" t="s">
+      <c r="AE13" s="304" t="s">
+        <v>560</v>
+      </c>
+      <c r="AF13" s="313" t="s">
         <v>41</v>
       </c>
-      <c r="AG13" s="321">
+      <c r="AG13" s="314">
         <v>12</v>
       </c>
     </row>
@@ -4154,28 +4175,28 @@
       <c r="Y14" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="Z14" s="295" t="s">
+      <c r="Z14" s="316" t="s">
         <v>64</v>
       </c>
-      <c r="AA14" s="296">
+      <c r="AA14" s="317">
         <v>3.5</v>
       </c>
-      <c r="AB14" s="297" t="s">
+      <c r="AB14" s="318" t="s">
         <v>78</v>
       </c>
-      <c r="AC14" s="295" t="s">
+      <c r="AC14" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="AD14" s="298">
+      <c r="AD14" s="319">
         <v>6</v>
       </c>
-      <c r="AE14" s="299" t="s">
+      <c r="AE14" s="320" t="s">
         <v>79</v>
       </c>
-      <c r="AF14" s="300" t="s">
+      <c r="AF14" s="321" t="s">
         <v>41</v>
       </c>
-      <c r="AG14" s="301">
+      <c r="AG14" s="322">
         <v>12</v>
       </c>
     </row>
@@ -4215,28 +4236,28 @@
       <c r="Y15" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="Z15" s="295" t="s">
+      <c r="Z15" s="316" t="s">
         <v>64</v>
       </c>
-      <c r="AA15" s="296">
+      <c r="AA15" s="317">
         <v>3.5</v>
       </c>
-      <c r="AB15" s="297" t="s">
+      <c r="AB15" s="318" t="s">
         <v>83</v>
       </c>
-      <c r="AC15" s="295" t="s">
+      <c r="AC15" s="316" t="s">
         <v>60</v>
       </c>
-      <c r="AD15" s="298">
+      <c r="AD15" s="319">
         <v>6</v>
       </c>
-      <c r="AE15" s="299" t="s">
+      <c r="AE15" s="320" t="s">
         <v>84</v>
       </c>
-      <c r="AF15" s="300" t="s">
+      <c r="AF15" s="321" t="s">
         <v>41</v>
       </c>
-      <c r="AG15" s="301">
+      <c r="AG15" s="322">
         <v>12.5</v>
       </c>
     </row>
@@ -4537,10 +4558,10 @@
   </sheetPr>
   <dimension ref="A1:AG47"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="Y23" sqref="Y23"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4775,7 +4796,7 @@
       <c r="W5" s="183"/>
       <c r="X5" s="183"/>
       <c r="Y5" s="178" t="s">
-        <v>531</v>
+        <v>569</v>
       </c>
       <c r="Z5" s="180"/>
       <c r="AA5" s="181">
@@ -4822,7 +4843,7 @@
       <c r="W6" s="183"/>
       <c r="X6" s="183"/>
       <c r="Y6" s="186" t="s">
-        <v>530</v>
+        <v>568</v>
       </c>
       <c r="Z6" s="56"/>
       <c r="AA6" s="181">
@@ -4867,7 +4888,7 @@
       <c r="W7" s="183"/>
       <c r="X7" s="183"/>
       <c r="Y7" s="196" t="s">
-        <v>529</v>
+        <v>570</v>
       </c>
       <c r="Z7" s="56"/>
       <c r="AA7" s="181">
@@ -4910,7 +4931,7 @@
       <c r="W8" s="285"/>
       <c r="X8" s="285"/>
       <c r="Y8" s="196" t="s">
-        <v>528</v>
+        <v>567</v>
       </c>
       <c r="Z8" s="56"/>
       <c r="AA8" s="181">
@@ -4960,7 +4981,7 @@
       <c r="W9" s="285"/>
       <c r="X9" s="285"/>
       <c r="Y9" s="196" t="s">
-        <v>532</v>
+        <v>571</v>
       </c>
       <c r="Z9" s="76"/>
       <c r="AA9" s="209">
@@ -5048,7 +5069,7 @@
       <c r="W11" s="192"/>
       <c r="X11" s="192"/>
       <c r="Y11" s="196" t="s">
-        <v>533</v>
+        <v>572</v>
       </c>
       <c r="Z11" s="56"/>
       <c r="AA11" s="181">
@@ -5302,7 +5323,9 @@
       <c r="O17" s="195"/>
       <c r="P17" s="195"/>
       <c r="Q17" s="195"/>
-      <c r="R17" s="195"/>
+      <c r="R17" s="195">
+        <v>1</v>
+      </c>
       <c r="S17" s="195">
         <v>1</v>
       </c>
@@ -5355,7 +5378,7 @@
       <c r="W18" s="193"/>
       <c r="X18" s="193"/>
       <c r="Y18" s="196" t="s">
-        <v>535</v>
+        <v>573</v>
       </c>
       <c r="Z18" s="56"/>
       <c r="AA18" s="181">
@@ -5374,19 +5397,27 @@
         <v>551</v>
       </c>
       <c r="G19" s="187" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="H19" s="261"/>
-      <c r="I19" s="193"/>
+      <c r="I19" s="193">
+        <v>1</v>
+      </c>
       <c r="J19" s="193"/>
-      <c r="K19" s="193"/>
+      <c r="K19" s="193">
+        <v>1</v>
+      </c>
       <c r="L19" s="193"/>
-      <c r="M19" s="193"/>
+      <c r="M19" s="193">
+        <v>1</v>
+      </c>
       <c r="N19" s="193"/>
       <c r="O19" s="193"/>
       <c r="P19" s="193"/>
       <c r="Q19" s="193"/>
-      <c r="R19" s="193"/>
+      <c r="R19" s="193">
+        <v>1</v>
+      </c>
       <c r="S19" s="193"/>
       <c r="T19" s="193"/>
       <c r="U19" s="193"/>
@@ -5394,7 +5425,7 @@
       <c r="W19" s="193"/>
       <c r="X19" s="193"/>
       <c r="Y19" s="196" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="Z19" s="76"/>
       <c r="AA19" s="209">
@@ -5442,7 +5473,7 @@
       <c r="E21" s="76" t="s">
         <v>361</v>
       </c>
-      <c r="F21" s="311" t="s">
+      <c r="F21" s="304" t="s">
         <v>370</v>
       </c>
       <c r="G21" s="91"/>
@@ -5479,7 +5510,7 @@
       <c r="E22" s="76" t="s">
         <v>362</v>
       </c>
-      <c r="F22" s="311" t="s">
+      <c r="F22" s="304" t="s">
         <v>371</v>
       </c>
       <c r="G22" s="91"/>
@@ -5516,7 +5547,7 @@
       <c r="E23" s="76" t="s">
         <v>483</v>
       </c>
-      <c r="F23" s="311" t="s">
+      <c r="F23" s="304" t="s">
         <v>484</v>
       </c>
       <c r="G23" s="91"/>
@@ -5549,7 +5580,7 @@
       <c r="E24" s="76" t="s">
         <v>485</v>
       </c>
-      <c r="F24" s="311" t="s">
+      <c r="F24" s="304" t="s">
         <v>497</v>
       </c>
       <c r="G24" s="91"/>
@@ -5582,7 +5613,7 @@
       <c r="E25" s="76" t="s">
         <v>487</v>
       </c>
-      <c r="F25" s="311" t="s">
+      <c r="F25" s="304" t="s">
         <v>498</v>
       </c>
       <c r="G25" s="91"/>
@@ -5615,7 +5646,7 @@
       <c r="E26" s="76" t="s">
         <v>491</v>
       </c>
-      <c r="F26" s="311" t="s">
+      <c r="F26" s="304" t="s">
         <v>499</v>
       </c>
       <c r="G26" s="91"/>
@@ -5648,7 +5679,7 @@
       <c r="E27" s="76" t="s">
         <v>488</v>
       </c>
-      <c r="F27" s="311" t="s">
+      <c r="F27" s="304" t="s">
         <v>489</v>
       </c>
       <c r="G27" s="91"/>
@@ -5681,7 +5712,7 @@
       <c r="E28" s="76" t="s">
         <v>538</v>
       </c>
-      <c r="F28" s="311" t="s">
+      <c r="F28" s="304" t="s">
         <v>490</v>
       </c>
       <c r="G28" s="91"/>
@@ -5714,7 +5745,7 @@
       <c r="E29" s="76" t="s">
         <v>332</v>
       </c>
-      <c r="F29" s="311" t="s">
+      <c r="F29" s="304" t="s">
         <v>341</v>
       </c>
       <c r="G29" s="219"/>
@@ -5751,7 +5782,7 @@
       <c r="E30" s="76" t="s">
         <v>333</v>
       </c>
-      <c r="F30" s="311" t="s">
+      <c r="F30" s="304" t="s">
         <v>348</v>
       </c>
       <c r="G30" s="219"/>
@@ -5790,7 +5821,7 @@
       <c r="E31" s="76" t="s">
         <v>334</v>
       </c>
-      <c r="F31" s="311" t="s">
+      <c r="F31" s="304" t="s">
         <v>342</v>
       </c>
       <c r="G31" s="219"/>
@@ -5829,7 +5860,7 @@
       <c r="E32" s="76" t="s">
         <v>335</v>
       </c>
-      <c r="F32" s="311" t="s">
+      <c r="F32" s="304" t="s">
         <v>343</v>
       </c>
       <c r="G32" s="219"/>
@@ -5868,7 +5899,7 @@
       <c r="E33" s="76" t="s">
         <v>336</v>
       </c>
-      <c r="F33" s="311" t="s">
+      <c r="F33" s="304" t="s">
         <v>492</v>
       </c>
       <c r="G33" s="219"/>
@@ -5905,7 +5936,7 @@
       <c r="E34" s="76" t="s">
         <v>337</v>
       </c>
-      <c r="F34" s="311" t="s">
+      <c r="F34" s="304" t="s">
         <v>344</v>
       </c>
       <c r="G34" s="219"/>
@@ -5942,7 +5973,7 @@
       <c r="E35" s="76" t="s">
         <v>338</v>
       </c>
-      <c r="F35" s="311" t="s">
+      <c r="F35" s="304" t="s">
         <v>345</v>
       </c>
       <c r="G35" s="219"/>
@@ -5979,7 +6010,7 @@
       <c r="E36" s="76" t="s">
         <v>339</v>
       </c>
-      <c r="F36" s="311" t="s">
+      <c r="F36" s="304" t="s">
         <v>346</v>
       </c>
       <c r="G36" s="219"/>
@@ -6016,7 +6047,7 @@
       <c r="E37" s="76" t="s">
         <v>340</v>
       </c>
-      <c r="F37" s="311" t="s">
+      <c r="F37" s="304" t="s">
         <v>347</v>
       </c>
       <c r="G37" s="219"/>
@@ -6053,7 +6084,7 @@
       <c r="E38" s="76" t="s">
         <v>493</v>
       </c>
-      <c r="F38" s="311" t="s">
+      <c r="F38" s="304" t="s">
         <v>496</v>
       </c>
       <c r="G38" s="253"/>
@@ -6090,7 +6121,7 @@
       <c r="E39" s="76" t="s">
         <v>494</v>
       </c>
-      <c r="F39" s="311" t="s">
+      <c r="F39" s="304" t="s">
         <v>495</v>
       </c>
       <c r="G39" s="253"/>
@@ -6123,7 +6154,7 @@
       <c r="E40" s="76" t="s">
         <v>349</v>
       </c>
-      <c r="F40" s="311" t="s">
+      <c r="F40" s="304" t="s">
         <v>350</v>
       </c>
       <c r="G40" s="219"/>
@@ -6164,7 +6195,7 @@
       <c r="E41" s="76" t="s">
         <v>363</v>
       </c>
-      <c r="F41" s="311" t="s">
+      <c r="F41" s="304" t="s">
         <v>351</v>
       </c>
       <c r="G41" s="219"/>
@@ -6203,7 +6234,7 @@
       <c r="E42" s="76" t="s">
         <v>358</v>
       </c>
-      <c r="F42" s="311" t="s">
+      <c r="F42" s="304" t="s">
         <v>357</v>
       </c>
       <c r="G42" s="219"/>
@@ -6242,7 +6273,7 @@
       <c r="E43" s="76" t="s">
         <v>359</v>
       </c>
-      <c r="F43" s="311" t="s">
+      <c r="F43" s="304" t="s">
         <v>360</v>
       </c>
       <c r="G43" s="219"/>
@@ -6281,7 +6312,7 @@
       <c r="E44" s="76" t="s">
         <v>372</v>
       </c>
-      <c r="F44" s="311" t="s">
+      <c r="F44" s="304" t="s">
         <v>373</v>
       </c>
       <c r="G44" s="219"/>
@@ -6322,7 +6353,7 @@
       <c r="E45" s="76" t="s">
         <v>352</v>
       </c>
-      <c r="F45" s="311" t="s">
+      <c r="F45" s="304" t="s">
         <v>356</v>
       </c>
       <c r="G45" s="256"/>
@@ -6361,7 +6392,7 @@
       <c r="E46" s="76" t="s">
         <v>353</v>
       </c>
-      <c r="F46" s="311" t="s">
+      <c r="F46" s="304" t="s">
         <v>355</v>
       </c>
       <c r="G46" s="256"/>
@@ -6393,14 +6424,14 @@
       </c>
     </row>
     <row r="47" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A47" s="302"/>
+      <c r="A47" s="295"/>
       <c r="B47" s="96"/>
-      <c r="C47" s="303"/>
+      <c r="C47" s="296"/>
       <c r="D47" s="208"/>
       <c r="E47" s="76" t="s">
         <v>354</v>
       </c>
-      <c r="F47" s="311" t="s">
+      <c r="F47" s="304" t="s">
         <v>486</v>
       </c>
       <c r="G47" s="256"/>
@@ -6444,8 +6475,8 @@
   </sheetPr>
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6572,9 +6603,9 @@
       </c>
     </row>
     <row r="4" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="312"/>
-      <c r="B4" s="312"/>
-      <c r="C4" s="313" t="s">
+      <c r="A4" s="305"/>
+      <c r="B4" s="305"/>
+      <c r="C4" s="306" t="s">
         <v>451</v>
       </c>
       <c r="D4" s="294" t="s">
@@ -6583,7 +6614,7 @@
       <c r="E4" s="167"/>
       <c r="F4" s="23"/>
       <c r="G4" s="168"/>
-      <c r="H4" s="314" t="s">
+      <c r="H4" s="307" t="s">
         <v>19</v>
       </c>
       <c r="I4" s="180" t="s">
@@ -6639,8 +6670,8 @@
       <c r="AA4" s="95"/>
     </row>
     <row r="5" spans="1:28" ht="30" x14ac:dyDescent="0.3">
-      <c r="A5" s="312"/>
-      <c r="B5" s="312"/>
+      <c r="A5" s="305"/>
+      <c r="B5" s="305"/>
       <c r="C5" s="96"/>
       <c r="D5" s="2"/>
       <c r="E5" s="180" t="s">
@@ -6649,7 +6680,7 @@
       <c r="F5" s="180" t="s">
         <v>464</v>
       </c>
-      <c r="G5" s="315" t="s">
+      <c r="G5" s="308" t="s">
         <v>468</v>
       </c>
       <c r="H5" s="132"/>
@@ -6677,13 +6708,13 @@
       <c r="X5" s="208"/>
       <c r="Y5" s="95"/>
       <c r="Z5" s="95"/>
-      <c r="AA5" s="316">
+      <c r="AA5" s="309">
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:28" ht="30" x14ac:dyDescent="0.3">
-      <c r="A6" s="312"/>
-      <c r="B6" s="312"/>
+      <c r="A6" s="305"/>
+      <c r="B6" s="305"/>
       <c r="C6" s="95"/>
       <c r="D6" s="95"/>
       <c r="E6" s="180" t="s">
@@ -6692,7 +6723,7 @@
       <c r="F6" s="180" t="s">
         <v>462</v>
       </c>
-      <c r="G6" s="315" t="s">
+      <c r="G6" s="308" t="s">
         <v>469</v>
       </c>
       <c r="H6" s="132"/>
@@ -6722,13 +6753,13 @@
       <c r="X6" s="208"/>
       <c r="Y6" s="95"/>
       <c r="Z6" s="95"/>
-      <c r="AA6" s="316">
+      <c r="AA6" s="309">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:28" ht="30" x14ac:dyDescent="0.3">
-      <c r="A7" s="312"/>
-      <c r="B7" s="312"/>
+      <c r="A7" s="305"/>
+      <c r="B7" s="305"/>
       <c r="C7" s="95"/>
       <c r="D7" s="95"/>
       <c r="E7" s="180" t="s">
@@ -6737,7 +6768,7 @@
       <c r="F7" s="180" t="s">
         <v>526</v>
       </c>
-      <c r="G7" s="315" t="s">
+      <c r="G7" s="308" t="s">
         <v>470</v>
       </c>
       <c r="H7" s="132"/>
@@ -6765,13 +6796,13 @@
       <c r="X7" s="208"/>
       <c r="Y7" s="95"/>
       <c r="Z7" s="95"/>
-      <c r="AA7" s="316">
+      <c r="AA7" s="309">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:28" ht="45" x14ac:dyDescent="0.3">
-      <c r="A8" s="312"/>
-      <c r="B8" s="312"/>
+      <c r="A8" s="305"/>
+      <c r="B8" s="305"/>
       <c r="C8" s="95"/>
       <c r="D8" s="95"/>
       <c r="E8" s="180" t="s">
@@ -6780,7 +6811,7 @@
       <c r="F8" s="180" t="s">
         <v>463</v>
       </c>
-      <c r="G8" s="315" t="s">
+      <c r="G8" s="308" t="s">
         <v>471</v>
       </c>
       <c r="H8" s="132"/>
@@ -6808,13 +6839,13 @@
       <c r="X8" s="208"/>
       <c r="Y8" s="95"/>
       <c r="Z8" s="95"/>
-      <c r="AA8" s="316">
+      <c r="AA8" s="309">
         <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:28" ht="45" x14ac:dyDescent="0.3">
-      <c r="A9" s="312"/>
-      <c r="B9" s="312"/>
+      <c r="A9" s="305"/>
+      <c r="B9" s="305"/>
       <c r="C9" s="95"/>
       <c r="D9" s="95"/>
       <c r="E9" s="180" t="s">
@@ -6823,7 +6854,7 @@
       <c r="F9" s="180" t="s">
         <v>466</v>
       </c>
-      <c r="G9" s="315" t="s">
+      <c r="G9" s="308" t="s">
         <v>472</v>
       </c>
       <c r="H9" s="132"/>
@@ -6853,13 +6884,13 @@
       <c r="X9" s="208"/>
       <c r="Y9" s="95"/>
       <c r="Z9" s="95"/>
-      <c r="AA9" s="316">
+      <c r="AA9" s="309">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:28" ht="45" x14ac:dyDescent="0.3">
-      <c r="A10" s="312"/>
-      <c r="B10" s="312"/>
+      <c r="A10" s="305"/>
+      <c r="B10" s="305"/>
       <c r="C10" s="95"/>
       <c r="D10" s="95"/>
       <c r="E10" s="180" t="s">
@@ -6868,7 +6899,7 @@
       <c r="F10" s="180" t="s">
         <v>525</v>
       </c>
-      <c r="G10" s="315" t="s">
+      <c r="G10" s="308" t="s">
         <v>473</v>
       </c>
       <c r="H10" s="132"/>
@@ -6896,13 +6927,13 @@
       <c r="X10" s="208"/>
       <c r="Y10" s="95"/>
       <c r="Z10" s="95"/>
-      <c r="AA10" s="316">
+      <c r="AA10" s="309">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:28" ht="60" x14ac:dyDescent="0.3">
-      <c r="A11" s="312"/>
-      <c r="B11" s="312"/>
+      <c r="A11" s="305"/>
+      <c r="B11" s="305"/>
       <c r="C11" s="95"/>
       <c r="D11" s="95"/>
       <c r="E11" s="180" t="s">
@@ -6911,7 +6942,7 @@
       <c r="F11" s="180" t="s">
         <v>465</v>
       </c>
-      <c r="G11" s="315" t="s">
+      <c r="G11" s="308" t="s">
         <v>474</v>
       </c>
       <c r="H11" s="132"/>
@@ -6945,13 +6976,13 @@
       <c r="X11" s="208"/>
       <c r="Y11" s="95"/>
       <c r="Z11" s="95"/>
-      <c r="AA11" s="316">
+      <c r="AA11" s="309">
         <v>3</v>
       </c>
     </row>
     <row r="12" spans="1:28" ht="60" x14ac:dyDescent="0.3">
-      <c r="A12" s="312"/>
-      <c r="B12" s="312"/>
+      <c r="A12" s="305"/>
+      <c r="B12" s="305"/>
       <c r="C12" s="95"/>
       <c r="D12" s="95"/>
       <c r="E12" s="180" t="s">
@@ -6960,7 +6991,7 @@
       <c r="F12" s="180" t="s">
         <v>467</v>
       </c>
-      <c r="G12" s="315" t="s">
+      <c r="G12" s="308" t="s">
         <v>475</v>
       </c>
       <c r="H12" s="132"/>
@@ -6996,13 +7027,13 @@
       <c r="X12" s="208"/>
       <c r="Y12" s="95"/>
       <c r="Z12" s="95"/>
-      <c r="AA12" s="316">
+      <c r="AA12" s="309">
         <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="312"/>
-      <c r="B13" s="312"/>
+      <c r="A13" s="305"/>
+      <c r="B13" s="305"/>
       <c r="C13" s="95"/>
       <c r="D13" s="95"/>
       <c r="E13" s="180" t="s">
@@ -7011,7 +7042,7 @@
       <c r="F13" s="180" t="s">
         <v>524</v>
       </c>
-      <c r="G13" s="315" t="s">
+      <c r="G13" s="308" t="s">
         <v>476</v>
       </c>
       <c r="H13" s="132"/>
@@ -7045,7 +7076,7 @@
       <c r="X13" s="208"/>
       <c r="Y13" s="95"/>
       <c r="Z13" s="95"/>
-      <c r="AA13" s="316">
+      <c r="AA13" s="309">
         <v>3</v>
       </c>
     </row>
@@ -7055,7 +7086,7 @@
       <c r="C14" s="198" t="s">
         <v>515</v>
       </c>
-      <c r="D14" s="310" t="s">
+      <c r="D14" s="303" t="s">
         <v>216</v>
       </c>
       <c r="E14" s="76"/>
@@ -7094,19 +7125,19 @@
         <v>500</v>
       </c>
       <c r="G15" s="70" t="s">
-        <v>555</v>
+        <v>566</v>
       </c>
       <c r="H15" s="250"/>
       <c r="I15" s="208"/>
       <c r="J15" s="208"/>
-      <c r="K15" s="208">
-        <v>1</v>
-      </c>
-      <c r="L15" s="208"/>
-      <c r="M15" s="208">
-        <v>1</v>
-      </c>
-      <c r="N15" s="208"/>
+      <c r="K15" s="192">
+        <v>1</v>
+      </c>
+      <c r="L15" s="192"/>
+      <c r="M15" s="192">
+        <v>1</v>
+      </c>
+      <c r="N15" s="192"/>
       <c r="O15" s="208"/>
       <c r="P15" s="208"/>
       <c r="Q15" s="208"/>
@@ -7144,16 +7175,18 @@
       <c r="J16" s="192">
         <v>1</v>
       </c>
-      <c r="K16" s="208">
-        <v>1</v>
-      </c>
-      <c r="L16" s="208"/>
-      <c r="M16" s="208"/>
-      <c r="N16" s="208"/>
+      <c r="K16" s="192">
+        <v>1</v>
+      </c>
+      <c r="L16" s="192"/>
+      <c r="M16" s="192"/>
+      <c r="N16" s="192"/>
       <c r="O16" s="208"/>
       <c r="P16" s="208"/>
       <c r="Q16" s="208"/>
-      <c r="R16" s="208"/>
+      <c r="R16" s="192">
+        <v>1</v>
+      </c>
       <c r="S16" s="208"/>
       <c r="T16" s="208"/>
       <c r="U16" s="208"/>
@@ -7183,14 +7216,14 @@
       <c r="H17" s="250"/>
       <c r="I17" s="208"/>
       <c r="J17" s="208"/>
-      <c r="K17" s="208">
-        <v>1</v>
-      </c>
-      <c r="L17" s="208"/>
-      <c r="M17" s="208">
-        <v>1</v>
-      </c>
-      <c r="N17" s="208">
+      <c r="K17" s="192">
+        <v>1</v>
+      </c>
+      <c r="L17" s="192"/>
+      <c r="M17" s="192">
+        <v>1</v>
+      </c>
+      <c r="N17" s="192">
         <v>1</v>
       </c>
       <c r="O17" s="208"/>
@@ -7226,14 +7259,14 @@
       <c r="H18" s="289"/>
       <c r="I18" s="208"/>
       <c r="J18" s="208"/>
-      <c r="K18" s="208">
-        <v>1</v>
-      </c>
-      <c r="L18" s="208"/>
+      <c r="K18" s="192">
+        <v>1</v>
+      </c>
+      <c r="L18" s="192"/>
       <c r="M18" s="192">
         <v>1</v>
       </c>
-      <c r="N18" s="208"/>
+      <c r="N18" s="192"/>
       <c r="O18" s="208"/>
       <c r="P18" s="208"/>
       <c r="Q18" s="208"/>
@@ -7584,7 +7617,7 @@
       <c r="C27" s="211" t="s">
         <v>221</v>
       </c>
-      <c r="D27" s="310" t="s">
+      <c r="D27" s="303" t="s">
         <v>222</v>
       </c>
       <c r="H27" s="250"/>
@@ -7667,7 +7700,7 @@
       <c r="G29" s="212" t="s">
         <v>436</v>
       </c>
-      <c r="H29" s="309"/>
+      <c r="H29" s="302"/>
       <c r="I29" s="208"/>
       <c r="J29" s="86">
         <v>1</v>
@@ -7709,17 +7742,15 @@
       <c r="F30" s="76" t="s">
         <v>550</v>
       </c>
-      <c r="G30" s="322" t="s">
-        <v>562</v>
+      <c r="G30" s="315" t="s">
+        <v>561</v>
       </c>
       <c r="H30" s="199"/>
       <c r="I30" s="208"/>
       <c r="J30" s="208"/>
-      <c r="K30" s="208">
-        <v>1</v>
-      </c>
+      <c r="K30" s="192"/>
       <c r="L30" s="208"/>
-      <c r="M30" s="208">
+      <c r="M30" s="192">
         <v>1</v>
       </c>
       <c r="N30" s="208"/>
@@ -7727,7 +7758,9 @@
       <c r="P30" s="208"/>
       <c r="Q30" s="208"/>
       <c r="R30" s="208"/>
-      <c r="S30" s="208"/>
+      <c r="S30" s="192">
+        <v>1</v>
+      </c>
       <c r="T30" s="208"/>
       <c r="U30" s="208"/>
       <c r="V30" s="208"/>
@@ -7752,7 +7785,7 @@
   </sheetPr>
   <dimension ref="A1:AG50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
@@ -7928,7 +7961,7 @@
         <v>223</v>
       </c>
       <c r="D4" s="134" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="H4" s="257" t="s">
         <v>19</v>
@@ -8739,7 +8772,7 @@
         <v>506</v>
       </c>
       <c r="D22" s="227" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="E22" s="284"/>
       <c r="F22" s="284"/>
@@ -9478,7 +9511,7 @@
         <v>285</v>
       </c>
       <c r="D39" s="236" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="E39" s="15"/>
       <c r="G39" s="15"/>
@@ -9977,8 +10010,8 @@
   </sheetPr>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10221,10 +10254,10 @@
       <c r="A5" s="29"/>
       <c r="B5" s="126"/>
       <c r="C5" s="15"/>
-      <c r="E5" s="304" t="s">
+      <c r="E5" s="297" t="s">
         <v>410</v>
       </c>
-      <c r="F5" s="304" t="s">
+      <c r="F5" s="297" t="s">
         <v>93</v>
       </c>
       <c r="G5" s="127"/>
@@ -10240,7 +10273,7 @@
       <c r="Q5" s="274"/>
       <c r="R5" s="274"/>
       <c r="S5" s="274"/>
-      <c r="T5" s="308">
+      <c r="T5" s="301">
         <v>1</v>
       </c>
       <c r="U5" s="274"/>
@@ -10270,10 +10303,10 @@
       <c r="B6" s="29"/>
       <c r="C6" s="58"/>
       <c r="D6" s="58"/>
-      <c r="E6" s="305" t="s">
+      <c r="E6" s="298" t="s">
         <v>411</v>
       </c>
-      <c r="F6" s="305" t="s">
+      <c r="F6" s="298" t="s">
         <v>96</v>
       </c>
       <c r="G6" s="131"/>
@@ -10289,7 +10322,7 @@
       <c r="Q6" s="274"/>
       <c r="R6" s="274"/>
       <c r="S6" s="274"/>
-      <c r="T6" s="308">
+      <c r="T6" s="301">
         <v>1</v>
       </c>
       <c r="U6" s="274"/>
@@ -10319,10 +10352,10 @@
       <c r="B7" s="29"/>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
-      <c r="E7" s="306" t="s">
+      <c r="E7" s="299" t="s">
         <v>412</v>
       </c>
-      <c r="F7" s="306" t="s">
+      <c r="F7" s="299" t="s">
         <v>97</v>
       </c>
       <c r="G7" s="133"/>
@@ -10338,7 +10371,7 @@
       <c r="Q7" s="274"/>
       <c r="R7" s="274"/>
       <c r="S7" s="274"/>
-      <c r="T7" s="308">
+      <c r="T7" s="301">
         <v>1</v>
       </c>
       <c r="U7" s="274"/>
@@ -10368,10 +10401,10 @@
       <c r="B8" s="29"/>
       <c r="C8" s="57"/>
       <c r="D8" s="57"/>
-      <c r="E8" s="305" t="s">
+      <c r="E8" s="298" t="s">
         <v>413</v>
       </c>
-      <c r="F8" s="305" t="s">
+      <c r="F8" s="298" t="s">
         <v>98</v>
       </c>
       <c r="G8" s="133"/>
@@ -10387,7 +10420,7 @@
       <c r="Q8" s="274"/>
       <c r="R8" s="274"/>
       <c r="S8" s="274"/>
-      <c r="T8" s="308">
+      <c r="T8" s="301">
         <v>1</v>
       </c>
       <c r="U8" s="274"/>
@@ -10417,10 +10450,10 @@
       <c r="B9" s="29"/>
       <c r="C9" s="57"/>
       <c r="D9" s="57"/>
-      <c r="E9" s="305" t="s">
+      <c r="E9" s="298" t="s">
         <v>414</v>
       </c>
-      <c r="F9" s="305" t="s">
+      <c r="F9" s="298" t="s">
         <v>99</v>
       </c>
       <c r="G9" s="78"/>
@@ -10436,7 +10469,7 @@
       <c r="Q9" s="274"/>
       <c r="R9" s="274"/>
       <c r="S9" s="274"/>
-      <c r="T9" s="308">
+      <c r="T9" s="301">
         <v>1</v>
       </c>
       <c r="U9" s="274"/>
@@ -11176,7 +11209,7 @@
       <c r="AC25" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="AD25" s="307">
+      <c r="AD25" s="300">
         <v>4.5</v>
       </c>
       <c r="AE25" s="15"/>
@@ -11221,7 +11254,7 @@
       <c r="AC26" s="138" t="s">
         <v>106</v>
       </c>
-      <c r="AD26" s="307">
+      <c r="AD26" s="300">
         <v>4.5</v>
       </c>
       <c r="AE26" s="15"/>

</xml_diff>

<commit_message>
Correzione colori e scritte
</commit_message>
<xml_diff>
--- a/excel/DATABASE_MENU_VENDITA.xlsx
+++ b/excel/DATABASE_MENU_VENDITA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Virginia\Desktop\JB\menu\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\JC\Desktop\menu-stable\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323AC7F1-C7C7-4EFD-B500-DC2991AC8D8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="707"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="707" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LE NOSTRE BIRRE" sheetId="1" r:id="rId1"/>
@@ -1359,15 +1360,6 @@
     <t>Panino farcito con burger di chianina**, scalogno cotto, bacon, formaggio di fossa di Sogliano DOP, aceto balsamico di Modena IGP, insalata, pomodoro. Servito con patate al forno * e salse.</t>
   </si>
   <si>
-    <t>Panino farcito con bocconcini di pollo alle spezie indiane, salsa alla menta, cipolla rossa cotta, verdurine miste cotte. Servito con patate al forno * e salse.</t>
-  </si>
-  <si>
-    <t>Panino farcito con bocconcini di pollo alle arachidi, scalogno cotto, verdurine miste cotte. Servito con patate al forno * e salse.</t>
-  </si>
-  <si>
-    <t>Panino farcito con polpettine di ceci*, salsa all'avocado con lime**, pepe rosa in grani, verdurine miste fresche, insalata, pomodoro. Servito con patate al forno * e salse.</t>
-  </si>
-  <si>
     <t>Panino farcito con burger di angus**, cipolla rossa cotta, salsa chimichurri, insalata, pomodoro. Servito con patate al forno * e salse.</t>
   </si>
   <si>
@@ -1377,9 +1369,6 @@
     <t>Panino farcito con chili, guacamole, insalata, pomodoro. Servito con patate al forno * e salse.</t>
   </si>
   <si>
-    <t>Panino farcito con salmone affumicato, salsa all' avocado con lime**, pepe rosa in grani, verdurine miste fresche, cetriolo fresco, insalata. Servito con patate al forno * e salse.</t>
-  </si>
-  <si>
     <t>HAPPY HOUR!</t>
   </si>
   <si>
@@ -1440,24 +1429,6 @@
     <t>2 panini dal nostro menù in versione mini (SANDOKAN &amp; SHERAZADE), nachos, salsa dip, patate al forno*.</t>
   </si>
   <si>
-    <t>2 panini dal nostro menù in versione mini (BACON &amp; BBQ &amp; JOHN BARLEYCORN), nachos, salsa dip, focaccia con pomodorini fatta in casa**, patate al forno*, 2 anelli di cipolla*.</t>
-  </si>
-  <si>
-    <t>2 panini dal nostro menù in versione mini (RAMA &amp; JIMMYMCCURRY), nachos, salsa dip, focaccia con pomodorini fatta in casa**, patate al forno*, 2 anelli di cipolla*.</t>
-  </si>
-  <si>
-    <t>2 panini dal nostro menù in versione mini (SANDOKAN &amp; SHERAZADE), nachos, salsa dip, focaccia con pomodorini fatta in casa**, patate al forno*, 2 anelli di cipolla*.</t>
-  </si>
-  <si>
-    <t>2 panini dal nostro menù in versione mini (BACON &amp; BBQ &amp; JOHN BARLEYCORN), nachos, salsa dip,focaccia con pomodorini fatta in casa**, patate al forno*, 2 anelli di cipolla*, 2 olive all'ascolana*, 1 aletta di pollo*.</t>
-  </si>
-  <si>
-    <t>2 panini dal nostro menù in versione mini (RAMA &amp; JIMMYMCCURRY), nachos, salsa dip, focaccia con pomodorini fatta in casa**, patate al forno*, 2 anelli di cipolla*, 2 olive all'ascolana*, 1 aletta di pollo*.</t>
-  </si>
-  <si>
-    <t>2 panini dal nostro menù in versione mini (SANDOKAN &amp; SHERAZADE), nachos, salsa dip, focaccia con pomodorini fatta in casa**, patate al forno*, 2 anelli di cipolla*, 2 olive all'ascolana*, 1 aletta di pollo*.</t>
-  </si>
-  <si>
     <t>rama</t>
   </si>
   <si>
@@ -1683,15 +1654,6 @@
     <t>limited edition</t>
   </si>
   <si>
-    <t>Polpettine di ceci*, insalata, pomodoro, cetrioli freschi, verdurine miste fresche, salsa chimichurri. Servita con focaccia ai pomodorini e origano**.</t>
-  </si>
-  <si>
-    <t>Bacon croccante, feta a dadini, pomodoro, insalata, cetrioli freschi. Servita con focaccia ai pomodorini e origano**.</t>
-  </si>
-  <si>
-    <t>Salmone affumicato, insalata, cetrioli freschi, verdurine miste fresche, salsa tzatsiki. Servita con focaccia ai pomodorini e origano**.</t>
-  </si>
-  <si>
     <t>soft drinks</t>
   </si>
   <si>
@@ -1719,9 +1681,6 @@
     <t xml:space="preserve">limited </t>
   </si>
   <si>
-    <t>Bocconcini di pollo, formaggio di fossa di Sogliano DOP, insalata, verdurine miste fresche, pera a pezzetti, miele. Servita con focaccia ai pomodorini e origano**.</t>
-  </si>
-  <si>
     <t>wauwau</t>
   </si>
   <si>
@@ -1750,18 +1709,60 @@
   </si>
   <si>
     <t>Un dolce al cucchiaio diverso ogni mese. Per il mese di LUGLIO: sorbetto all'anguria.</t>
+  </si>
+  <si>
+    <t>Panino farcito con bocconcini di pollo alle spezie indiane, menta fresca, cipolla rossa cotta, verdure miste. Servito con patate al forno * e salse.</t>
+  </si>
+  <si>
+    <t>Panino farcito con salmone affumicato, salsa all' avocado con lime**, pepe rosa in grani, verdure miste, cetriolo fresco, insalata. Servito con patate al forno * e salse.</t>
+  </si>
+  <si>
+    <t>Panino farcito con bocconcini di pollo alle arachidi, scalogno cotto, verdure miste. Servito con patate al forno * e salse.</t>
+  </si>
+  <si>
+    <t>Panino farcito con polpettine di ceci*, salsa all'avocado con lime**, pepe rosa in grani, verdure miste, insalata, pomodoro. Servito con patate al forno * e salse.</t>
+  </si>
+  <si>
+    <t>Polpettine di ceci*, insalata, pomodoro, cetrioli freschi, verdure miste, salsa chimichurri. Servita con focaccia fatta in casa**.</t>
+  </si>
+  <si>
+    <t>Salmone affumicato, insalata, cetrioli freschi, verdure miste, salsa tzatsiki. Servita con focaccia fatta in casa**.</t>
+  </si>
+  <si>
+    <t>Bacon croccante, feta a dadini, pomodoro, insalata, cetrioli freschi. Servita con focaccia fatta in casa**.</t>
+  </si>
+  <si>
+    <t>2 panini dal nostro menù in versione mini (BACON &amp; BBQ &amp; JOHN BARLEYCORN), nachos, salsa dip, focaccia fatta in casa**, patate al forno*, 2 anelli di cipolla*.</t>
+  </si>
+  <si>
+    <t>2 panini dal nostro menù in versione mini (RAMA &amp; JIMMYMCCURRY), nachos, salsa dip, focaccia fatta in casa**, patate al forno*, 2 anelli di cipolla*.</t>
+  </si>
+  <si>
+    <t>2 panini dal nostro menù in versione mini (SANDOKAN &amp; SHERAZADE), nachos, salsa dip, focaccia fatta in casa**, patate al forno*, 2 anelli di cipolla*.</t>
+  </si>
+  <si>
+    <t>2 panini dal nostro menù in versione mini (BACON &amp; BBQ &amp; JOHN BARLEYCORN), nachos, salsa dip, focaccia fatta in casa**, patate al forno*, 2 anelli di cipolla*, 2 olive all'ascolana*, 1 aletta di pollo*.</t>
+  </si>
+  <si>
+    <t>2 panini dal nostro menù in versione mini (RAMA &amp; JIMMYMCCURRY), nachos, salsa dip, focaccia fatta in casa**, patate al forno*, 2 anelli di cipolla*, 2 olive all'ascolana*, 1 aletta di pollo*.</t>
+  </si>
+  <si>
+    <t>2 panini dal nostro menù in versione mini (SANDOKAN &amp; SHERAZADE), nachos, salsa dip, focaccia fatta in casa**, patate al forno*, 2 anelli di cipolla*, 2 olive all'ascolana*, 1 aletta di pollo*.</t>
+  </si>
+  <si>
+    <t>Bocconcini di pollo, formaggio di fossa di Sogliano DOP, insalata, verdure miste, pera a pezzetti, miele. Servita con focaccia fatta in casa**.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="5">
-    <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="&quot;€ &quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
-    <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
-    <numFmt numFmtId="167" formatCode="&quot;€&quot;\ #,##0.00"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;€&quot;\ * #,##0.00_-;\-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="&quot;€ &quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="#,##0\ [$€-1];[Red]\-#,##0\ [$€-1]"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ [$€-1];[Red]\-#,##0.00\ [$€-1]"/>
+    <numFmt numFmtId="168" formatCode="&quot;€&quot;\ #,##0.00"/>
   </numFmts>
   <fonts count="27" x14ac:knownFonts="1">
     <font>
@@ -2175,7 +2176,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="323">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2284,22 +2285,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -2316,22 +2317,22 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2353,7 +2354,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2393,13 +2394,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2408,7 +2409,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -2417,27 +2418,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2445,7 +2446,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -2457,10 +2458,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2478,7 +2479,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2493,10 +2494,10 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2505,43 +2506,43 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2619,7 +2620,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2682,7 +2683,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2695,7 +2696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2713,7 +2714,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2731,13 +2732,13 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2747,7 +2748,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2775,7 +2776,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2808,7 +2809,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2863,7 +2864,7 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2916,10 +2917,10 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2938,7 +2939,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="24" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2965,22 +2966,22 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="26" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2989,13 +2990,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3004,7 +3005,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3355,14 +3356,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:AG41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC17" sqref="AC17"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3625,7 +3626,7 @@
         <v>36</v>
       </c>
       <c r="F5" s="41" t="s">
-        <v>546</v>
+        <v>536</v>
       </c>
       <c r="G5" s="42" t="s">
         <v>37</v>
@@ -3686,7 +3687,7 @@
         <v>42</v>
       </c>
       <c r="F6" s="56" t="s">
-        <v>545</v>
+        <v>535</v>
       </c>
       <c r="G6" s="43" t="s">
         <v>43</v>
@@ -3747,7 +3748,7 @@
         <v>47</v>
       </c>
       <c r="F7" s="56" t="s">
-        <v>544</v>
+        <v>534</v>
       </c>
       <c r="G7" s="66" t="s">
         <v>48</v>
@@ -3802,7 +3803,7 @@
         <v>51</v>
       </c>
       <c r="F8" s="68" t="s">
-        <v>561</v>
+        <v>548</v>
       </c>
       <c r="G8" s="69" t="s">
         <v>52</v>
@@ -3863,7 +3864,7 @@
         <v>56</v>
       </c>
       <c r="F9" s="68" t="s">
-        <v>560</v>
+        <v>547</v>
       </c>
       <c r="G9" s="70" t="s">
         <v>57</v>
@@ -3924,7 +3925,7 @@
         <v>62</v>
       </c>
       <c r="F10" s="68" t="s">
-        <v>543</v>
+        <v>533</v>
       </c>
       <c r="G10" s="74" t="s">
         <v>63</v>
@@ -3979,7 +3980,7 @@
         <v>67</v>
       </c>
       <c r="F11" s="76" t="s">
-        <v>542</v>
+        <v>532</v>
       </c>
       <c r="G11" s="77" t="s">
         <v>68</v>
@@ -4034,7 +4035,7 @@
         <v>71</v>
       </c>
       <c r="F12" s="68" t="s">
-        <v>509</v>
+        <v>499</v>
       </c>
       <c r="G12" s="69" t="s">
         <v>72</v>
@@ -4086,13 +4087,13 @@
       <c r="C13" s="54"/>
       <c r="D13" s="54"/>
       <c r="E13" s="67" t="s">
-        <v>538</v>
+        <v>528</v>
       </c>
       <c r="F13" s="180" t="s">
-        <v>539</v>
+        <v>529</v>
       </c>
       <c r="G13" s="70" t="s">
-        <v>547</v>
+        <v>537</v>
       </c>
       <c r="H13" s="249"/>
       <c r="I13" s="71"/>
@@ -4112,7 +4113,7 @@
       <c r="W13" s="71"/>
       <c r="X13" s="45"/>
       <c r="Y13" s="304" t="s">
-        <v>557</v>
+        <v>544</v>
       </c>
       <c r="Z13" s="288" t="s">
         <v>64</v>
@@ -4121,7 +4122,7 @@
         <v>3.5</v>
       </c>
       <c r="AB13" s="311" t="s">
-        <v>558</v>
+        <v>545</v>
       </c>
       <c r="AC13" s="288" t="s">
         <v>60</v>
@@ -4130,7 +4131,7 @@
         <v>6</v>
       </c>
       <c r="AE13" s="304" t="s">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="AF13" s="313" t="s">
         <v>41</v>
@@ -4148,7 +4149,7 @@
         <v>75</v>
       </c>
       <c r="F14" s="56" t="s">
-        <v>540</v>
+        <v>530</v>
       </c>
       <c r="G14" s="78" t="s">
         <v>76</v>
@@ -4209,7 +4210,7 @@
         <v>80</v>
       </c>
       <c r="F15" s="56" t="s">
-        <v>541</v>
+        <v>531</v>
       </c>
       <c r="G15" s="43" t="s">
         <v>81</v>
@@ -4309,7 +4310,7 @@
         <v>87</v>
       </c>
       <c r="F17" s="90" t="s">
-        <v>510</v>
+        <v>500</v>
       </c>
       <c r="G17" s="57" t="s">
         <v>407</v>
@@ -4354,7 +4355,7 @@
         <v>89</v>
       </c>
       <c r="F18" s="90" t="s">
-        <v>511</v>
+        <v>501</v>
       </c>
       <c r="G18" s="57" t="s">
         <v>408</v>
@@ -4401,10 +4402,10 @@
         <v>404</v>
       </c>
       <c r="F19" s="99" t="s">
-        <v>512</v>
+        <v>502</v>
       </c>
       <c r="G19" s="71" t="s">
-        <v>513</v>
+        <v>503</v>
       </c>
       <c r="H19" s="247"/>
       <c r="I19" s="15"/>
@@ -4552,16 +4553,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:AG47"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="G19" sqref="G19"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4695,7 +4696,7 @@
       <c r="A4" s="15"/>
       <c r="B4" s="15"/>
       <c r="C4" s="171" t="s">
-        <v>506</v>
+        <v>496</v>
       </c>
       <c r="D4" s="172" t="s">
         <v>205</v>
@@ -4771,7 +4772,7 @@
         <v>330</v>
       </c>
       <c r="F5" s="178" t="s">
-        <v>530</v>
+        <v>520</v>
       </c>
       <c r="G5" s="254" t="s">
         <v>438</v>
@@ -4796,7 +4797,7 @@
       <c r="W5" s="183"/>
       <c r="X5" s="183"/>
       <c r="Y5" s="178" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="Z5" s="180"/>
       <c r="AA5" s="181">
@@ -4816,7 +4817,7 @@
         <v>206</v>
       </c>
       <c r="F6" s="186" t="s">
-        <v>529</v>
+        <v>519</v>
       </c>
       <c r="G6" s="179" t="s">
         <v>439</v>
@@ -4843,7 +4844,7 @@
       <c r="W6" s="183"/>
       <c r="X6" s="183"/>
       <c r="Y6" s="186" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="Z6" s="56"/>
       <c r="AA6" s="181">
@@ -4859,7 +4860,7 @@
         <v>207</v>
       </c>
       <c r="F7" s="185" t="s">
-        <v>528</v>
+        <v>518</v>
       </c>
       <c r="G7" s="187" t="s">
         <v>440</v>
@@ -4888,7 +4889,7 @@
       <c r="W7" s="183"/>
       <c r="X7" s="183"/>
       <c r="Y7" s="196" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="Z7" s="56"/>
       <c r="AA7" s="181">
@@ -4901,13 +4902,13 @@
       <c r="C8" s="171"/>
       <c r="D8" s="170"/>
       <c r="E8" s="185" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="F8" s="185" t="s">
-        <v>527</v>
+        <v>517</v>
       </c>
       <c r="G8" s="187" t="s">
-        <v>535</v>
+        <v>525</v>
       </c>
       <c r="H8" s="259"/>
       <c r="I8" s="285"/>
@@ -4931,7 +4932,7 @@
       <c r="W8" s="285"/>
       <c r="X8" s="285"/>
       <c r="Y8" s="196" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="Z8" s="56"/>
       <c r="AA8" s="181">
@@ -4952,7 +4953,7 @@
         <v>331</v>
       </c>
       <c r="F9" s="196" t="s">
-        <v>531</v>
+        <v>521</v>
       </c>
       <c r="G9" s="187" t="s">
         <v>441</v>
@@ -4981,7 +4982,7 @@
       <c r="W9" s="285"/>
       <c r="X9" s="285"/>
       <c r="Y9" s="196" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="Z9" s="76"/>
       <c r="AA9" s="209">
@@ -4997,7 +4998,7 @@
       <c r="A10" s="182"/>
       <c r="B10" s="182"/>
       <c r="C10" s="171" t="s">
-        <v>507</v>
+        <v>497</v>
       </c>
       <c r="D10" s="191" t="s">
         <v>208</v>
@@ -5040,7 +5041,7 @@
         <v>209</v>
       </c>
       <c r="F11" s="185" t="s">
-        <v>532</v>
+        <v>522</v>
       </c>
       <c r="G11" s="187" t="s">
         <v>442</v>
@@ -5069,14 +5070,14 @@
       <c r="W11" s="192"/>
       <c r="X11" s="192"/>
       <c r="Y11" s="196" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="Z11" s="56"/>
       <c r="AA11" s="181">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:33" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="182"/>
       <c r="B12" s="182"/>
       <c r="C12" s="171"/>
@@ -5085,10 +5086,10 @@
         <v>213</v>
       </c>
       <c r="F12" s="186" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="G12" s="179" t="s">
-        <v>443</v>
+        <v>560</v>
       </c>
       <c r="H12" s="261"/>
       <c r="I12" s="193">
@@ -5114,7 +5115,7 @@
       <c r="W12" s="192"/>
       <c r="X12" s="192"/>
       <c r="Y12" s="186" t="s">
-        <v>476</v>
+        <v>466</v>
       </c>
       <c r="Z12" s="56"/>
       <c r="AA12" s="181">
@@ -5127,13 +5128,13 @@
       <c r="C13" s="171"/>
       <c r="D13" s="170"/>
       <c r="E13" s="185" t="s">
-        <v>478</v>
+        <v>468</v>
       </c>
       <c r="F13" s="185" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="G13" s="187" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="H13" s="260"/>
       <c r="I13" s="192"/>
@@ -5157,7 +5158,7 @@
       <c r="W13" s="192"/>
       <c r="X13" s="192"/>
       <c r="Y13" s="196" t="s">
-        <v>477</v>
+        <v>467</v>
       </c>
       <c r="Z13" s="56"/>
       <c r="AA13" s="181">
@@ -5173,10 +5174,10 @@
         <v>211</v>
       </c>
       <c r="F14" s="186" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="G14" s="179" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="H14" s="260"/>
       <c r="I14" s="192">
@@ -5200,7 +5201,7 @@
       <c r="W14" s="192"/>
       <c r="X14" s="192"/>
       <c r="Y14" s="186" t="s">
-        <v>479</v>
+        <v>469</v>
       </c>
       <c r="Z14" s="56"/>
       <c r="AA14" s="181">
@@ -5216,10 +5217,10 @@
         <v>215</v>
       </c>
       <c r="F15" s="196" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="G15" s="255" t="s">
-        <v>449</v>
+        <v>561</v>
       </c>
       <c r="H15" s="261"/>
       <c r="I15" s="193"/>
@@ -5243,7 +5244,7 @@
       <c r="W15" s="192"/>
       <c r="X15" s="192"/>
       <c r="Y15" s="196" t="s">
-        <v>533</v>
+        <v>523</v>
       </c>
       <c r="Z15" s="76"/>
       <c r="AA15" s="181">
@@ -5259,10 +5260,10 @@
         <v>212</v>
       </c>
       <c r="F16" s="186" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="G16" s="179" t="s">
-        <v>444</v>
+        <v>562</v>
       </c>
       <c r="H16" s="260"/>
       <c r="I16" s="192"/>
@@ -5288,7 +5289,7 @@
       <c r="W16" s="192"/>
       <c r="X16" s="192"/>
       <c r="Y16" s="186" t="s">
-        <v>480</v>
+        <v>470</v>
       </c>
       <c r="Z16" s="56"/>
       <c r="AA16" s="181">
@@ -5304,10 +5305,10 @@
         <v>214</v>
       </c>
       <c r="F17" s="185" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="G17" s="194" t="s">
-        <v>445</v>
+        <v>563</v>
       </c>
       <c r="H17" s="262"/>
       <c r="I17" s="195"/>
@@ -5335,7 +5336,7 @@
       <c r="W17" s="195"/>
       <c r="X17" s="195"/>
       <c r="Y17" s="196" t="s">
-        <v>481</v>
+        <v>471</v>
       </c>
       <c r="Z17" s="56"/>
       <c r="AA17" s="181">
@@ -5351,10 +5352,10 @@
         <v>210</v>
       </c>
       <c r="F18" s="185" t="s">
-        <v>534</v>
+        <v>524</v>
       </c>
       <c r="G18" s="187" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="H18" s="261"/>
       <c r="I18" s="193">
@@ -5378,7 +5379,7 @@
       <c r="W18" s="193"/>
       <c r="X18" s="193"/>
       <c r="Y18" s="196" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="Z18" s="56"/>
       <c r="AA18" s="181">
@@ -5391,13 +5392,13 @@
       <c r="C19" s="208"/>
       <c r="D19" s="170"/>
       <c r="E19" s="196" t="s">
-        <v>515</v>
+        <v>505</v>
       </c>
       <c r="F19" s="196" t="s">
-        <v>550</v>
+        <v>540</v>
       </c>
       <c r="G19" s="187" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="H19" s="261"/>
       <c r="I19" s="193">
@@ -5425,7 +5426,7 @@
       <c r="W19" s="193"/>
       <c r="X19" s="193"/>
       <c r="Y19" s="196" t="s">
-        <v>562</v>
+        <v>549</v>
       </c>
       <c r="Z19" s="76"/>
       <c r="AA19" s="209">
@@ -5496,7 +5497,7 @@
       <c r="X21" s="208"/>
       <c r="Y21" s="91"/>
       <c r="Z21" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA21" s="252">
         <v>2</v>
@@ -5533,7 +5534,7 @@
       <c r="X22" s="208"/>
       <c r="Y22" s="91"/>
       <c r="Z22" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA22" s="252">
         <v>1.5</v>
@@ -5545,10 +5546,10 @@
       <c r="C23" s="208"/>
       <c r="D23" s="245"/>
       <c r="E23" s="76" t="s">
-        <v>482</v>
+        <v>472</v>
       </c>
       <c r="F23" s="304" t="s">
-        <v>483</v>
+        <v>473</v>
       </c>
       <c r="G23" s="91"/>
       <c r="H23" s="263"/>
@@ -5578,10 +5579,10 @@
       <c r="C24" s="208"/>
       <c r="D24" s="245"/>
       <c r="E24" s="76" t="s">
-        <v>484</v>
+        <v>474</v>
       </c>
       <c r="F24" s="304" t="s">
-        <v>496</v>
+        <v>486</v>
       </c>
       <c r="G24" s="91"/>
       <c r="H24" s="263"/>
@@ -5611,10 +5612,10 @@
       <c r="C25" s="208"/>
       <c r="D25" s="245"/>
       <c r="E25" s="76" t="s">
-        <v>486</v>
+        <v>476</v>
       </c>
       <c r="F25" s="304" t="s">
-        <v>497</v>
+        <v>487</v>
       </c>
       <c r="G25" s="91"/>
       <c r="H25" s="263"/>
@@ -5644,10 +5645,10 @@
       <c r="C26" s="208"/>
       <c r="D26" s="245"/>
       <c r="E26" s="76" t="s">
-        <v>490</v>
+        <v>480</v>
       </c>
       <c r="F26" s="304" t="s">
-        <v>498</v>
+        <v>488</v>
       </c>
       <c r="G26" s="91"/>
       <c r="H26" s="263"/>
@@ -5677,10 +5678,10 @@
       <c r="C27" s="208"/>
       <c r="D27" s="245"/>
       <c r="E27" s="76" t="s">
-        <v>487</v>
+        <v>477</v>
       </c>
       <c r="F27" s="304" t="s">
-        <v>488</v>
+        <v>478</v>
       </c>
       <c r="G27" s="91"/>
       <c r="H27" s="263"/>
@@ -5710,10 +5711,10 @@
       <c r="C28" s="208"/>
       <c r="D28" s="245"/>
       <c r="E28" s="76" t="s">
-        <v>537</v>
+        <v>527</v>
       </c>
       <c r="F28" s="304" t="s">
-        <v>489</v>
+        <v>479</v>
       </c>
       <c r="G28" s="91"/>
       <c r="H28" s="263"/>
@@ -5768,7 +5769,7 @@
       <c r="X29" s="208"/>
       <c r="Y29" s="91"/>
       <c r="Z29" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA29" s="252">
         <v>0.5</v>
@@ -5807,7 +5808,7 @@
       <c r="X30" s="208"/>
       <c r="Y30" s="91"/>
       <c r="Z30" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA30" s="252">
         <v>0.5</v>
@@ -5846,7 +5847,7 @@
       <c r="X31" s="208"/>
       <c r="Y31" s="91"/>
       <c r="Z31" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA31" s="252">
         <v>1</v>
@@ -5885,7 +5886,7 @@
       <c r="X32" s="208"/>
       <c r="Y32" s="91"/>
       <c r="Z32" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA32" s="252">
         <v>0.5</v>
@@ -5900,7 +5901,7 @@
         <v>336</v>
       </c>
       <c r="F33" s="304" t="s">
-        <v>491</v>
+        <v>481</v>
       </c>
       <c r="G33" s="219"/>
       <c r="H33" s="263"/>
@@ -5922,7 +5923,7 @@
       <c r="X33" s="208"/>
       <c r="Y33" s="91"/>
       <c r="Z33" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA33" s="252">
         <v>0.5</v>
@@ -5959,7 +5960,7 @@
       <c r="X34" s="208"/>
       <c r="Y34" s="91"/>
       <c r="Z34" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA34" s="252">
         <v>0.5</v>
@@ -5996,7 +5997,7 @@
       <c r="X35" s="208"/>
       <c r="Y35" s="91"/>
       <c r="Z35" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA35" s="252">
         <v>0.5</v>
@@ -6033,7 +6034,7 @@
       <c r="X36" s="208"/>
       <c r="Y36" s="91"/>
       <c r="Z36" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA36" s="252">
         <v>0.5</v>
@@ -6070,7 +6071,7 @@
       <c r="X37" s="208"/>
       <c r="Y37" s="91"/>
       <c r="Z37" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA37" s="252">
         <v>0.5</v>
@@ -6082,10 +6083,10 @@
       <c r="C38" s="208"/>
       <c r="D38" s="208"/>
       <c r="E38" s="76" t="s">
-        <v>492</v>
+        <v>482</v>
       </c>
       <c r="F38" s="304" t="s">
-        <v>495</v>
+        <v>485</v>
       </c>
       <c r="G38" s="253"/>
       <c r="H38" s="263"/>
@@ -6107,7 +6108,7 @@
       <c r="X38" s="208"/>
       <c r="Y38" s="91"/>
       <c r="Z38" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA38" s="252">
         <v>0.5</v>
@@ -6119,10 +6120,10 @@
       <c r="C39" s="208"/>
       <c r="D39" s="208"/>
       <c r="E39" s="76" t="s">
-        <v>493</v>
+        <v>483</v>
       </c>
       <c r="F39" s="304" t="s">
-        <v>494</v>
+        <v>484</v>
       </c>
       <c r="G39" s="253"/>
       <c r="H39" s="263"/>
@@ -6181,7 +6182,7 @@
       <c r="X40" s="208"/>
       <c r="Y40" s="91"/>
       <c r="Z40" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA40" s="252">
         <v>0.5</v>
@@ -6220,7 +6221,7 @@
       <c r="X41" s="208"/>
       <c r="Y41" s="91"/>
       <c r="Z41" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA41" s="252">
         <v>0.5</v>
@@ -6259,7 +6260,7 @@
       <c r="X42" s="208"/>
       <c r="Y42" s="91"/>
       <c r="Z42" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA42" s="252">
         <v>0.5</v>
@@ -6298,7 +6299,7 @@
       <c r="X43" s="208"/>
       <c r="Y43" s="91"/>
       <c r="Z43" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA43" s="252">
         <v>0.5</v>
@@ -6339,7 +6340,7 @@
       <c r="X44" s="286"/>
       <c r="Y44" s="91"/>
       <c r="Z44" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA44" s="252">
         <v>0.5</v>
@@ -6378,7 +6379,7 @@
       <c r="X45" s="208"/>
       <c r="Y45" s="91"/>
       <c r="Z45" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA45" s="252">
         <v>0.5</v>
@@ -6417,7 +6418,7 @@
       <c r="X46" s="208"/>
       <c r="Y46" s="91"/>
       <c r="Z46" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA46" s="252">
         <v>0.5</v>
@@ -6432,7 +6433,7 @@
         <v>354</v>
       </c>
       <c r="F47" s="304" t="s">
-        <v>485</v>
+        <v>475</v>
       </c>
       <c r="G47" s="256"/>
       <c r="H47" s="263"/>
@@ -6456,7 +6457,7 @@
       <c r="X47" s="208"/>
       <c r="Y47" s="91"/>
       <c r="Z47" s="91" t="s">
-        <v>536</v>
+        <v>526</v>
       </c>
       <c r="AA47" s="252">
         <v>0.5</v>
@@ -6469,14 +6470,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6553,7 +6554,7 @@
     </row>
     <row r="3" spans="1:28" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="166" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="B3" s="166" t="s">
         <v>432</v>
@@ -6606,10 +6607,10 @@
       <c r="A4" s="305"/>
       <c r="B4" s="305"/>
       <c r="C4" s="306" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="D4" s="294" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="E4" s="167"/>
       <c r="F4" s="23"/>
@@ -6675,13 +6676,13 @@
       <c r="C5" s="96"/>
       <c r="D5" s="2"/>
       <c r="E5" s="180" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="F5" s="180" t="s">
+        <v>459</v>
+      </c>
+      <c r="G5" s="308" t="s">
         <v>463</v>
-      </c>
-      <c r="G5" s="308" t="s">
-        <v>467</v>
       </c>
       <c r="H5" s="132"/>
       <c r="I5" s="208"/>
@@ -6718,13 +6719,13 @@
       <c r="C6" s="95"/>
       <c r="D6" s="95"/>
       <c r="E6" s="180" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="F6" s="180" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="G6" s="308" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="H6" s="132"/>
       <c r="I6" s="208">
@@ -6763,13 +6764,13 @@
       <c r="C7" s="95"/>
       <c r="D7" s="95"/>
       <c r="E7" s="180" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="F7" s="180" t="s">
-        <v>525</v>
+        <v>515</v>
       </c>
       <c r="G7" s="308" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="H7" s="132"/>
       <c r="I7" s="208"/>
@@ -6806,13 +6807,13 @@
       <c r="C8" s="95"/>
       <c r="D8" s="95"/>
       <c r="E8" s="180" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="F8" s="180" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="G8" s="308" t="s">
-        <v>470</v>
+        <v>567</v>
       </c>
       <c r="H8" s="132"/>
       <c r="I8" s="208"/>
@@ -6849,13 +6850,13 @@
       <c r="C9" s="95"/>
       <c r="D9" s="95"/>
       <c r="E9" s="180" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="F9" s="180" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="G9" s="308" t="s">
-        <v>471</v>
+        <v>568</v>
       </c>
       <c r="H9" s="132"/>
       <c r="I9" s="208">
@@ -6894,13 +6895,13 @@
       <c r="C10" s="95"/>
       <c r="D10" s="95"/>
       <c r="E10" s="180" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="F10" s="180" t="s">
-        <v>524</v>
+        <v>514</v>
       </c>
       <c r="G10" s="308" t="s">
-        <v>472</v>
+        <v>569</v>
       </c>
       <c r="H10" s="132"/>
       <c r="I10" s="208"/>
@@ -6931,19 +6932,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="60" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="45" x14ac:dyDescent="0.3">
       <c r="A11" s="305"/>
       <c r="B11" s="305"/>
       <c r="C11" s="95"/>
       <c r="D11" s="95"/>
       <c r="E11" s="180" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="F11" s="180" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="G11" s="308" t="s">
-        <v>473</v>
+        <v>570</v>
       </c>
       <c r="H11" s="132"/>
       <c r="I11" s="208"/>
@@ -6986,13 +6987,13 @@
       <c r="C12" s="95"/>
       <c r="D12" s="95"/>
       <c r="E12" s="180" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="F12" s="180" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="G12" s="308" t="s">
-        <v>474</v>
+        <v>571</v>
       </c>
       <c r="H12" s="132"/>
       <c r="I12" s="208">
@@ -7037,13 +7038,13 @@
       <c r="C13" s="95"/>
       <c r="D13" s="95"/>
       <c r="E13" s="180" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="F13" s="180" t="s">
-        <v>523</v>
+        <v>513</v>
       </c>
       <c r="G13" s="308" t="s">
-        <v>475</v>
+        <v>572</v>
       </c>
       <c r="H13" s="132"/>
       <c r="I13" s="208"/>
@@ -7084,7 +7085,7 @@
       <c r="A14" s="197"/>
       <c r="B14" s="197"/>
       <c r="C14" s="198" t="s">
-        <v>514</v>
+        <v>504</v>
       </c>
       <c r="D14" s="303" t="s">
         <v>216</v>
@@ -7122,10 +7123,10 @@
         <v>329</v>
       </c>
       <c r="F15" s="196" t="s">
-        <v>499</v>
+        <v>489</v>
       </c>
       <c r="G15" s="70" t="s">
-        <v>563</v>
+        <v>573</v>
       </c>
       <c r="H15" s="250"/>
       <c r="I15" s="208"/>
@@ -7154,7 +7155,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="114"/>
       <c r="B16" s="114"/>
       <c r="C16" s="208"/>
@@ -7163,10 +7164,10 @@
         <v>217</v>
       </c>
       <c r="F16" s="196" t="s">
-        <v>500</v>
+        <v>490</v>
       </c>
       <c r="G16" s="224" t="s">
-        <v>551</v>
+        <v>564</v>
       </c>
       <c r="H16" s="250"/>
       <c r="I16" s="192">
@@ -7199,7 +7200,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="114"/>
       <c r="B17" s="114"/>
       <c r="C17" s="208"/>
@@ -7208,10 +7209,10 @@
         <v>218</v>
       </c>
       <c r="F17" s="196" t="s">
-        <v>501</v>
+        <v>491</v>
       </c>
       <c r="G17" s="74" t="s">
-        <v>553</v>
+        <v>565</v>
       </c>
       <c r="H17" s="250"/>
       <c r="I17" s="208"/>
@@ -7251,10 +7252,10 @@
         <v>219</v>
       </c>
       <c r="F18" s="196" t="s">
-        <v>502</v>
+        <v>492</v>
       </c>
       <c r="G18" s="133" t="s">
-        <v>552</v>
+        <v>566</v>
       </c>
       <c r="H18" s="289"/>
       <c r="I18" s="208"/>
@@ -7287,7 +7288,7 @@
       <c r="A19" s="114"/>
       <c r="B19" s="114"/>
       <c r="C19" s="200" t="s">
-        <v>508</v>
+        <v>498</v>
       </c>
       <c r="D19" s="201" t="s">
         <v>433</v>
@@ -7325,7 +7326,7 @@
         <v>369</v>
       </c>
       <c r="F20" s="205" t="s">
-        <v>522</v>
+        <v>512</v>
       </c>
       <c r="G20" s="206"/>
       <c r="H20" s="290"/>
@@ -7362,7 +7363,7 @@
         <v>368</v>
       </c>
       <c r="F21" s="196" t="s">
-        <v>521</v>
+        <v>511</v>
       </c>
       <c r="G21" s="287"/>
       <c r="H21" s="291"/>
@@ -7401,7 +7402,7 @@
         <v>367</v>
       </c>
       <c r="F22" s="196" t="s">
-        <v>520</v>
+        <v>510</v>
       </c>
       <c r="G22" s="287"/>
       <c r="H22" s="291"/>
@@ -7440,7 +7441,7 @@
         <v>366</v>
       </c>
       <c r="F23" s="196" t="s">
-        <v>519</v>
+        <v>509</v>
       </c>
       <c r="G23" s="287"/>
       <c r="H23" s="291"/>
@@ -7479,7 +7480,7 @@
         <v>365</v>
       </c>
       <c r="F24" s="196" t="s">
-        <v>518</v>
+        <v>508</v>
       </c>
       <c r="G24" s="71"/>
       <c r="H24" s="291"/>
@@ -7522,7 +7523,7 @@
         <v>364</v>
       </c>
       <c r="F25" s="196" t="s">
-        <v>517</v>
+        <v>507</v>
       </c>
       <c r="G25" s="71" t="s">
         <v>220</v>
@@ -7569,7 +7570,7 @@
         <v>395</v>
       </c>
       <c r="F26" s="196" t="s">
-        <v>516</v>
+        <v>506</v>
       </c>
       <c r="G26" s="210" t="s">
         <v>381</v>
@@ -7737,13 +7738,13 @@
       <c r="C30" s="208"/>
       <c r="D30" s="208"/>
       <c r="E30" s="76" t="s">
-        <v>548</v>
+        <v>538</v>
       </c>
       <c r="F30" s="76" t="s">
-        <v>549</v>
+        <v>539</v>
       </c>
       <c r="G30" s="315" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
       <c r="H30" s="199"/>
       <c r="I30" s="208"/>
@@ -7779,7 +7780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
@@ -7893,10 +7894,10 @@
     </row>
     <row r="3" spans="1:33" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="166" t="s">
-        <v>504</v>
+        <v>494</v>
       </c>
       <c r="B3" s="166" t="s">
-        <v>503</v>
+        <v>493</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>2</v>
@@ -7961,7 +7962,7 @@
         <v>223</v>
       </c>
       <c r="D4" s="134" t="s">
-        <v>555</v>
+        <v>542</v>
       </c>
       <c r="H4" s="257" t="s">
         <v>19</v>
@@ -8769,10 +8770,10 @@
       <c r="A22" s="166"/>
       <c r="B22" s="166"/>
       <c r="C22" s="58" t="s">
-        <v>505</v>
+        <v>495</v>
       </c>
       <c r="D22" s="227" t="s">
-        <v>554</v>
+        <v>541</v>
       </c>
       <c r="E22" s="284"/>
       <c r="F22" s="284"/>
@@ -9511,7 +9512,7 @@
         <v>285</v>
       </c>
       <c r="D39" s="236" t="s">
-        <v>556</v>
+        <v>543</v>
       </c>
       <c r="E39" s="15"/>
       <c r="G39" s="15"/>
@@ -10004,7 +10005,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>

</xml_diff>

<commit_message>
Fixed missing items due to empty line
</commit_message>
<xml_diff>
--- a/excel/DATABASE_MENU_VENDITA.xlsx
+++ b/excel/DATABASE_MENU_VENDITA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LE NOSTRE BIRRE" sheetId="1" state="visible" r:id="rId2"/>
@@ -2104,7 +2104,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="252">
+  <cellXfs count="251">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3102,10 +3102,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="19" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3193,11 +3189,11 @@
   </sheetPr>
   <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G26" activeCellId="0" sqref="G26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -4456,7 +4452,7 @@
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="100" width="42"/>
@@ -6367,7 +6363,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="100" width="42"/>
@@ -7684,7 +7680,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="46.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="24.29"/>
@@ -9911,13 +9907,13 @@
     <tabColor rgb="FF00B0F0"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AG57"/>
+  <dimension ref="A1:AG1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.76953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="41.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="19.42"/>
@@ -11046,9 +11042,15 @@
       <c r="B24" s="29"/>
       <c r="C24" s="90"/>
       <c r="D24" s="90"/>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="35"/>
+      <c r="E24" s="85" t="s">
+        <v>498</v>
+      </c>
+      <c r="F24" s="85" t="s">
+        <v>499</v>
+      </c>
+      <c r="G24" s="35" t="s">
+        <v>500</v>
+      </c>
       <c r="H24" s="197"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
@@ -11066,29 +11068,33 @@
       <c r="V24" s="12"/>
       <c r="W24" s="12"/>
       <c r="X24" s="12"/>
-      <c r="Y24" s="82"/>
+      <c r="Y24" s="38"/>
       <c r="Z24" s="39"/>
       <c r="AA24" s="249"/>
       <c r="AB24" s="35"/>
-      <c r="AC24" s="240"/>
-      <c r="AD24" s="250"/>
+      <c r="AC24" s="240" t="s">
+        <v>469</v>
+      </c>
+      <c r="AD24" s="247" t="n">
+        <v>4.5</v>
+      </c>
       <c r="AE24" s="12"/>
       <c r="AF24" s="12"/>
       <c r="AG24" s="12"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="29"/>
       <c r="B25" s="29"/>
-      <c r="C25" s="90"/>
-      <c r="D25" s="90"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
       <c r="E25" s="85" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="F25" s="85" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="H25" s="197"/>
       <c r="I25" s="12"/>
@@ -11107,10 +11113,10 @@
       <c r="V25" s="12"/>
       <c r="W25" s="12"/>
       <c r="X25" s="12"/>
-      <c r="Y25" s="38"/>
+      <c r="Y25" s="12"/>
       <c r="Z25" s="39"/>
-      <c r="AA25" s="249"/>
-      <c r="AB25" s="35"/>
+      <c r="AA25" s="84"/>
+      <c r="AB25" s="12"/>
       <c r="AC25" s="240" t="s">
         <v>469</v>
       </c>
@@ -11122,18 +11128,18 @@
       <c r="AG25" s="12"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="29"/>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
       <c r="E26" s="85" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="F26" s="85" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="G26" s="35" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="H26" s="197"/>
       <c r="I26" s="12"/>
@@ -11153,13 +11159,17 @@
       <c r="W26" s="12"/>
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
-      <c r="Z26" s="39"/>
-      <c r="AA26" s="84"/>
+      <c r="Z26" s="39" t="s">
+        <v>477</v>
+      </c>
+      <c r="AA26" s="84" t="n">
+        <v>2.5</v>
+      </c>
       <c r="AB26" s="12"/>
       <c r="AC26" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD26" s="247" t="n">
+      <c r="AD26" s="250" t="n">
         <v>4.5</v>
       </c>
       <c r="AE26" s="12"/>
@@ -11172,10 +11182,10 @@
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="85" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="F27" s="85" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="G27" s="35" t="s">
         <v>506</v>
@@ -11202,14 +11212,14 @@
         <v>477</v>
       </c>
       <c r="AA27" s="84" t="n">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="AB27" s="12"/>
       <c r="AC27" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD27" s="251" t="n">
-        <v>4.5</v>
+      <c r="AD27" s="250" t="n">
+        <v>7.5</v>
       </c>
       <c r="AE27" s="12"/>
       <c r="AF27" s="12"/>
@@ -11221,13 +11231,13 @@
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="85" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="F28" s="85" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
       <c r="G28" s="35" t="s">
-        <v>506</v>
+        <v>511</v>
       </c>
       <c r="H28" s="197"/>
       <c r="I28" s="12"/>
@@ -11257,7 +11267,7 @@
       <c r="AC28" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD28" s="251" t="n">
+      <c r="AD28" s="250" t="n">
         <v>7.5</v>
       </c>
       <c r="AE28" s="12"/>
@@ -11270,13 +11280,13 @@
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="85" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="F29" s="85" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="H29" s="197"/>
       <c r="I29" s="12"/>
@@ -11300,14 +11310,14 @@
         <v>477</v>
       </c>
       <c r="AA29" s="84" t="n">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="AB29" s="12"/>
       <c r="AC29" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD29" s="251" t="n">
-        <v>7.5</v>
+      <c r="AD29" s="250" t="n">
+        <v>5</v>
       </c>
       <c r="AE29" s="12"/>
       <c r="AF29" s="12"/>
@@ -11319,10 +11329,10 @@
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="85" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="F30" s="85" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="G30" s="35" t="s">
         <v>514</v>
@@ -11355,7 +11365,7 @@
       <c r="AC30" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD30" s="251" t="n">
+      <c r="AD30" s="250" t="n">
         <v>5</v>
       </c>
       <c r="AE30" s="12"/>
@@ -11368,13 +11378,13 @@
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="85" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="F31" s="85" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="G31" s="35" t="s">
-        <v>514</v>
+        <v>519</v>
       </c>
       <c r="H31" s="197"/>
       <c r="I31" s="12"/>
@@ -11404,7 +11414,7 @@
       <c r="AC31" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD31" s="251" t="n">
+      <c r="AD31" s="250" t="n">
         <v>5</v>
       </c>
       <c r="AE31" s="12"/>
@@ -11417,10 +11427,10 @@
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="85" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="F32" s="85" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="G32" s="35" t="s">
         <v>519</v>
@@ -11447,14 +11457,14 @@
         <v>477</v>
       </c>
       <c r="AA32" s="84" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AB32" s="12"/>
       <c r="AC32" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD32" s="251" t="n">
-        <v>5</v>
+      <c r="AD32" s="250" t="n">
+        <v>7</v>
       </c>
       <c r="AE32" s="12"/>
       <c r="AF32" s="12"/>
@@ -11466,10 +11476,10 @@
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="85" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="F33" s="85" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="G33" s="35" t="s">
         <v>519</v>
@@ -11496,14 +11506,14 @@
         <v>477</v>
       </c>
       <c r="AA33" s="84" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="AB33" s="12"/>
       <c r="AC33" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD33" s="251" t="n">
-        <v>7</v>
+      <c r="AD33" s="250" t="n">
+        <v>8</v>
       </c>
       <c r="AE33" s="12"/>
       <c r="AF33" s="12"/>
@@ -11515,13 +11525,13 @@
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="85" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="F34" s="85" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="H34" s="197"/>
       <c r="I34" s="12"/>
@@ -11545,14 +11555,14 @@
         <v>477</v>
       </c>
       <c r="AA34" s="84" t="n">
-        <v>4.5</v>
+        <v>3</v>
       </c>
       <c r="AB34" s="12"/>
       <c r="AC34" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD34" s="251" t="n">
-        <v>8</v>
+      <c r="AD34" s="250" t="n">
+        <v>5</v>
       </c>
       <c r="AE34" s="12"/>
       <c r="AF34" s="12"/>
@@ -11564,10 +11574,10 @@
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="85" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="F35" s="85" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="G35" s="35" t="s">
         <v>526</v>
@@ -11594,14 +11604,14 @@
         <v>477</v>
       </c>
       <c r="AA35" s="84" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AB35" s="12"/>
       <c r="AC35" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD35" s="251" t="n">
-        <v>5</v>
+      <c r="AD35" s="250" t="n">
+        <v>9.5</v>
       </c>
       <c r="AE35" s="12"/>
       <c r="AF35" s="12"/>
@@ -11612,11 +11622,11 @@
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
-      <c r="E36" s="85" t="s">
-        <v>527</v>
+      <c r="E36" s="245" t="s">
+        <v>529</v>
       </c>
       <c r="F36" s="85" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="G36" s="35" t="s">
         <v>526</v>
@@ -11643,14 +11653,14 @@
         <v>477</v>
       </c>
       <c r="AA36" s="84" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="AB36" s="12"/>
       <c r="AC36" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD36" s="251" t="n">
-        <v>9.5</v>
+      <c r="AD36" s="250" t="n">
+        <v>5</v>
       </c>
       <c r="AE36" s="12"/>
       <c r="AF36" s="12"/>
@@ -11661,11 +11671,11 @@
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
-      <c r="E37" s="245" t="s">
-        <v>529</v>
+      <c r="E37" s="85" t="s">
+        <v>531</v>
       </c>
       <c r="F37" s="85" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="G37" s="35" t="s">
         <v>526</v>
@@ -11698,7 +11708,7 @@
       <c r="AC37" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD37" s="251" t="n">
+      <c r="AD37" s="250" t="n">
         <v>5</v>
       </c>
       <c r="AE37" s="12"/>
@@ -11711,10 +11721,10 @@
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="85" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="F38" s="85" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="G38" s="35" t="s">
         <v>526</v>
@@ -11747,7 +11757,7 @@
       <c r="AC38" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD38" s="251" t="n">
+      <c r="AD38" s="250" t="n">
         <v>5</v>
       </c>
       <c r="AE38" s="12"/>
@@ -11760,14 +11770,12 @@
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="85" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
       <c r="F39" s="85" t="s">
-        <v>534</v>
-      </c>
-      <c r="G39" s="35" t="s">
-        <v>526</v>
-      </c>
+        <v>536</v>
+      </c>
+      <c r="G39" s="35"/>
       <c r="H39" s="197"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
@@ -11796,8 +11804,8 @@
       <c r="AC39" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD39" s="251" t="n">
-        <v>5</v>
+      <c r="AD39" s="250" t="n">
+        <v>4.5</v>
       </c>
       <c r="AE39" s="12"/>
       <c r="AF39" s="12"/>
@@ -11809,10 +11817,10 @@
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="85" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="F40" s="85" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="G40" s="35"/>
       <c r="H40" s="197"/>
@@ -11837,14 +11845,14 @@
         <v>477</v>
       </c>
       <c r="AA40" s="84" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AB40" s="12"/>
       <c r="AC40" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD40" s="251" t="n">
-        <v>4.5</v>
+      <c r="AD40" s="250" t="n">
+        <v>4</v>
       </c>
       <c r="AE40" s="12"/>
       <c r="AF40" s="12"/>
@@ -11856,10 +11864,10 @@
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="85" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="F41" s="85" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="G41" s="35"/>
       <c r="H41" s="197"/>
@@ -11890,23 +11898,23 @@
       <c r="AC41" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD41" s="251" t="n">
+      <c r="AD41" s="250" t="n">
         <v>4</v>
       </c>
       <c r="AE41" s="12"/>
       <c r="AF41" s="12"/>
       <c r="AG41" s="12"/>
     </row>
-    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="12"/>
       <c r="B42" s="12"/>
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="85" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="F42" s="85" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="G42" s="35"/>
       <c r="H42" s="197"/>
@@ -11937,24 +11945,22 @@
       <c r="AC42" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD42" s="251" t="n">
+      <c r="AD42" s="250" t="n">
         <v>4</v>
       </c>
       <c r="AE42" s="12"/>
       <c r="AF42" s="12"/>
       <c r="AG42" s="12"/>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
-      <c r="D43" s="12"/>
-      <c r="E43" s="85" t="s">
-        <v>541</v>
-      </c>
-      <c r="F43" s="85" t="s">
-        <v>542</v>
-      </c>
+      <c r="C43" s="192" t="s">
+        <v>543</v>
+      </c>
+      <c r="D43" s="192"/>
+      <c r="E43" s="85"/>
+      <c r="F43" s="85"/>
       <c r="G43" s="35"/>
       <c r="H43" s="197"/>
       <c r="I43" s="12"/>
@@ -11974,33 +11980,25 @@
       <c r="W43" s="12"/>
       <c r="X43" s="12"/>
       <c r="Y43" s="12"/>
-      <c r="Z43" s="39" t="s">
-        <v>477</v>
-      </c>
-      <c r="AA43" s="84" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="Z43" s="39"/>
+      <c r="AA43" s="84"/>
       <c r="AB43" s="12"/>
-      <c r="AC43" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD43" s="251" t="n">
-        <v>4</v>
-      </c>
+      <c r="AC43" s="240"/>
+      <c r="AD43" s="250"/>
       <c r="AE43" s="12"/>
       <c r="AF43" s="12"/>
       <c r="AG43" s="12"/>
     </row>
-    <row r="44" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="192" t="s">
-        <v>543</v>
-      </c>
-      <c r="D44" s="192"/>
-      <c r="E44" s="85"/>
-      <c r="F44" s="85"/>
-      <c r="G44" s="35"/>
+      <c r="B44" s="97"/>
+      <c r="E44" s="85" t="s">
+        <v>544</v>
+      </c>
+      <c r="F44" s="85" t="s">
+        <v>545</v>
+      </c>
+      <c r="G44" s="12"/>
       <c r="H44" s="197"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
@@ -12019,23 +12017,33 @@
       <c r="W44" s="12"/>
       <c r="X44" s="12"/>
       <c r="Y44" s="12"/>
-      <c r="Z44" s="39"/>
-      <c r="AA44" s="84"/>
+      <c r="Z44" s="39" t="s">
+        <v>477</v>
+      </c>
+      <c r="AA44" s="84" t="n">
+        <v>3</v>
+      </c>
       <c r="AB44" s="12"/>
-      <c r="AC44" s="240"/>
-      <c r="AD44" s="251"/>
+      <c r="AC44" s="240" t="s">
+        <v>469</v>
+      </c>
+      <c r="AD44" s="250" t="n">
+        <v>4.5</v>
+      </c>
       <c r="AE44" s="12"/>
       <c r="AF44" s="12"/>
       <c r="AG44" s="12"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12"/>
-      <c r="B45" s="97"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
       <c r="E45" s="85" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="F45" s="85" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="197"/>
@@ -12060,14 +12068,14 @@
         <v>477</v>
       </c>
       <c r="AA45" s="84" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="AB45" s="12"/>
       <c r="AC45" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD45" s="251" t="n">
-        <v>4.5</v>
+      <c r="AD45" s="250" t="n">
+        <v>6</v>
       </c>
       <c r="AE45" s="12"/>
       <c r="AF45" s="12"/>
@@ -12079,10 +12087,10 @@
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="85" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
       <c r="F46" s="85" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="197"/>
@@ -12107,14 +12115,14 @@
         <v>477</v>
       </c>
       <c r="AA46" s="84" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="AB46" s="12"/>
       <c r="AC46" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD46" s="251" t="n">
-        <v>6</v>
+      <c r="AD46" s="250" t="n">
+        <v>4.5</v>
       </c>
       <c r="AE46" s="12"/>
       <c r="AF46" s="12"/>
@@ -12126,12 +12134,14 @@
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="85" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="F47" s="85" t="s">
-        <v>549</v>
-      </c>
-      <c r="G47" s="12"/>
+        <v>551</v>
+      </c>
+      <c r="G47" s="35" t="s">
+        <v>552</v>
+      </c>
       <c r="H47" s="197"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
@@ -12160,7 +12170,7 @@
       <c r="AC47" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD47" s="251" t="n">
+      <c r="AD47" s="250" t="n">
         <v>4.5</v>
       </c>
       <c r="AE47" s="12"/>
@@ -12173,14 +12183,12 @@
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="85" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="F48" s="85" t="s">
-        <v>551</v>
-      </c>
-      <c r="G48" s="35" t="s">
-        <v>552</v>
-      </c>
+        <v>554</v>
+      </c>
+      <c r="G48" s="12"/>
       <c r="H48" s="197"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
@@ -12209,7 +12217,7 @@
       <c r="AC48" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD48" s="251" t="n">
+      <c r="AD48" s="250" t="n">
         <v>4.5</v>
       </c>
       <c r="AE48" s="12"/>
@@ -12222,10 +12230,10 @@
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="85" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
       <c r="F49" s="85" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="G49" s="12"/>
       <c r="H49" s="197"/>
@@ -12250,14 +12258,14 @@
         <v>477</v>
       </c>
       <c r="AA49" s="84" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="AB49" s="12"/>
       <c r="AC49" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD49" s="251" t="n">
-        <v>4.5</v>
+      <c r="AD49" s="250" t="n">
+        <v>4</v>
       </c>
       <c r="AE49" s="12"/>
       <c r="AF49" s="12"/>
@@ -12269,10 +12277,10 @@
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="85" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="F50" s="85" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="G50" s="12"/>
       <c r="H50" s="197"/>
@@ -12303,24 +12311,22 @@
       <c r="AC50" s="240" t="s">
         <v>469</v>
       </c>
-      <c r="AD50" s="251" t="n">
+      <c r="AD50" s="250" t="n">
         <v>4</v>
       </c>
       <c r="AE50" s="12"/>
       <c r="AF50" s="12"/>
       <c r="AG50" s="12"/>
     </row>
-    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
-      <c r="C51" s="12"/>
-      <c r="D51" s="12"/>
-      <c r="E51" s="85" t="s">
-        <v>557</v>
-      </c>
-      <c r="F51" s="85" t="s">
-        <v>558</v>
-      </c>
+      <c r="C51" s="192" t="s">
+        <v>559</v>
+      </c>
+      <c r="D51" s="192"/>
+      <c r="E51" s="85"/>
+      <c r="F51" s="85"/>
       <c r="G51" s="12"/>
       <c r="H51" s="197"/>
       <c r="I51" s="12"/>
@@ -12340,32 +12346,25 @@
       <c r="W51" s="12"/>
       <c r="X51" s="12"/>
       <c r="Y51" s="12"/>
-      <c r="Z51" s="39" t="s">
-        <v>477</v>
-      </c>
-      <c r="AA51" s="84" t="n">
-        <v>2.5</v>
-      </c>
+      <c r="Z51" s="39"/>
+      <c r="AA51" s="84"/>
       <c r="AB51" s="12"/>
-      <c r="AC51" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD51" s="251" t="n">
-        <v>4</v>
-      </c>
+      <c r="AC51" s="240"/>
+      <c r="AD51" s="250"/>
       <c r="AE51" s="12"/>
       <c r="AF51" s="12"/>
       <c r="AG51" s="12"/>
     </row>
-    <row r="52" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="12"/>
-      <c r="B52" s="12"/>
-      <c r="C52" s="192" t="s">
-        <v>559</v>
-      </c>
-      <c r="D52" s="192"/>
-      <c r="E52" s="85"/>
-      <c r="F52" s="85"/>
+      <c r="B52" s="97"/>
+      <c r="C52" s="12"/>
+      <c r="E52" s="85" t="s">
+        <v>560</v>
+      </c>
+      <c r="F52" s="85" t="s">
+        <v>561</v>
+      </c>
       <c r="G52" s="12"/>
       <c r="H52" s="197"/>
       <c r="I52" s="12"/>
@@ -12385,32 +12384,41 @@
       <c r="W52" s="12"/>
       <c r="X52" s="12"/>
       <c r="Y52" s="12"/>
-      <c r="Z52" s="39"/>
-      <c r="AA52" s="84"/>
+      <c r="Z52" s="39" t="s">
+        <v>477</v>
+      </c>
+      <c r="AA52" s="84" t="n">
+        <v>3.5</v>
+      </c>
       <c r="AB52" s="12"/>
-      <c r="AC52" s="240"/>
-      <c r="AD52" s="251"/>
+      <c r="AC52" s="12"/>
+      <c r="AD52" s="250"/>
       <c r="AE52" s="12"/>
       <c r="AF52" s="12"/>
       <c r="AG52" s="12"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="12"/>
-      <c r="B53" s="97"/>
+      <c r="B53" s="12"/>
       <c r="C53" s="12"/>
+      <c r="D53" s="12"/>
       <c r="E53" s="85" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
       <c r="F53" s="85" t="s">
-        <v>561</v>
-      </c>
-      <c r="G53" s="12"/>
+        <v>563</v>
+      </c>
+      <c r="G53" s="35" t="s">
+        <v>564</v>
+      </c>
       <c r="H53" s="197"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
       <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
+      <c r="M53" s="83" t="n">
+        <v>1</v>
+      </c>
       <c r="N53" s="12"/>
       <c r="O53" s="12"/>
       <c r="P53" s="12"/>
@@ -12431,7 +12439,7 @@
       </c>
       <c r="AB53" s="12"/>
       <c r="AC53" s="12"/>
-      <c r="AD53" s="251"/>
+      <c r="AD53" s="250"/>
       <c r="AE53" s="12"/>
       <c r="AF53" s="12"/>
       <c r="AG53" s="12"/>
@@ -12442,13 +12450,13 @@
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="85" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="F54" s="85" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="G54" s="35" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="H54" s="197"/>
       <c r="I54" s="12"/>
@@ -12474,11 +12482,11 @@
         <v>477</v>
       </c>
       <c r="AA54" s="84" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="AB54" s="12"/>
       <c r="AC54" s="12"/>
-      <c r="AD54" s="251"/>
+      <c r="AD54" s="250"/>
       <c r="AE54" s="12"/>
       <c r="AF54" s="12"/>
       <c r="AG54" s="12"/>
@@ -12489,13 +12497,13 @@
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="85" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="F55" s="85" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="G55" s="35" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="H55" s="197"/>
       <c r="I55" s="12"/>
@@ -12521,28 +12529,28 @@
         <v>477</v>
       </c>
       <c r="AA55" s="84" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="AB55" s="12"/>
       <c r="AC55" s="12"/>
-      <c r="AD55" s="251"/>
+      <c r="AD55" s="250"/>
       <c r="AE55" s="12"/>
       <c r="AF55" s="12"/>
       <c r="AG55" s="12"/>
     </row>
-    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="12"/>
       <c r="B56" s="12"/>
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
-      <c r="E56" s="85" t="s">
-        <v>568</v>
-      </c>
-      <c r="F56" s="85" t="s">
-        <v>569</v>
-      </c>
-      <c r="G56" s="35" t="s">
-        <v>570</v>
+      <c r="E56" s="61" t="s">
+        <v>571</v>
+      </c>
+      <c r="F56" s="61" t="s">
+        <v>572</v>
+      </c>
+      <c r="G56" s="51" t="s">
+        <v>573</v>
       </c>
       <c r="H56" s="197"/>
       <c r="I56" s="12"/>
@@ -12567,63 +12575,17 @@
       <c r="Z56" s="39" t="s">
         <v>477</v>
       </c>
-      <c r="AA56" s="84" t="n">
-        <v>3.5</v>
+      <c r="AA56" s="44" t="n">
+        <v>4</v>
       </c>
       <c r="AB56" s="12"/>
       <c r="AC56" s="12"/>
-      <c r="AD56" s="251"/>
+      <c r="AD56" s="250"/>
       <c r="AE56" s="12"/>
       <c r="AF56" s="12"/>
       <c r="AG56" s="12"/>
     </row>
-    <row r="57" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="12"/>
-      <c r="B57" s="12"/>
-      <c r="C57" s="12"/>
-      <c r="D57" s="12"/>
-      <c r="E57" s="61" t="s">
-        <v>571</v>
-      </c>
-      <c r="F57" s="61" t="s">
-        <v>572</v>
-      </c>
-      <c r="G57" s="51" t="s">
-        <v>573</v>
-      </c>
-      <c r="H57" s="197"/>
-      <c r="I57" s="12"/>
-      <c r="J57" s="12"/>
-      <c r="K57" s="12"/>
-      <c r="L57" s="12"/>
-      <c r="M57" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="N57" s="12"/>
-      <c r="O57" s="12"/>
-      <c r="P57" s="12"/>
-      <c r="Q57" s="12"/>
-      <c r="R57" s="12"/>
-      <c r="S57" s="12"/>
-      <c r="T57" s="12"/>
-      <c r="U57" s="12"/>
-      <c r="V57" s="12"/>
-      <c r="W57" s="12"/>
-      <c r="X57" s="12"/>
-      <c r="Y57" s="12"/>
-      <c r="Z57" s="39" t="s">
-        <v>477</v>
-      </c>
-      <c r="AA57" s="44" t="n">
-        <v>4</v>
-      </c>
-      <c r="AB57" s="12"/>
-      <c r="AC57" s="12"/>
-      <c r="AD57" s="251"/>
-      <c r="AE57" s="12"/>
-      <c r="AF57" s="12"/>
-      <c r="AG57" s="12"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Updated with menu capodanno
</commit_message>
<xml_diff>
--- a/excel/DATABASE_MENU_VENDITA.xlsx
+++ b/excel/DATABASE_MENU_VENDITA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LE NOSTRE BIRRE" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="579">
   <si>
     <t xml:space="preserve">macro-category:</t>
   </si>
@@ -975,6 +975,21 @@
   </si>
   <si>
     <t xml:space="preserve">Un dolce al cucchiaio diverso ogni mese. Per il mese di LUGLIO: sorbetto all'anguria.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENU A TEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">menu_tema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MENU CAPODANNO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">capodanno</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Menu di capodanno.</t>
   </si>
   <si>
     <t xml:space="preserve">DRINKS &amp; CAFFÈ</t>
@@ -1752,13 +1767,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="&quot;€ &quot;#,##0.00"/>
     <numFmt numFmtId="166" formatCode="#,##0.00\ [$€-1];[RED]\-#,##0.00\ [$€-1]"/>
     <numFmt numFmtId="167" formatCode="#,##0\ [$€-1];[RED]\-#,##0\ [$€-1]"/>
     <numFmt numFmtId="168" formatCode="0.00"/>
     <numFmt numFmtId="169" formatCode="_-&quot;€ &quot;* #,##0.00_-;&quot;-€ &quot;* #,##0.00_-;_-&quot;€ &quot;* \-??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="[$€-410]\ #,##0.00;[RED]\-[$€-410]\ #,##0.00"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -2104,7 +2120,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="251">
+  <cellXfs count="252">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2847,6 +2863,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -3189,11 +3209,11 @@
   </sheetPr>
   <dimension ref="A1:AG45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AD11" activeCellId="0" sqref="AD11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -4447,12 +4467,12 @@
   <dimension ref="A1:AG47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="4" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="100" width="42"/>
@@ -6357,13 +6377,13 @@
     <tabColor rgb="FFC5E0B4"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB30"/>
+  <dimension ref="A1:AB32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F35" activeCellId="0" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="100" width="42"/>
@@ -7657,6 +7677,28 @@
         <v>4</v>
       </c>
     </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C31" s="180" t="s">
+        <v>317</v>
+      </c>
+      <c r="D31" s="100" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="101" t="s">
+        <v>319</v>
+      </c>
+      <c r="F32" s="101" t="s">
+        <v>320</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AA32" s="186" t="n">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -7680,7 +7722,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="46.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="24.29"/>
@@ -7706,39 +7748,39 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="187" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="187"/>
+      <c r="B1" s="188"/>
       <c r="E1" s="12"/>
       <c r="F1" s="12"/>
-      <c r="G1" s="188"/>
-      <c r="H1" s="188"/>
-      <c r="I1" s="188"/>
-      <c r="J1" s="188"/>
-      <c r="K1" s="188"/>
-      <c r="L1" s="188"/>
-      <c r="M1" s="188"/>
-      <c r="N1" s="188"/>
-      <c r="O1" s="188"/>
-      <c r="P1" s="188"/>
-      <c r="Q1" s="188"/>
-      <c r="R1" s="188"/>
-      <c r="S1" s="188"/>
-      <c r="T1" s="188"/>
-      <c r="U1" s="188"/>
-      <c r="V1" s="188"/>
-      <c r="W1" s="188"/>
-      <c r="X1" s="188"/>
-      <c r="Y1" s="188"/>
-      <c r="Z1" s="188"/>
-      <c r="AA1" s="188"/>
-      <c r="AB1" s="188"/>
-      <c r="AC1" s="188"/>
-      <c r="AD1" s="188"/>
-      <c r="AE1" s="188"/>
-      <c r="AF1" s="188"/>
-      <c r="AG1" s="188"/>
+      <c r="G1" s="189"/>
+      <c r="H1" s="189"/>
+      <c r="I1" s="189"/>
+      <c r="J1" s="189"/>
+      <c r="K1" s="189"/>
+      <c r="L1" s="189"/>
+      <c r="M1" s="189"/>
+      <c r="N1" s="189"/>
+      <c r="O1" s="189"/>
+      <c r="P1" s="189"/>
+      <c r="Q1" s="189"/>
+      <c r="R1" s="189"/>
+      <c r="S1" s="189"/>
+      <c r="T1" s="189"/>
+      <c r="U1" s="189"/>
+      <c r="V1" s="189"/>
+      <c r="W1" s="189"/>
+      <c r="X1" s="189"/>
+      <c r="Y1" s="189"/>
+      <c r="Z1" s="189"/>
+      <c r="AA1" s="189"/>
+      <c r="AB1" s="189"/>
+      <c r="AC1" s="189"/>
+      <c r="AD1" s="189"/>
+      <c r="AE1" s="189"/>
+      <c r="AF1" s="189"/>
+      <c r="AG1" s="189"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="9" t="s">
@@ -7784,10 +7826,10 @@
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="112" t="s">
-        <v>317</v>
+        <v>322</v>
       </c>
       <c r="B3" s="112" t="s">
-        <v>318</v>
+        <v>323</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>2</v>
@@ -7805,7 +7847,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>319</v>
+        <v>324</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -7822,14 +7864,14 @@
       <c r="U3" s="10"/>
       <c r="V3" s="10"/>
       <c r="W3" s="10"/>
-      <c r="X3" s="189"/>
+      <c r="X3" s="190"/>
       <c r="Y3" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="Z3" s="190" t="s">
+      <c r="Z3" s="191" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="191" t="s">
+      <c r="AA3" s="192" t="s">
         <v>12</v>
       </c>
       <c r="AB3" s="23" t="s">
@@ -7838,23 +7880,23 @@
       <c r="AC3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="191" t="s">
+      <c r="AD3" s="192" t="s">
         <v>15</v>
       </c>
       <c r="AE3" s="12"/>
       <c r="AF3" s="12"/>
       <c r="AG3" s="12"/>
     </row>
-    <row r="4" s="194" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="195" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="23"/>
-      <c r="C4" s="192" t="s">
-        <v>320</v>
-      </c>
-      <c r="D4" s="193" t="s">
-        <v>321</v>
+      <c r="C4" s="193" t="s">
+        <v>325</v>
+      </c>
+      <c r="D4" s="194" t="s">
+        <v>326</v>
       </c>
       <c r="H4" s="121" t="s">
         <v>19</v>
@@ -7917,21 +7959,21 @@
       <c r="AF4" s="151"/>
       <c r="AG4" s="151"/>
     </row>
-    <row r="5" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="23"/>
       <c r="B5" s="23"/>
       <c r="C5" s="151"/>
       <c r="D5" s="151"/>
-      <c r="E5" s="195" t="s">
-        <v>322</v>
-      </c>
-      <c r="F5" s="195" t="s">
-        <v>323</v>
-      </c>
-      <c r="G5" s="196" t="s">
-        <v>324</v>
-      </c>
-      <c r="H5" s="197"/>
+      <c r="E5" s="196" t="s">
+        <v>327</v>
+      </c>
+      <c r="F5" s="196" t="s">
+        <v>328</v>
+      </c>
+      <c r="G5" s="197" t="s">
+        <v>329</v>
+      </c>
+      <c r="H5" s="198"/>
       <c r="I5" s="12"/>
       <c r="J5" s="12"/>
       <c r="K5" s="12"/>
@@ -7949,32 +7991,32 @@
       <c r="W5" s="12"/>
       <c r="X5" s="12"/>
       <c r="Y5" s="23"/>
-      <c r="Z5" s="198"/>
+      <c r="Z5" s="199"/>
       <c r="AA5" s="81" t="n">
         <v>6</v>
       </c>
       <c r="AB5" s="23"/>
       <c r="AC5" s="23"/>
-      <c r="AD5" s="199"/>
+      <c r="AD5" s="200"/>
       <c r="AE5" s="23"/>
       <c r="AF5" s="23"/>
-      <c r="AG5" s="191"/>
-    </row>
-    <row r="6" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG5" s="192"/>
+    </row>
+    <row r="6" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23"/>
       <c r="B6" s="23"/>
       <c r="C6" s="151"/>
       <c r="D6" s="151"/>
-      <c r="E6" s="195" t="s">
-        <v>325</v>
-      </c>
-      <c r="F6" s="195" t="s">
-        <v>326</v>
-      </c>
-      <c r="G6" s="196" t="s">
-        <v>327</v>
-      </c>
-      <c r="H6" s="197"/>
+      <c r="E6" s="196" t="s">
+        <v>330</v>
+      </c>
+      <c r="F6" s="196" t="s">
+        <v>331</v>
+      </c>
+      <c r="G6" s="197" t="s">
+        <v>332</v>
+      </c>
+      <c r="H6" s="198"/>
       <c r="I6" s="12"/>
       <c r="J6" s="12"/>
       <c r="K6" s="12"/>
@@ -7992,32 +8034,32 @@
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
       <c r="Y6" s="23"/>
-      <c r="Z6" s="198"/>
+      <c r="Z6" s="199"/>
       <c r="AA6" s="81" t="n">
         <v>6</v>
       </c>
       <c r="AB6" s="23"/>
       <c r="AC6" s="23"/>
-      <c r="AD6" s="199"/>
+      <c r="AD6" s="200"/>
       <c r="AE6" s="23"/>
       <c r="AF6" s="23"/>
-      <c r="AG6" s="191"/>
-    </row>
-    <row r="7" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG6" s="192"/>
+    </row>
+    <row r="7" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23"/>
       <c r="B7" s="23"/>
       <c r="C7" s="151"/>
       <c r="D7" s="151"/>
-      <c r="E7" s="195" t="s">
-        <v>328</v>
-      </c>
-      <c r="F7" s="195" t="s">
-        <v>329</v>
-      </c>
-      <c r="G7" s="196" t="s">
-        <v>330</v>
-      </c>
-      <c r="H7" s="197"/>
+      <c r="E7" s="196" t="s">
+        <v>333</v>
+      </c>
+      <c r="F7" s="196" t="s">
+        <v>334</v>
+      </c>
+      <c r="G7" s="197" t="s">
+        <v>335</v>
+      </c>
+      <c r="H7" s="198"/>
       <c r="I7" s="12"/>
       <c r="J7" s="12"/>
       <c r="K7" s="12"/>
@@ -8035,32 +8077,32 @@
       <c r="W7" s="12"/>
       <c r="X7" s="12"/>
       <c r="Y7" s="23"/>
-      <c r="Z7" s="198"/>
+      <c r="Z7" s="199"/>
       <c r="AA7" s="81" t="n">
         <v>6</v>
       </c>
       <c r="AB7" s="23"/>
       <c r="AC7" s="23"/>
-      <c r="AD7" s="199"/>
+      <c r="AD7" s="200"/>
       <c r="AE7" s="23"/>
       <c r="AF7" s="23"/>
-      <c r="AG7" s="191"/>
-    </row>
-    <row r="8" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG7" s="192"/>
+    </row>
+    <row r="8" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23"/>
       <c r="B8" s="23"/>
       <c r="C8" s="151"/>
       <c r="D8" s="151"/>
-      <c r="E8" s="195" t="s">
-        <v>331</v>
-      </c>
-      <c r="F8" s="195" t="s">
-        <v>332</v>
+      <c r="E8" s="196" t="s">
+        <v>336</v>
+      </c>
+      <c r="F8" s="196" t="s">
+        <v>337</v>
       </c>
       <c r="G8" s="160" t="s">
-        <v>333</v>
-      </c>
-      <c r="H8" s="197"/>
+        <v>338</v>
+      </c>
+      <c r="H8" s="198"/>
       <c r="I8" s="12"/>
       <c r="J8" s="12"/>
       <c r="K8" s="12"/>
@@ -8078,32 +8120,32 @@
       <c r="W8" s="12"/>
       <c r="X8" s="12"/>
       <c r="Y8" s="23"/>
-      <c r="Z8" s="198"/>
+      <c r="Z8" s="199"/>
       <c r="AA8" s="42" t="n">
         <v>6</v>
       </c>
       <c r="AB8" s="23"/>
       <c r="AC8" s="23"/>
-      <c r="AD8" s="191"/>
+      <c r="AD8" s="192"/>
       <c r="AE8" s="23"/>
       <c r="AF8" s="23"/>
-      <c r="AG8" s="191"/>
-    </row>
-    <row r="9" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG8" s="192"/>
+    </row>
+    <row r="9" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="23"/>
       <c r="B9" s="23"/>
       <c r="C9" s="151"/>
       <c r="D9" s="151"/>
-      <c r="E9" s="195" t="s">
-        <v>334</v>
-      </c>
-      <c r="F9" s="195" t="s">
-        <v>335</v>
+      <c r="E9" s="196" t="s">
+        <v>339</v>
+      </c>
+      <c r="F9" s="196" t="s">
+        <v>340</v>
       </c>
       <c r="G9" s="160" t="s">
-        <v>336</v>
-      </c>
-      <c r="H9" s="197"/>
+        <v>341</v>
+      </c>
+      <c r="H9" s="198"/>
       <c r="I9" s="12"/>
       <c r="J9" s="12"/>
       <c r="K9" s="12"/>
@@ -8121,32 +8163,32 @@
       <c r="W9" s="12"/>
       <c r="X9" s="12"/>
       <c r="Y9" s="23"/>
-      <c r="Z9" s="198"/>
+      <c r="Z9" s="199"/>
       <c r="AA9" s="42" t="n">
         <v>6</v>
       </c>
       <c r="AB9" s="23"/>
       <c r="AC9" s="23"/>
-      <c r="AD9" s="191"/>
+      <c r="AD9" s="192"/>
       <c r="AE9" s="23"/>
       <c r="AF9" s="23"/>
-      <c r="AG9" s="191"/>
-    </row>
-    <row r="10" s="194" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG9" s="192"/>
+    </row>
+    <row r="10" s="195" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="151"/>
       <c r="D10" s="151"/>
-      <c r="E10" s="195" t="s">
-        <v>337</v>
-      </c>
-      <c r="F10" s="195" t="s">
-        <v>338</v>
-      </c>
-      <c r="G10" s="196" t="s">
-        <v>339</v>
-      </c>
-      <c r="H10" s="197"/>
+      <c r="E10" s="196" t="s">
+        <v>342</v>
+      </c>
+      <c r="F10" s="196" t="s">
+        <v>343</v>
+      </c>
+      <c r="G10" s="197" t="s">
+        <v>344</v>
+      </c>
+      <c r="H10" s="198"/>
       <c r="I10" s="12"/>
       <c r="J10" s="12"/>
       <c r="K10" s="12"/>
@@ -8164,30 +8206,30 @@
       <c r="W10" s="12"/>
       <c r="X10" s="12"/>
       <c r="Y10" s="23"/>
-      <c r="Z10" s="198"/>
+      <c r="Z10" s="199"/>
       <c r="AA10" s="42" t="n">
         <v>5</v>
       </c>
       <c r="AB10" s="23"/>
       <c r="AC10" s="23"/>
-      <c r="AD10" s="191"/>
+      <c r="AD10" s="192"/>
       <c r="AE10" s="23"/>
       <c r="AF10" s="23"/>
-      <c r="AG10" s="191"/>
-    </row>
-    <row r="11" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG10" s="192"/>
+    </row>
+    <row r="11" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="151"/>
       <c r="D11" s="151"/>
-      <c r="E11" s="195" t="s">
-        <v>340</v>
-      </c>
-      <c r="F11" s="195" t="s">
-        <v>341</v>
+      <c r="E11" s="196" t="s">
+        <v>345</v>
+      </c>
+      <c r="F11" s="196" t="s">
+        <v>346</v>
       </c>
       <c r="G11" s="160"/>
-      <c r="H11" s="197"/>
+      <c r="H11" s="198"/>
       <c r="I11" s="12"/>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
@@ -8205,40 +8247,40 @@
       <c r="W11" s="12"/>
       <c r="X11" s="12"/>
       <c r="Y11" s="23"/>
-      <c r="Z11" s="200" t="s">
-        <v>342</v>
+      <c r="Z11" s="201" t="s">
+        <v>347</v>
       </c>
       <c r="AA11" s="42" t="n">
         <v>7</v>
       </c>
       <c r="AB11" s="23"/>
-      <c r="AC11" s="200" t="s">
-        <v>343</v>
+      <c r="AC11" s="201" t="s">
+        <v>348</v>
       </c>
       <c r="AD11" s="65" t="n">
         <v>9</v>
       </c>
       <c r="AE11" s="23"/>
       <c r="AF11" s="160" t="s">
-        <v>344</v>
+        <v>349</v>
       </c>
       <c r="AG11" s="65" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="12" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
       <c r="C12" s="151"/>
       <c r="D12" s="151"/>
-      <c r="E12" s="195" t="s">
-        <v>345</v>
-      </c>
-      <c r="F12" s="195" t="s">
-        <v>346</v>
+      <c r="E12" s="196" t="s">
+        <v>350</v>
+      </c>
+      <c r="F12" s="196" t="s">
+        <v>351</v>
       </c>
       <c r="G12" s="160"/>
-      <c r="H12" s="197"/>
+      <c r="H12" s="198"/>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
@@ -8256,15 +8298,15 @@
       <c r="W12" s="12"/>
       <c r="X12" s="12"/>
       <c r="Y12" s="23"/>
-      <c r="Z12" s="200" t="s">
-        <v>347</v>
+      <c r="Z12" s="201" t="s">
+        <v>352</v>
       </c>
       <c r="AA12" s="42" t="n">
         <v>6</v>
       </c>
       <c r="AB12" s="23"/>
-      <c r="AC12" s="200" t="s">
-        <v>348</v>
+      <c r="AC12" s="201" t="s">
+        <v>353</v>
       </c>
       <c r="AD12" s="65" t="n">
         <v>11</v>
@@ -8273,21 +8315,21 @@
       <c r="AF12" s="160"/>
       <c r="AG12" s="65"/>
     </row>
-    <row r="13" s="194" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="13" s="195" customFormat="true" ht="49.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="23"/>
       <c r="B13" s="23"/>
       <c r="C13" s="151"/>
       <c r="D13" s="151"/>
-      <c r="E13" s="195" t="s">
-        <v>349</v>
-      </c>
-      <c r="F13" s="195" t="s">
-        <v>350</v>
+      <c r="E13" s="196" t="s">
+        <v>354</v>
+      </c>
+      <c r="F13" s="196" t="s">
+        <v>355</v>
       </c>
       <c r="G13" s="160" t="s">
-        <v>351</v>
-      </c>
-      <c r="H13" s="197"/>
+        <v>356</v>
+      </c>
+      <c r="H13" s="198"/>
       <c r="I13" s="12"/>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
@@ -8305,30 +8347,30 @@
       <c r="W13" s="12"/>
       <c r="X13" s="12"/>
       <c r="Y13" s="23"/>
-      <c r="Z13" s="198"/>
+      <c r="Z13" s="199"/>
       <c r="AA13" s="42" t="n">
         <v>7</v>
       </c>
       <c r="AB13" s="23"/>
       <c r="AC13" s="23"/>
-      <c r="AD13" s="191"/>
+      <c r="AD13" s="192"/>
       <c r="AE13" s="23"/>
       <c r="AF13" s="23"/>
-      <c r="AG13" s="191"/>
-    </row>
-    <row r="14" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG13" s="192"/>
+    </row>
+    <row r="14" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23"/>
       <c r="B14" s="105"/>
-      <c r="E14" s="195" t="s">
-        <v>352</v>
-      </c>
-      <c r="F14" s="195" t="s">
-        <v>353</v>
-      </c>
-      <c r="G14" s="196" t="s">
-        <v>354</v>
-      </c>
-      <c r="H14" s="197"/>
+      <c r="E14" s="196" t="s">
+        <v>357</v>
+      </c>
+      <c r="F14" s="196" t="s">
+        <v>358</v>
+      </c>
+      <c r="G14" s="197" t="s">
+        <v>359</v>
+      </c>
+      <c r="H14" s="198"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -8346,32 +8388,32 @@
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="23"/>
-      <c r="Z14" s="198"/>
+      <c r="Z14" s="199"/>
       <c r="AA14" s="42" t="n">
         <v>6</v>
       </c>
       <c r="AB14" s="23"/>
       <c r="AC14" s="23"/>
-      <c r="AD14" s="191"/>
+      <c r="AD14" s="192"/>
       <c r="AE14" s="23"/>
       <c r="AF14" s="23"/>
-      <c r="AG14" s="191"/>
-    </row>
-    <row r="15" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG14" s="192"/>
+    </row>
+    <row r="15" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="151"/>
       <c r="D15" s="151"/>
-      <c r="E15" s="195" t="s">
-        <v>355</v>
-      </c>
-      <c r="F15" s="195" t="s">
-        <v>356</v>
-      </c>
-      <c r="G15" s="196" t="s">
-        <v>357</v>
-      </c>
-      <c r="H15" s="197"/>
+      <c r="E15" s="196" t="s">
+        <v>360</v>
+      </c>
+      <c r="F15" s="196" t="s">
+        <v>361</v>
+      </c>
+      <c r="G15" s="197" t="s">
+        <v>362</v>
+      </c>
+      <c r="H15" s="198"/>
       <c r="I15" s="12"/>
       <c r="J15" s="12"/>
       <c r="K15" s="12"/>
@@ -8389,32 +8431,32 @@
       <c r="W15" s="12"/>
       <c r="X15" s="12"/>
       <c r="Y15" s="23"/>
-      <c r="Z15" s="198"/>
+      <c r="Z15" s="199"/>
       <c r="AA15" s="42" t="n">
         <v>6</v>
       </c>
       <c r="AB15" s="23"/>
       <c r="AC15" s="23"/>
-      <c r="AD15" s="191"/>
+      <c r="AD15" s="192"/>
       <c r="AE15" s="23"/>
       <c r="AF15" s="23"/>
-      <c r="AG15" s="191"/>
-    </row>
-    <row r="16" s="194" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG15" s="192"/>
+    </row>
+    <row r="16" s="195" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="151"/>
       <c r="D16" s="151"/>
-      <c r="E16" s="195" t="s">
-        <v>358</v>
-      </c>
-      <c r="F16" s="195" t="s">
-        <v>359</v>
-      </c>
-      <c r="G16" s="196" t="s">
-        <v>360</v>
-      </c>
-      <c r="H16" s="197"/>
+      <c r="E16" s="196" t="s">
+        <v>363</v>
+      </c>
+      <c r="F16" s="196" t="s">
+        <v>364</v>
+      </c>
+      <c r="G16" s="197" t="s">
+        <v>365</v>
+      </c>
+      <c r="H16" s="198"/>
       <c r="I16" s="12"/>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
@@ -8432,32 +8474,32 @@
       <c r="W16" s="12"/>
       <c r="X16" s="12"/>
       <c r="Y16" s="23"/>
-      <c r="Z16" s="198"/>
+      <c r="Z16" s="199"/>
       <c r="AA16" s="42" t="n">
         <v>6</v>
       </c>
       <c r="AB16" s="23"/>
       <c r="AC16" s="23"/>
-      <c r="AD16" s="191"/>
+      <c r="AD16" s="192"/>
       <c r="AE16" s="23"/>
       <c r="AF16" s="23"/>
-      <c r="AG16" s="191"/>
-    </row>
-    <row r="17" s="194" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG16" s="192"/>
+    </row>
+    <row r="17" s="195" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="151"/>
       <c r="D17" s="151"/>
-      <c r="E17" s="195" t="s">
-        <v>361</v>
-      </c>
-      <c r="F17" s="195" t="s">
-        <v>362</v>
-      </c>
-      <c r="G17" s="196" t="s">
-        <v>363</v>
-      </c>
-      <c r="H17" s="197"/>
+      <c r="E17" s="196" t="s">
+        <v>366</v>
+      </c>
+      <c r="F17" s="196" t="s">
+        <v>367</v>
+      </c>
+      <c r="G17" s="197" t="s">
+        <v>368</v>
+      </c>
+      <c r="H17" s="198"/>
       <c r="I17" s="12"/>
       <c r="J17" s="12"/>
       <c r="K17" s="12"/>
@@ -8475,32 +8517,32 @@
       <c r="W17" s="12"/>
       <c r="X17" s="12"/>
       <c r="Y17" s="23"/>
-      <c r="Z17" s="198"/>
+      <c r="Z17" s="199"/>
       <c r="AA17" s="42" t="n">
         <v>6</v>
       </c>
       <c r="AB17" s="23"/>
       <c r="AC17" s="23"/>
-      <c r="AD17" s="191"/>
+      <c r="AD17" s="192"/>
       <c r="AE17" s="23"/>
       <c r="AF17" s="23"/>
-      <c r="AG17" s="191"/>
-    </row>
-    <row r="18" s="194" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG17" s="192"/>
+    </row>
+    <row r="18" s="195" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="151"/>
       <c r="B18" s="151"/>
       <c r="C18" s="151"/>
-      <c r="D18" s="201"/>
-      <c r="E18" s="195" t="s">
-        <v>364</v>
-      </c>
-      <c r="F18" s="195" t="s">
-        <v>365</v>
+      <c r="D18" s="202"/>
+      <c r="E18" s="196" t="s">
+        <v>369</v>
+      </c>
+      <c r="F18" s="196" t="s">
+        <v>370</v>
       </c>
       <c r="G18" s="160" t="s">
-        <v>366</v>
-      </c>
-      <c r="H18" s="197"/>
+        <v>371</v>
+      </c>
+      <c r="H18" s="198"/>
       <c r="I18" s="12"/>
       <c r="J18" s="12"/>
       <c r="K18" s="12"/>
@@ -8518,32 +8560,32 @@
       <c r="W18" s="12"/>
       <c r="X18" s="12"/>
       <c r="Y18" s="23"/>
-      <c r="Z18" s="198"/>
+      <c r="Z18" s="199"/>
       <c r="AA18" s="42" t="n">
         <v>8</v>
       </c>
       <c r="AB18" s="23"/>
       <c r="AC18" s="23"/>
-      <c r="AD18" s="191"/>
+      <c r="AD18" s="192"/>
       <c r="AE18" s="23"/>
       <c r="AF18" s="23"/>
-      <c r="AG18" s="191"/>
-    </row>
-    <row r="19" s="194" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AG18" s="192"/>
+    </row>
+    <row r="19" s="195" customFormat="true" ht="60" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="151"/>
       <c r="B19" s="151"/>
       <c r="C19" s="151"/>
       <c r="D19" s="151"/>
-      <c r="E19" s="195" t="s">
-        <v>367</v>
-      </c>
-      <c r="F19" s="195" t="s">
-        <v>368</v>
-      </c>
-      <c r="G19" s="202" t="s">
-        <v>369</v>
-      </c>
-      <c r="H19" s="197"/>
+      <c r="E19" s="196" t="s">
+        <v>372</v>
+      </c>
+      <c r="F19" s="196" t="s">
+        <v>373</v>
+      </c>
+      <c r="G19" s="203" t="s">
+        <v>374</v>
+      </c>
+      <c r="H19" s="198"/>
       <c r="I19" s="12"/>
       <c r="J19" s="12"/>
       <c r="K19" s="12"/>
@@ -8561,32 +8603,32 @@
       <c r="W19" s="12"/>
       <c r="X19" s="12"/>
       <c r="Y19" s="23"/>
-      <c r="Z19" s="198"/>
+      <c r="Z19" s="199"/>
       <c r="AA19" s="42" t="n">
         <v>8</v>
       </c>
       <c r="AB19" s="23"/>
       <c r="AC19" s="23"/>
-      <c r="AD19" s="191"/>
+      <c r="AD19" s="192"/>
       <c r="AE19" s="23"/>
       <c r="AF19" s="23"/>
-      <c r="AG19" s="191"/>
+      <c r="AG19" s="192"/>
     </row>
     <row r="20" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
-      <c r="E20" s="195" t="s">
-        <v>370</v>
-      </c>
-      <c r="F20" s="195" t="s">
-        <v>371</v>
-      </c>
-      <c r="G20" s="202" t="s">
-        <v>372</v>
-      </c>
-      <c r="H20" s="197"/>
+      <c r="E20" s="196" t="s">
+        <v>375</v>
+      </c>
+      <c r="F20" s="196" t="s">
+        <v>376</v>
+      </c>
+      <c r="G20" s="203" t="s">
+        <v>377</v>
+      </c>
+      <c r="H20" s="198"/>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
       <c r="K20" s="12"/>
@@ -8620,16 +8662,16 @@
       <c r="B21" s="165"/>
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
-      <c r="E21" s="195" t="s">
-        <v>373</v>
-      </c>
-      <c r="F21" s="195" t="s">
-        <v>374</v>
-      </c>
-      <c r="G21" s="202" t="s">
-        <v>375</v>
-      </c>
-      <c r="H21" s="197"/>
+      <c r="E21" s="196" t="s">
+        <v>378</v>
+      </c>
+      <c r="F21" s="196" t="s">
+        <v>379</v>
+      </c>
+      <c r="G21" s="203" t="s">
+        <v>380</v>
+      </c>
+      <c r="H21" s="198"/>
       <c r="I21" s="12"/>
       <c r="J21" s="12"/>
       <c r="K21" s="12"/>
@@ -8662,15 +8704,15 @@
       <c r="A22" s="112"/>
       <c r="B22" s="112"/>
       <c r="C22" s="36" t="s">
-        <v>376</v>
-      </c>
-      <c r="D22" s="203" t="s">
-        <v>377</v>
+        <v>381</v>
+      </c>
+      <c r="D22" s="204" t="s">
+        <v>382</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
       <c r="G22" s="10"/>
-      <c r="H22" s="197"/>
+      <c r="H22" s="198"/>
       <c r="I22" s="12"/>
       <c r="J22" s="12"/>
       <c r="K22" s="12"/>
@@ -8688,11 +8730,11 @@
       <c r="W22" s="12"/>
       <c r="X22" s="12"/>
       <c r="Y22" s="23"/>
-      <c r="Z22" s="190"/>
-      <c r="AA22" s="191"/>
+      <c r="Z22" s="191"/>
+      <c r="AA22" s="192"/>
       <c r="AB22" s="23"/>
       <c r="AC22" s="23"/>
-      <c r="AD22" s="191"/>
+      <c r="AD22" s="192"/>
       <c r="AE22" s="12"/>
       <c r="AF22" s="12"/>
       <c r="AG22" s="12"/>
@@ -8703,15 +8745,15 @@
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="31" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>379</v>
+        <v>384</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>380</v>
-      </c>
-      <c r="H23" s="204"/>
+        <v>385</v>
+      </c>
+      <c r="H23" s="205"/>
       <c r="I23" s="33"/>
       <c r="J23" s="33"/>
       <c r="K23" s="33"/>
@@ -8728,18 +8770,18 @@
       <c r="V23" s="33"/>
       <c r="W23" s="33"/>
       <c r="X23" s="33"/>
-      <c r="Y23" s="205"/>
-      <c r="Z23" s="206" t="s">
+      <c r="Y23" s="206"/>
+      <c r="Z23" s="207" t="s">
         <v>47</v>
       </c>
-      <c r="AA23" s="207" t="n">
-        <v>1</v>
-      </c>
-      <c r="AB23" s="208"/>
-      <c r="AC23" s="208" t="s">
-        <v>381</v>
-      </c>
-      <c r="AD23" s="207" t="n">
+      <c r="AA23" s="208" t="n">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="209"/>
+      <c r="AC23" s="209" t="s">
+        <v>386</v>
+      </c>
+      <c r="AD23" s="208" t="n">
         <v>2</v>
       </c>
       <c r="AE23" s="12"/>
@@ -8752,15 +8794,15 @@
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="31" t="s">
-        <v>382</v>
+        <v>387</v>
       </c>
       <c r="F24" s="31" t="s">
-        <v>383</v>
+        <v>388</v>
       </c>
       <c r="G24" s="33" t="s">
-        <v>380</v>
-      </c>
-      <c r="H24" s="204"/>
+        <v>385</v>
+      </c>
+      <c r="H24" s="205"/>
       <c r="I24" s="33"/>
       <c r="J24" s="33"/>
       <c r="K24" s="33"/>
@@ -8777,12 +8819,12 @@
       <c r="V24" s="33"/>
       <c r="W24" s="33"/>
       <c r="X24" s="33"/>
-      <c r="Y24" s="205"/>
-      <c r="Z24" s="206"/>
-      <c r="AA24" s="207"/>
-      <c r="AB24" s="208"/>
-      <c r="AC24" s="208"/>
-      <c r="AD24" s="207"/>
+      <c r="Y24" s="206"/>
+      <c r="Z24" s="207"/>
+      <c r="AA24" s="208"/>
+      <c r="AB24" s="209"/>
+      <c r="AC24" s="209"/>
+      <c r="AD24" s="208"/>
       <c r="AE24" s="12"/>
       <c r="AF24" s="12"/>
       <c r="AG24" s="12"/>
@@ -8793,15 +8835,15 @@
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="31" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>385</v>
+        <v>390</v>
       </c>
       <c r="G25" s="33" t="s">
-        <v>386</v>
-      </c>
-      <c r="H25" s="204"/>
+        <v>391</v>
+      </c>
+      <c r="H25" s="205"/>
       <c r="I25" s="33"/>
       <c r="J25" s="33"/>
       <c r="K25" s="33"/>
@@ -8818,18 +8860,18 @@
       <c r="V25" s="33"/>
       <c r="W25" s="33"/>
       <c r="X25" s="33"/>
-      <c r="Y25" s="205"/>
-      <c r="Z25" s="206" t="s">
+      <c r="Y25" s="206"/>
+      <c r="Z25" s="207" t="s">
         <v>76</v>
       </c>
-      <c r="AA25" s="207" t="n">
+      <c r="AA25" s="208" t="n">
         <v>3</v>
       </c>
-      <c r="AB25" s="208"/>
-      <c r="AC25" s="208" t="s">
-        <v>387</v>
-      </c>
-      <c r="AD25" s="207" t="n">
+      <c r="AB25" s="209"/>
+      <c r="AC25" s="209" t="s">
+        <v>392</v>
+      </c>
+      <c r="AD25" s="208" t="n">
         <v>4</v>
       </c>
       <c r="AE25" s="12"/>
@@ -8842,15 +8884,15 @@
       <c r="C26" s="35"/>
       <c r="D26" s="35"/>
       <c r="E26" s="85" t="s">
-        <v>388</v>
+        <v>393</v>
       </c>
       <c r="F26" s="85" t="s">
-        <v>389</v>
+        <v>394</v>
       </c>
       <c r="G26" s="33" t="s">
-        <v>386</v>
-      </c>
-      <c r="H26" s="204"/>
+        <v>391</v>
+      </c>
+      <c r="H26" s="205"/>
       <c r="I26" s="33"/>
       <c r="J26" s="33"/>
       <c r="K26" s="33"/>
@@ -8867,16 +8909,16 @@
       <c r="V26" s="33"/>
       <c r="W26" s="33"/>
       <c r="X26" s="33"/>
-      <c r="Y26" s="205"/>
-      <c r="Z26" s="206" t="s">
+      <c r="Y26" s="206"/>
+      <c r="Z26" s="207" t="s">
         <v>76</v>
       </c>
-      <c r="AA26" s="207" t="n">
+      <c r="AA26" s="208" t="n">
         <v>3</v>
       </c>
-      <c r="AB26" s="208"/>
-      <c r="AC26" s="208"/>
-      <c r="AD26" s="207"/>
+      <c r="AB26" s="209"/>
+      <c r="AC26" s="209"/>
+      <c r="AD26" s="208"/>
       <c r="AE26" s="12"/>
       <c r="AF26" s="12"/>
       <c r="AG26" s="12"/>
@@ -8887,15 +8929,15 @@
       <c r="C27" s="35"/>
       <c r="D27" s="35"/>
       <c r="E27" s="85" t="s">
-        <v>390</v>
+        <v>395</v>
       </c>
       <c r="F27" s="85" t="s">
+        <v>396</v>
+      </c>
+      <c r="G27" s="33" t="s">
         <v>391</v>
       </c>
-      <c r="G27" s="33" t="s">
-        <v>386</v>
-      </c>
-      <c r="H27" s="204"/>
+      <c r="H27" s="205"/>
       <c r="I27" s="33"/>
       <c r="J27" s="33"/>
       <c r="K27" s="33"/>
@@ -8912,16 +8954,16 @@
       <c r="V27" s="33"/>
       <c r="W27" s="33"/>
       <c r="X27" s="33"/>
-      <c r="Y27" s="205"/>
-      <c r="Z27" s="206" t="s">
+      <c r="Y27" s="206"/>
+      <c r="Z27" s="207" t="s">
         <v>76</v>
       </c>
-      <c r="AA27" s="207" t="n">
+      <c r="AA27" s="208" t="n">
         <v>3</v>
       </c>
-      <c r="AB27" s="208"/>
-      <c r="AC27" s="208"/>
-      <c r="AD27" s="207"/>
+      <c r="AB27" s="209"/>
+      <c r="AC27" s="209"/>
+      <c r="AD27" s="208"/>
       <c r="AE27" s="12"/>
       <c r="AF27" s="12"/>
       <c r="AG27" s="12"/>
@@ -8932,15 +8974,15 @@
       <c r="C28" s="35"/>
       <c r="D28" s="35"/>
       <c r="E28" s="85" t="s">
-        <v>392</v>
+        <v>397</v>
       </c>
       <c r="F28" s="85" t="s">
-        <v>393</v>
+        <v>398</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>394</v>
-      </c>
-      <c r="H28" s="204"/>
+        <v>399</v>
+      </c>
+      <c r="H28" s="205"/>
       <c r="I28" s="33"/>
       <c r="J28" s="33"/>
       <c r="K28" s="33"/>
@@ -8957,14 +8999,14 @@
       <c r="V28" s="33"/>
       <c r="W28" s="33"/>
       <c r="X28" s="33"/>
-      <c r="Y28" s="205"/>
-      <c r="Z28" s="206"/>
-      <c r="AA28" s="207" t="n">
+      <c r="Y28" s="206"/>
+      <c r="Z28" s="207"/>
+      <c r="AA28" s="208" t="n">
         <v>3.5</v>
       </c>
-      <c r="AB28" s="208"/>
-      <c r="AC28" s="208"/>
-      <c r="AD28" s="207"/>
+      <c r="AB28" s="209"/>
+      <c r="AC28" s="209"/>
+      <c r="AD28" s="208"/>
       <c r="AE28" s="12"/>
       <c r="AF28" s="12"/>
       <c r="AG28" s="12"/>
@@ -8975,13 +9017,13 @@
       <c r="C29" s="35"/>
       <c r="D29" s="35"/>
       <c r="E29" s="85" t="s">
-        <v>395</v>
+        <v>400</v>
       </c>
       <c r="F29" s="85" t="s">
-        <v>396</v>
+        <v>401</v>
       </c>
       <c r="G29" s="33"/>
-      <c r="H29" s="204"/>
+      <c r="H29" s="205"/>
       <c r="I29" s="33"/>
       <c r="J29" s="33"/>
       <c r="K29" s="33"/>
@@ -8998,14 +9040,14 @@
       <c r="V29" s="33"/>
       <c r="W29" s="33"/>
       <c r="X29" s="33"/>
-      <c r="Y29" s="205"/>
-      <c r="Z29" s="206"/>
-      <c r="AA29" s="207" t="n">
+      <c r="Y29" s="206"/>
+      <c r="Z29" s="207"/>
+      <c r="AA29" s="208" t="n">
         <v>3.5</v>
       </c>
-      <c r="AB29" s="208"/>
-      <c r="AC29" s="208"/>
-      <c r="AD29" s="207"/>
+      <c r="AB29" s="209"/>
+      <c r="AC29" s="209"/>
+      <c r="AD29" s="208"/>
       <c r="AE29" s="12"/>
       <c r="AF29" s="12"/>
       <c r="AG29" s="12"/>
@@ -9016,15 +9058,15 @@
       <c r="C30" s="35"/>
       <c r="D30" s="35"/>
       <c r="E30" s="60" t="s">
-        <v>397</v>
+        <v>402</v>
       </c>
       <c r="F30" s="60" t="s">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>399</v>
-      </c>
-      <c r="H30" s="204"/>
+        <v>404</v>
+      </c>
+      <c r="H30" s="205"/>
       <c r="I30" s="33"/>
       <c r="J30" s="33"/>
       <c r="K30" s="33"/>
@@ -9041,14 +9083,14 @@
       <c r="V30" s="33"/>
       <c r="W30" s="33"/>
       <c r="X30" s="33"/>
-      <c r="Y30" s="205"/>
-      <c r="Z30" s="206"/>
-      <c r="AA30" s="207" t="n">
+      <c r="Y30" s="206"/>
+      <c r="Z30" s="207"/>
+      <c r="AA30" s="208" t="n">
         <v>2.5</v>
       </c>
-      <c r="AB30" s="208"/>
-      <c r="AC30" s="208"/>
-      <c r="AD30" s="207"/>
+      <c r="AB30" s="209"/>
+      <c r="AC30" s="209"/>
+      <c r="AD30" s="208"/>
       <c r="AE30" s="12"/>
       <c r="AF30" s="12"/>
       <c r="AG30" s="12"/>
@@ -9059,15 +9101,15 @@
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
       <c r="E31" s="31" t="s">
-        <v>400</v>
+        <v>405</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>394</v>
-      </c>
-      <c r="H31" s="204"/>
+        <v>399</v>
+      </c>
+      <c r="H31" s="205"/>
       <c r="I31" s="33"/>
       <c r="J31" s="33"/>
       <c r="K31" s="33"/>
@@ -9084,14 +9126,14 @@
       <c r="V31" s="33"/>
       <c r="W31" s="33"/>
       <c r="X31" s="33"/>
-      <c r="Y31" s="205"/>
-      <c r="Z31" s="206"/>
-      <c r="AA31" s="207" t="n">
+      <c r="Y31" s="206"/>
+      <c r="Z31" s="207"/>
+      <c r="AA31" s="208" t="n">
         <v>3.5</v>
       </c>
-      <c r="AB31" s="208"/>
-      <c r="AC31" s="208"/>
-      <c r="AD31" s="207"/>
+      <c r="AB31" s="209"/>
+      <c r="AC31" s="209"/>
+      <c r="AD31" s="208"/>
       <c r="AE31" s="12"/>
       <c r="AF31" s="12"/>
       <c r="AG31" s="12"/>
@@ -9099,18 +9141,18 @@
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="23"/>
       <c r="B32" s="23"/>
-      <c r="C32" s="209"/>
-      <c r="D32" s="209"/>
-      <c r="E32" s="210" t="s">
-        <v>402</v>
+      <c r="C32" s="210"/>
+      <c r="D32" s="210"/>
+      <c r="E32" s="211" t="s">
+        <v>407</v>
       </c>
       <c r="F32" s="61" t="s">
-        <v>403</v>
+        <v>408</v>
       </c>
       <c r="G32" s="33" t="s">
-        <v>394</v>
-      </c>
-      <c r="H32" s="204"/>
+        <v>399</v>
+      </c>
+      <c r="H32" s="205"/>
       <c r="I32" s="33"/>
       <c r="J32" s="33"/>
       <c r="K32" s="33"/>
@@ -9127,14 +9169,14 @@
       <c r="V32" s="33"/>
       <c r="W32" s="33"/>
       <c r="X32" s="33"/>
-      <c r="Y32" s="205"/>
-      <c r="Z32" s="206"/>
-      <c r="AA32" s="207" t="n">
+      <c r="Y32" s="206"/>
+      <c r="Z32" s="207"/>
+      <c r="AA32" s="208" t="n">
         <v>4</v>
       </c>
-      <c r="AB32" s="208"/>
-      <c r="AC32" s="208"/>
-      <c r="AD32" s="207"/>
+      <c r="AB32" s="209"/>
+      <c r="AC32" s="209"/>
+      <c r="AD32" s="208"/>
       <c r="AE32" s="12"/>
       <c r="AF32" s="12"/>
       <c r="AG32" s="12"/>
@@ -9142,18 +9184,18 @@
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="23"/>
       <c r="B33" s="23"/>
-      <c r="C33" s="209"/>
-      <c r="D33" s="209"/>
-      <c r="E33" s="210" t="s">
-        <v>404</v>
+      <c r="C33" s="210"/>
+      <c r="D33" s="210"/>
+      <c r="E33" s="211" t="s">
+        <v>409</v>
       </c>
       <c r="F33" s="61" t="s">
-        <v>405</v>
+        <v>410</v>
       </c>
       <c r="G33" s="33" t="s">
-        <v>394</v>
-      </c>
-      <c r="H33" s="204"/>
+        <v>399</v>
+      </c>
+      <c r="H33" s="205"/>
       <c r="I33" s="33"/>
       <c r="J33" s="33"/>
       <c r="K33" s="33"/>
@@ -9170,14 +9212,14 @@
       <c r="V33" s="33"/>
       <c r="W33" s="33"/>
       <c r="X33" s="33"/>
-      <c r="Y33" s="205"/>
-      <c r="Z33" s="206"/>
-      <c r="AA33" s="207" t="n">
+      <c r="Y33" s="206"/>
+      <c r="Z33" s="207"/>
+      <c r="AA33" s="208" t="n">
         <v>4</v>
       </c>
-      <c r="AB33" s="208"/>
-      <c r="AC33" s="208"/>
-      <c r="AD33" s="207"/>
+      <c r="AB33" s="209"/>
+      <c r="AC33" s="209"/>
+      <c r="AD33" s="208"/>
       <c r="AE33" s="12"/>
       <c r="AF33" s="12"/>
       <c r="AG33" s="12"/>
@@ -9188,15 +9230,15 @@
       <c r="C34" s="35"/>
       <c r="D34" s="35"/>
       <c r="E34" s="31" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>380</v>
-      </c>
-      <c r="H34" s="204"/>
+        <v>385</v>
+      </c>
+      <c r="H34" s="205"/>
       <c r="I34" s="33"/>
       <c r="J34" s="33"/>
       <c r="K34" s="33"/>
@@ -9213,14 +9255,14 @@
       <c r="V34" s="33"/>
       <c r="W34" s="33"/>
       <c r="X34" s="33"/>
-      <c r="Y34" s="205"/>
-      <c r="Z34" s="206"/>
-      <c r="AA34" s="207" t="n">
+      <c r="Y34" s="206"/>
+      <c r="Z34" s="207"/>
+      <c r="AA34" s="208" t="n">
         <v>3</v>
       </c>
-      <c r="AB34" s="208"/>
-      <c r="AC34" s="208"/>
-      <c r="AD34" s="207"/>
+      <c r="AB34" s="209"/>
+      <c r="AC34" s="209"/>
+      <c r="AD34" s="208"/>
       <c r="AE34" s="12"/>
       <c r="AF34" s="12"/>
       <c r="AG34" s="12"/>
@@ -9231,15 +9273,15 @@
       <c r="C35" s="35"/>
       <c r="D35" s="35"/>
       <c r="E35" s="31" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>380</v>
-      </c>
-      <c r="H35" s="204"/>
+        <v>385</v>
+      </c>
+      <c r="H35" s="205"/>
       <c r="I35" s="33"/>
       <c r="J35" s="33"/>
       <c r="K35" s="33"/>
@@ -9256,14 +9298,14 @@
       <c r="V35" s="33"/>
       <c r="W35" s="33"/>
       <c r="X35" s="33"/>
-      <c r="Y35" s="205"/>
-      <c r="Z35" s="206"/>
-      <c r="AA35" s="207" t="n">
+      <c r="Y35" s="206"/>
+      <c r="Z35" s="207"/>
+      <c r="AA35" s="208" t="n">
         <v>2.5</v>
       </c>
-      <c r="AB35" s="208"/>
-      <c r="AC35" s="208"/>
-      <c r="AD35" s="207"/>
+      <c r="AB35" s="209"/>
+      <c r="AC35" s="209"/>
+      <c r="AD35" s="208"/>
       <c r="AE35" s="12"/>
       <c r="AF35" s="12"/>
       <c r="AG35" s="12"/>
@@ -9274,15 +9316,15 @@
       <c r="C36" s="35"/>
       <c r="D36" s="35"/>
       <c r="E36" s="31" t="s">
-        <v>410</v>
+        <v>415</v>
       </c>
       <c r="F36" s="31" t="s">
-        <v>411</v>
+        <v>416</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>380</v>
-      </c>
-      <c r="H36" s="204"/>
+        <v>385</v>
+      </c>
+      <c r="H36" s="205"/>
       <c r="I36" s="33"/>
       <c r="J36" s="33"/>
       <c r="K36" s="33"/>
@@ -9299,14 +9341,14 @@
       <c r="V36" s="33"/>
       <c r="W36" s="33"/>
       <c r="X36" s="33"/>
-      <c r="Y36" s="205"/>
-      <c r="Z36" s="206"/>
-      <c r="AA36" s="207" t="n">
+      <c r="Y36" s="206"/>
+      <c r="Z36" s="207"/>
+      <c r="AA36" s="208" t="n">
         <v>4</v>
       </c>
-      <c r="AB36" s="208"/>
-      <c r="AC36" s="208"/>
-      <c r="AD36" s="207"/>
+      <c r="AB36" s="209"/>
+      <c r="AC36" s="209"/>
+      <c r="AD36" s="208"/>
       <c r="AE36" s="12"/>
       <c r="AF36" s="12"/>
       <c r="AG36" s="12"/>
@@ -9317,15 +9359,15 @@
       <c r="C37" s="35"/>
       <c r="D37" s="35"/>
       <c r="E37" s="31" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="F37" s="31" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>380</v>
-      </c>
-      <c r="H37" s="204"/>
+        <v>385</v>
+      </c>
+      <c r="H37" s="205"/>
       <c r="I37" s="33"/>
       <c r="J37" s="33"/>
       <c r="K37" s="33"/>
@@ -9342,14 +9384,14 @@
       <c r="V37" s="33"/>
       <c r="W37" s="33"/>
       <c r="X37" s="33"/>
-      <c r="Y37" s="205"/>
-      <c r="Z37" s="206"/>
-      <c r="AA37" s="207" t="n">
+      <c r="Y37" s="206"/>
+      <c r="Z37" s="207"/>
+      <c r="AA37" s="208" t="n">
         <v>4</v>
       </c>
-      <c r="AB37" s="208"/>
-      <c r="AC37" s="208"/>
-      <c r="AD37" s="207"/>
+      <c r="AB37" s="209"/>
+      <c r="AC37" s="209"/>
+      <c r="AD37" s="208"/>
       <c r="AE37" s="12"/>
       <c r="AF37" s="12"/>
       <c r="AG37" s="12"/>
@@ -9360,15 +9402,15 @@
       <c r="C38" s="35"/>
       <c r="D38" s="35"/>
       <c r="E38" s="31" t="s">
-        <v>414</v>
+        <v>419</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>415</v>
+        <v>420</v>
       </c>
       <c r="G38" s="33" t="s">
-        <v>416</v>
-      </c>
-      <c r="H38" s="204"/>
+        <v>421</v>
+      </c>
+      <c r="H38" s="205"/>
       <c r="I38" s="33"/>
       <c r="J38" s="33"/>
       <c r="K38" s="33"/>
@@ -9385,14 +9427,14 @@
       <c r="V38" s="33"/>
       <c r="W38" s="33"/>
       <c r="X38" s="33"/>
-      <c r="Y38" s="205"/>
-      <c r="Z38" s="206"/>
-      <c r="AA38" s="207" t="n">
+      <c r="Y38" s="206"/>
+      <c r="Z38" s="207"/>
+      <c r="AA38" s="208" t="n">
         <v>4</v>
       </c>
-      <c r="AB38" s="208"/>
-      <c r="AC38" s="208"/>
-      <c r="AD38" s="207"/>
+      <c r="AB38" s="209"/>
+      <c r="AC38" s="209"/>
+      <c r="AD38" s="208"/>
       <c r="AE38" s="12"/>
       <c r="AF38" s="12"/>
       <c r="AG38" s="12"/>
@@ -9400,15 +9442,15 @@
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="29"/>
       <c r="B39" s="29"/>
-      <c r="C39" s="211" t="s">
-        <v>417</v>
-      </c>
-      <c r="D39" s="212" t="s">
-        <v>418</v>
+      <c r="C39" s="212" t="s">
+        <v>422</v>
+      </c>
+      <c r="D39" s="213" t="s">
+        <v>423</v>
       </c>
       <c r="E39" s="12"/>
       <c r="G39" s="12"/>
-      <c r="H39" s="197"/>
+      <c r="H39" s="198"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
@@ -9427,7 +9469,7 @@
       <c r="X39" s="12"/>
       <c r="Y39" s="12"/>
       <c r="Z39" s="12"/>
-      <c r="AA39" s="213"/>
+      <c r="AA39" s="214"/>
       <c r="AB39" s="12"/>
       <c r="AC39" s="12"/>
       <c r="AD39" s="12"/>
@@ -9440,14 +9482,14 @@
       <c r="B40" s="29"/>
       <c r="C40" s="12"/>
       <c r="D40" s="165"/>
-      <c r="E40" s="214" t="s">
-        <v>419</v>
-      </c>
-      <c r="F40" s="214" t="s">
-        <v>420</v>
+      <c r="E40" s="215" t="s">
+        <v>424</v>
+      </c>
+      <c r="F40" s="215" t="s">
+        <v>425</v>
       </c>
       <c r="G40" s="51"/>
-      <c r="H40" s="215"/>
+      <c r="H40" s="216"/>
       <c r="I40" s="51"/>
       <c r="J40" s="51"/>
       <c r="K40" s="51"/>
@@ -9481,14 +9523,14 @@
       <c r="B41" s="29"/>
       <c r="C41" s="12"/>
       <c r="D41" s="165"/>
-      <c r="E41" s="214" t="s">
-        <v>421</v>
-      </c>
-      <c r="F41" s="214" t="s">
-        <v>422</v>
+      <c r="E41" s="215" t="s">
+        <v>426</v>
+      </c>
+      <c r="F41" s="215" t="s">
+        <v>427</v>
       </c>
       <c r="G41" s="51"/>
-      <c r="H41" s="215"/>
+      <c r="H41" s="216"/>
       <c r="I41" s="51"/>
       <c r="J41" s="51"/>
       <c r="K41" s="51"/>
@@ -9507,7 +9549,7 @@
       <c r="X41" s="51"/>
       <c r="Y41" s="39"/>
       <c r="Z41" s="39"/>
-      <c r="AA41" s="216" t="n">
+      <c r="AA41" s="217" t="n">
         <v>1.1</v>
       </c>
       <c r="AB41" s="12"/>
@@ -9522,14 +9564,14 @@
       <c r="B42" s="29"/>
       <c r="C42" s="12"/>
       <c r="D42" s="165"/>
-      <c r="E42" s="214" t="s">
-        <v>423</v>
-      </c>
-      <c r="F42" s="214" t="s">
-        <v>424</v>
+      <c r="E42" s="215" t="s">
+        <v>428</v>
+      </c>
+      <c r="F42" s="215" t="s">
+        <v>429</v>
       </c>
       <c r="G42" s="51"/>
-      <c r="H42" s="215"/>
+      <c r="H42" s="216"/>
       <c r="I42" s="51"/>
       <c r="J42" s="51"/>
       <c r="K42" s="51"/>
@@ -9563,33 +9605,33 @@
       <c r="B43" s="12"/>
       <c r="C43" s="12"/>
       <c r="D43" s="165"/>
-      <c r="E43" s="214" t="s">
-        <v>425</v>
-      </c>
-      <c r="F43" s="214" t="s">
-        <v>426</v>
-      </c>
-      <c r="G43" s="217"/>
-      <c r="H43" s="218"/>
-      <c r="I43" s="217"/>
-      <c r="J43" s="217"/>
-      <c r="K43" s="217"/>
-      <c r="L43" s="217"/>
-      <c r="M43" s="217"/>
-      <c r="N43" s="217"/>
-      <c r="O43" s="217"/>
-      <c r="P43" s="217"/>
-      <c r="Q43" s="217"/>
-      <c r="R43" s="217"/>
-      <c r="S43" s="217"/>
-      <c r="T43" s="217"/>
-      <c r="U43" s="217"/>
-      <c r="V43" s="217"/>
-      <c r="W43" s="217"/>
-      <c r="X43" s="217"/>
+      <c r="E43" s="215" t="s">
+        <v>430</v>
+      </c>
+      <c r="F43" s="215" t="s">
+        <v>431</v>
+      </c>
+      <c r="G43" s="218"/>
+      <c r="H43" s="219"/>
+      <c r="I43" s="218"/>
+      <c r="J43" s="218"/>
+      <c r="K43" s="218"/>
+      <c r="L43" s="218"/>
+      <c r="M43" s="218"/>
+      <c r="N43" s="218"/>
+      <c r="O43" s="218"/>
+      <c r="P43" s="218"/>
+      <c r="Q43" s="218"/>
+      <c r="R43" s="218"/>
+      <c r="S43" s="218"/>
+      <c r="T43" s="218"/>
+      <c r="U43" s="218"/>
+      <c r="V43" s="218"/>
+      <c r="W43" s="218"/>
+      <c r="X43" s="218"/>
       <c r="Y43" s="39"/>
       <c r="Z43" s="39"/>
-      <c r="AA43" s="216" t="n">
+      <c r="AA43" s="217" t="n">
         <v>1.5</v>
       </c>
       <c r="AB43" s="12"/>
@@ -9604,11 +9646,11 @@
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="165"/>
-      <c r="E44" s="214" t="s">
-        <v>427</v>
-      </c>
-      <c r="F44" s="214" t="s">
-        <v>428</v>
+      <c r="E44" s="215" t="s">
+        <v>432</v>
+      </c>
+      <c r="F44" s="215" t="s">
+        <v>433</v>
       </c>
       <c r="G44" s="185"/>
       <c r="H44" s="149"/>
@@ -9645,11 +9687,11 @@
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="165"/>
-      <c r="E45" s="214" t="s">
-        <v>429</v>
-      </c>
-      <c r="F45" s="214" t="s">
-        <v>430</v>
+      <c r="E45" s="215" t="s">
+        <v>434</v>
+      </c>
+      <c r="F45" s="215" t="s">
+        <v>435</v>
       </c>
       <c r="G45" s="185"/>
       <c r="H45" s="149"/>
@@ -9671,7 +9713,7 @@
       <c r="X45" s="185"/>
       <c r="Y45" s="39"/>
       <c r="Z45" s="39"/>
-      <c r="AA45" s="216" t="n">
+      <c r="AA45" s="217" t="n">
         <v>1.2</v>
       </c>
       <c r="AB45" s="12"/>
@@ -9686,11 +9728,11 @@
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="165"/>
-      <c r="E46" s="214" t="s">
-        <v>431</v>
-      </c>
-      <c r="F46" s="214" t="s">
-        <v>432</v>
+      <c r="E46" s="215" t="s">
+        <v>436</v>
+      </c>
+      <c r="F46" s="215" t="s">
+        <v>437</v>
       </c>
       <c r="G46" s="185"/>
       <c r="H46" s="149"/>
@@ -9727,11 +9769,11 @@
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="165"/>
-      <c r="E47" s="214" t="s">
-        <v>433</v>
-      </c>
-      <c r="F47" s="214" t="s">
-        <v>434</v>
+      <c r="E47" s="215" t="s">
+        <v>438</v>
+      </c>
+      <c r="F47" s="215" t="s">
+        <v>439</v>
       </c>
       <c r="G47" s="185"/>
       <c r="H47" s="149"/>
@@ -9768,11 +9810,11 @@
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="165"/>
-      <c r="E48" s="214" t="s">
-        <v>435</v>
-      </c>
-      <c r="F48" s="214" t="s">
-        <v>436</v>
+      <c r="E48" s="215" t="s">
+        <v>440</v>
+      </c>
+      <c r="F48" s="215" t="s">
+        <v>441</v>
       </c>
       <c r="G48" s="185"/>
       <c r="H48" s="149"/>
@@ -9794,7 +9836,7 @@
       <c r="X48" s="185"/>
       <c r="Y48" s="39"/>
       <c r="Z48" s="39"/>
-      <c r="AA48" s="216" t="n">
+      <c r="AA48" s="217" t="n">
         <v>4</v>
       </c>
       <c r="AB48" s="12"/>
@@ -9809,11 +9851,11 @@
       <c r="B49" s="12"/>
       <c r="C49" s="12"/>
       <c r="D49" s="165"/>
-      <c r="E49" s="214" t="s">
-        <v>437</v>
-      </c>
-      <c r="F49" s="214" t="s">
-        <v>438</v>
+      <c r="E49" s="215" t="s">
+        <v>442</v>
+      </c>
+      <c r="F49" s="215" t="s">
+        <v>443</v>
       </c>
       <c r="G49" s="185"/>
       <c r="H49" s="149"/>
@@ -9846,41 +9888,41 @@
       <c r="AG49" s="12"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="219"/>
-      <c r="B50" s="219"/>
+      <c r="A50" s="220"/>
+      <c r="B50" s="220"/>
       <c r="C50" s="12"/>
       <c r="D50" s="165"/>
-      <c r="E50" s="214" t="s">
-        <v>439</v>
-      </c>
-      <c r="F50" s="214" t="s">
-        <v>440</v>
-      </c>
-      <c r="G50" s="220" t="s">
-        <v>441</v>
-      </c>
-      <c r="H50" s="221"/>
-      <c r="I50" s="222"/>
-      <c r="J50" s="222"/>
-      <c r="K50" s="222"/>
-      <c r="L50" s="222"/>
-      <c r="M50" s="222" t="n">
-        <v>1</v>
-      </c>
-      <c r="N50" s="222"/>
-      <c r="O50" s="222"/>
-      <c r="P50" s="222"/>
-      <c r="Q50" s="222"/>
-      <c r="R50" s="222"/>
-      <c r="S50" s="222"/>
-      <c r="T50" s="222"/>
-      <c r="U50" s="222"/>
-      <c r="V50" s="222"/>
-      <c r="W50" s="222"/>
-      <c r="X50" s="222"/>
+      <c r="E50" s="215" t="s">
+        <v>444</v>
+      </c>
+      <c r="F50" s="215" t="s">
+        <v>445</v>
+      </c>
+      <c r="G50" s="221" t="s">
+        <v>446</v>
+      </c>
+      <c r="H50" s="222"/>
+      <c r="I50" s="223"/>
+      <c r="J50" s="223"/>
+      <c r="K50" s="223"/>
+      <c r="L50" s="223"/>
+      <c r="M50" s="223" t="n">
+        <v>1</v>
+      </c>
+      <c r="N50" s="223"/>
+      <c r="O50" s="223"/>
+      <c r="P50" s="223"/>
+      <c r="Q50" s="223"/>
+      <c r="R50" s="223"/>
+      <c r="S50" s="223"/>
+      <c r="T50" s="223"/>
+      <c r="U50" s="223"/>
+      <c r="V50" s="223"/>
+      <c r="W50" s="223"/>
+      <c r="X50" s="223"/>
       <c r="Y50" s="39"/>
       <c r="Z50" s="39"/>
-      <c r="AA50" s="216" t="n">
+      <c r="AA50" s="217" t="n">
         <v>6</v>
       </c>
       <c r="AB50" s="12"/>
@@ -9913,7 +9955,7 @@
       <selection pane="topLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="41.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="19.42"/>
@@ -9933,62 +9975,62 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="5.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="10.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="223" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="224" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="223" width="9.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="224" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="11.3"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="186" t="s">
+      <c r="A1" s="187" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="187"/>
+      <c r="B1" s="188"/>
       <c r="E1" s="165"/>
       <c r="F1" s="97"/>
-      <c r="G1" s="224"/>
-      <c r="H1" s="224"/>
-      <c r="I1" s="224"/>
-      <c r="J1" s="224"/>
-      <c r="K1" s="224"/>
-      <c r="L1" s="224"/>
-      <c r="M1" s="224"/>
-      <c r="N1" s="224"/>
-      <c r="O1" s="224"/>
-      <c r="P1" s="224"/>
-      <c r="Q1" s="224"/>
-      <c r="R1" s="224"/>
-      <c r="S1" s="224"/>
-      <c r="T1" s="224"/>
-      <c r="U1" s="224"/>
-      <c r="V1" s="224"/>
-      <c r="W1" s="224"/>
-      <c r="X1" s="224"/>
-      <c r="Y1" s="224"/>
-      <c r="Z1" s="224"/>
-      <c r="AA1" s="225"/>
-      <c r="AB1" s="224"/>
-      <c r="AC1" s="224"/>
-      <c r="AD1" s="225"/>
+      <c r="G1" s="225"/>
+      <c r="H1" s="225"/>
+      <c r="I1" s="225"/>
+      <c r="J1" s="225"/>
+      <c r="K1" s="225"/>
+      <c r="L1" s="225"/>
+      <c r="M1" s="225"/>
+      <c r="N1" s="225"/>
+      <c r="O1" s="225"/>
+      <c r="P1" s="225"/>
+      <c r="Q1" s="225"/>
+      <c r="R1" s="225"/>
+      <c r="S1" s="225"/>
+      <c r="T1" s="225"/>
+      <c r="U1" s="225"/>
+      <c r="V1" s="225"/>
+      <c r="W1" s="225"/>
+      <c r="X1" s="225"/>
+      <c r="Y1" s="225"/>
+      <c r="Z1" s="225"/>
+      <c r="AA1" s="226"/>
+      <c r="AB1" s="225"/>
+      <c r="AC1" s="225"/>
+      <c r="AD1" s="226"/>
       <c r="AE1" s="97"/>
       <c r="AF1" s="97"/>
       <c r="AG1" s="97"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="226" t="s">
+      <c r="A2" s="227" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="227" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="228"/>
-      <c r="E2" s="229" t="s">
+      <c r="C2" s="228" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="229"/>
+      <c r="E2" s="230" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="230"/>
+      <c r="F2" s="231"/>
       <c r="G2" s="97"/>
       <c r="H2" s="97"/>
       <c r="I2" s="97"/>
@@ -10009,22 +10051,22 @@
       <c r="X2" s="97"/>
       <c r="Y2" s="97"/>
       <c r="Z2" s="93"/>
-      <c r="AA2" s="231"/>
+      <c r="AA2" s="232"/>
       <c r="AB2" s="93"/>
       <c r="AC2" s="93"/>
-      <c r="AD2" s="231"/>
+      <c r="AD2" s="232"/>
       <c r="AE2" s="97"/>
       <c r="AF2" s="97"/>
       <c r="AG2" s="97"/>
     </row>
     <row r="3" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="112" t="s">
-        <v>442</v>
+        <v>447</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>443</v>
-      </c>
-      <c r="C3" s="227" t="s">
+        <v>448</v>
+      </c>
+      <c r="C3" s="228" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="5" t="s">
@@ -10040,7 +10082,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="85" t="s">
-        <v>444</v>
+        <v>449</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -10066,7 +10108,7 @@
       <c r="Z3" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="AA3" s="232" t="s">
+      <c r="AA3" s="233" t="s">
         <v>12</v>
       </c>
       <c r="AB3" s="46" t="s">
@@ -10075,17 +10117,17 @@
       <c r="AC3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="232" t="s">
+      <c r="AD3" s="233" t="s">
         <v>15</v>
       </c>
       <c r="AE3" s="46" t="s">
-        <v>445</v>
+        <v>450</v>
       </c>
       <c r="AF3" s="46" t="s">
-        <v>446</v>
-      </c>
-      <c r="AG3" s="232" t="s">
-        <v>447</v>
+        <v>451</v>
+      </c>
+      <c r="AG3" s="233" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10093,11 +10135,11 @@
         <v>16</v>
       </c>
       <c r="B4" s="23"/>
-      <c r="C4" s="192" t="s">
-        <v>448</v>
-      </c>
-      <c r="D4" s="192" t="s">
-        <v>449</v>
+      <c r="C4" s="193" t="s">
+        <v>453</v>
+      </c>
+      <c r="D4" s="193" t="s">
+        <v>454</v>
       </c>
       <c r="H4" s="121" t="s">
         <v>19</v>
@@ -10155,14 +10197,14 @@
       <c r="A5" s="23"/>
       <c r="B5" s="105"/>
       <c r="C5" s="12"/>
-      <c r="E5" s="233" t="s">
-        <v>450</v>
-      </c>
-      <c r="F5" s="233" t="s">
-        <v>451</v>
-      </c>
-      <c r="G5" s="234"/>
-      <c r="H5" s="204"/>
+      <c r="E5" s="234" t="s">
+        <v>455</v>
+      </c>
+      <c r="F5" s="234" t="s">
+        <v>456</v>
+      </c>
+      <c r="G5" s="235"/>
+      <c r="H5" s="205"/>
       <c r="I5" s="33"/>
       <c r="J5" s="33"/>
       <c r="K5" s="33"/>
@@ -10174,25 +10216,25 @@
       <c r="Q5" s="33"/>
       <c r="R5" s="33"/>
       <c r="S5" s="33"/>
-      <c r="T5" s="235" t="n">
+      <c r="T5" s="236" t="n">
         <v>1</v>
       </c>
       <c r="U5" s="33"/>
       <c r="V5" s="33"/>
       <c r="W5" s="33"/>
       <c r="X5" s="33"/>
-      <c r="Y5" s="205"/>
+      <c r="Y5" s="206"/>
       <c r="Z5" s="87" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="AA5" s="81" t="n">
         <v>5</v>
       </c>
-      <c r="AB5" s="205"/>
+      <c r="AB5" s="206"/>
       <c r="AC5" s="87" t="s">
-        <v>453</v>
-      </c>
-      <c r="AD5" s="236" t="n">
+        <v>458</v>
+      </c>
+      <c r="AD5" s="237" t="n">
         <v>15</v>
       </c>
       <c r="AE5" s="12"/>
@@ -10204,14 +10246,14 @@
       <c r="B6" s="23"/>
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
-      <c r="E6" s="237" t="s">
-        <v>454</v>
-      </c>
-      <c r="F6" s="237" t="s">
-        <v>455</v>
+      <c r="E6" s="238" t="s">
+        <v>459</v>
+      </c>
+      <c r="F6" s="238" t="s">
+        <v>460</v>
       </c>
       <c r="G6" s="71"/>
-      <c r="H6" s="204"/>
+      <c r="H6" s="205"/>
       <c r="I6" s="33"/>
       <c r="J6" s="33"/>
       <c r="K6" s="33"/>
@@ -10223,7 +10265,7 @@
       <c r="Q6" s="33"/>
       <c r="R6" s="33"/>
       <c r="S6" s="33"/>
-      <c r="T6" s="235" t="n">
+      <c r="T6" s="236" t="n">
         <v>1</v>
       </c>
       <c r="U6" s="33"/>
@@ -10232,16 +10274,16 @@
       <c r="X6" s="33"/>
       <c r="Y6" s="23"/>
       <c r="Z6" s="87" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="AA6" s="81" t="n">
         <v>4</v>
       </c>
       <c r="AB6" s="23"/>
       <c r="AC6" s="87" t="s">
-        <v>453</v>
-      </c>
-      <c r="AD6" s="236" t="n">
+        <v>458</v>
+      </c>
+      <c r="AD6" s="237" t="n">
         <v>12</v>
       </c>
       <c r="AE6" s="12"/>
@@ -10254,13 +10296,13 @@
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
       <c r="E7" s="60" t="s">
-        <v>456</v>
+        <v>461</v>
       </c>
       <c r="F7" s="60" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="G7" s="51"/>
-      <c r="H7" s="204"/>
+      <c r="H7" s="205"/>
       <c r="I7" s="33"/>
       <c r="J7" s="33"/>
       <c r="K7" s="33"/>
@@ -10272,7 +10314,7 @@
       <c r="Q7" s="33"/>
       <c r="R7" s="33"/>
       <c r="S7" s="33"/>
-      <c r="T7" s="235" t="n">
+      <c r="T7" s="236" t="n">
         <v>1</v>
       </c>
       <c r="U7" s="33"/>
@@ -10281,16 +10323,16 @@
       <c r="X7" s="33"/>
       <c r="Y7" s="23"/>
       <c r="Z7" s="87" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="AA7" s="81" t="n">
         <v>4</v>
       </c>
       <c r="AB7" s="23"/>
       <c r="AC7" s="87" t="s">
-        <v>453</v>
-      </c>
-      <c r="AD7" s="236" t="n">
+        <v>458</v>
+      </c>
+      <c r="AD7" s="237" t="n">
         <v>12</v>
       </c>
       <c r="AE7" s="12"/>
@@ -10302,14 +10344,14 @@
       <c r="B8" s="23"/>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
-      <c r="E8" s="237" t="s">
-        <v>458</v>
-      </c>
-      <c r="F8" s="237" t="s">
-        <v>459</v>
+      <c r="E8" s="238" t="s">
+        <v>463</v>
+      </c>
+      <c r="F8" s="238" t="s">
+        <v>464</v>
       </c>
       <c r="G8" s="51"/>
-      <c r="H8" s="204"/>
+      <c r="H8" s="205"/>
       <c r="I8" s="33"/>
       <c r="J8" s="33"/>
       <c r="K8" s="33"/>
@@ -10321,7 +10363,7 @@
       <c r="Q8" s="33"/>
       <c r="R8" s="33"/>
       <c r="S8" s="33"/>
-      <c r="T8" s="235" t="n">
+      <c r="T8" s="236" t="n">
         <v>1</v>
       </c>
       <c r="U8" s="33"/>
@@ -10330,16 +10372,16 @@
       <c r="X8" s="33"/>
       <c r="Y8" s="23"/>
       <c r="Z8" s="87" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="AA8" s="81" t="n">
         <v>4</v>
       </c>
       <c r="AB8" s="23"/>
       <c r="AC8" s="87" t="s">
-        <v>453</v>
-      </c>
-      <c r="AD8" s="236" t="n">
+        <v>458</v>
+      </c>
+      <c r="AD8" s="237" t="n">
         <v>12</v>
       </c>
       <c r="AE8" s="12"/>
@@ -10351,14 +10393,14 @@
       <c r="B9" s="23"/>
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
-      <c r="E9" s="237" t="s">
-        <v>460</v>
-      </c>
-      <c r="F9" s="237" t="s">
-        <v>461</v>
+      <c r="E9" s="238" t="s">
+        <v>465</v>
+      </c>
+      <c r="F9" s="238" t="s">
+        <v>466</v>
       </c>
       <c r="G9" s="71"/>
-      <c r="H9" s="204"/>
+      <c r="H9" s="205"/>
       <c r="I9" s="33"/>
       <c r="J9" s="33"/>
       <c r="K9" s="33"/>
@@ -10370,7 +10412,7 @@
       <c r="Q9" s="33"/>
       <c r="R9" s="33"/>
       <c r="S9" s="33"/>
-      <c r="T9" s="235" t="n">
+      <c r="T9" s="236" t="n">
         <v>1</v>
       </c>
       <c r="U9" s="33"/>
@@ -10379,16 +10421,16 @@
       <c r="X9" s="33"/>
       <c r="Y9" s="23"/>
       <c r="Z9" s="87" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="AA9" s="81" t="n">
         <v>4.5</v>
       </c>
       <c r="AB9" s="23"/>
       <c r="AC9" s="87" t="s">
-        <v>453</v>
-      </c>
-      <c r="AD9" s="236" t="n">
+        <v>458</v>
+      </c>
+      <c r="AD9" s="237" t="n">
         <v>14</v>
       </c>
       <c r="AE9" s="12"/>
@@ -10398,13 +10440,13 @@
     <row r="10" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
-      <c r="C10" s="192" t="s">
-        <v>462</v>
-      </c>
-      <c r="D10" s="193" t="s">
-        <v>463</v>
-      </c>
-      <c r="H10" s="204"/>
+      <c r="C10" s="193" t="s">
+        <v>467</v>
+      </c>
+      <c r="D10" s="194" t="s">
+        <v>468</v>
+      </c>
+      <c r="H10" s="205"/>
       <c r="I10" s="33"/>
       <c r="J10" s="33"/>
       <c r="K10" s="33"/>
@@ -10421,7 +10463,7 @@
       <c r="V10" s="33"/>
       <c r="W10" s="33"/>
       <c r="X10" s="33"/>
-      <c r="AA10" s="238"/>
+      <c r="AA10" s="239"/>
       <c r="AE10" s="12"/>
       <c r="AF10" s="12"/>
       <c r="AG10" s="12"/>
@@ -10429,16 +10471,16 @@
     <row r="11" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
-      <c r="C11" s="192"/>
-      <c r="D11" s="192"/>
+      <c r="C11" s="193"/>
+      <c r="D11" s="193"/>
       <c r="E11" s="60" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="F11" s="60" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="G11" s="51"/>
-      <c r="H11" s="204"/>
+      <c r="H11" s="205"/>
       <c r="I11" s="33"/>
       <c r="J11" s="33"/>
       <c r="K11" s="33"/>
@@ -10457,14 +10499,14 @@
       <c r="X11" s="33"/>
       <c r="Y11" s="23"/>
       <c r="Z11" s="87" t="s">
-        <v>452</v>
+        <v>457</v>
       </c>
       <c r="AA11" s="81" t="n">
         <v>4</v>
       </c>
       <c r="AB11" s="23"/>
       <c r="AC11" s="87"/>
-      <c r="AD11" s="239"/>
+      <c r="AD11" s="240"/>
       <c r="AE11" s="12"/>
       <c r="AF11" s="12"/>
       <c r="AG11" s="12"/>
@@ -10474,16 +10516,16 @@
       <c r="B12" s="23"/>
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
-      <c r="E12" s="237" t="s">
-        <v>466</v>
-      </c>
-      <c r="F12" s="237" t="s">
-        <v>467</v>
+      <c r="E12" s="238" t="s">
+        <v>471</v>
+      </c>
+      <c r="F12" s="238" t="s">
+        <v>472</v>
       </c>
       <c r="G12" s="71" t="s">
-        <v>468</v>
-      </c>
-      <c r="H12" s="204"/>
+        <v>473</v>
+      </c>
+      <c r="H12" s="205"/>
       <c r="I12" s="33"/>
       <c r="J12" s="33"/>
       <c r="K12" s="33"/>
@@ -10501,15 +10543,15 @@
       <c r="W12" s="33"/>
       <c r="X12" s="33"/>
       <c r="Y12" s="23"/>
-      <c r="Z12" s="240" t="s">
-        <v>469</v>
+      <c r="Z12" s="241" t="s">
+        <v>474</v>
       </c>
       <c r="AA12" s="81" t="n">
         <v>5</v>
       </c>
       <c r="AB12" s="23"/>
       <c r="AC12" s="87"/>
-      <c r="AD12" s="239"/>
+      <c r="AD12" s="240"/>
       <c r="AE12" s="12"/>
       <c r="AF12" s="12"/>
       <c r="AG12" s="12"/>
@@ -10520,15 +10562,15 @@
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
       <c r="E13" s="60" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="F13" s="60" t="s">
-        <v>471</v>
+        <v>476</v>
       </c>
       <c r="G13" s="51" t="s">
-        <v>468</v>
-      </c>
-      <c r="H13" s="204"/>
+        <v>473</v>
+      </c>
+      <c r="H13" s="205"/>
       <c r="I13" s="33"/>
       <c r="J13" s="33"/>
       <c r="K13" s="33"/>
@@ -10546,15 +10588,15 @@
       <c r="W13" s="33"/>
       <c r="X13" s="33"/>
       <c r="Y13" s="23"/>
-      <c r="Z13" s="240" t="s">
-        <v>469</v>
+      <c r="Z13" s="241" t="s">
+        <v>474</v>
       </c>
       <c r="AA13" s="81" t="n">
         <v>5</v>
       </c>
       <c r="AB13" s="23"/>
       <c r="AC13" s="87"/>
-      <c r="AD13" s="239"/>
+      <c r="AD13" s="240"/>
       <c r="AE13" s="12"/>
       <c r="AF13" s="12"/>
       <c r="AG13" s="12"/>
@@ -10562,16 +10604,16 @@
     <row r="14" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
-      <c r="C14" s="192" t="s">
-        <v>472</v>
-      </c>
-      <c r="D14" s="192" t="s">
-        <v>473</v>
+      <c r="C14" s="193" t="s">
+        <v>477</v>
+      </c>
+      <c r="D14" s="193" t="s">
+        <v>478</v>
       </c>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
       <c r="G14" s="51"/>
-      <c r="H14" s="197"/>
+      <c r="H14" s="198"/>
       <c r="I14" s="12"/>
       <c r="J14" s="12"/>
       <c r="K14" s="12"/>
@@ -10589,28 +10631,28 @@
       <c r="W14" s="12"/>
       <c r="X14" s="12"/>
       <c r="Y14" s="23"/>
-      <c r="Z14" s="240"/>
-      <c r="AA14" s="241"/>
+      <c r="Z14" s="241"/>
+      <c r="AA14" s="242"/>
       <c r="AB14" s="23"/>
       <c r="AC14" s="87"/>
-      <c r="AD14" s="239"/>
+      <c r="AD14" s="240"/>
       <c r="AE14" s="12"/>
       <c r="AF14" s="12"/>
       <c r="AG14" s="12"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29"/>
-      <c r="B15" s="242"/>
-      <c r="E15" s="237" t="s">
-        <v>474</v>
-      </c>
-      <c r="F15" s="237" t="s">
-        <v>475</v>
+      <c r="B15" s="243"/>
+      <c r="E15" s="238" t="s">
+        <v>479</v>
+      </c>
+      <c r="F15" s="238" t="s">
+        <v>480</v>
       </c>
       <c r="G15" s="71" t="s">
-        <v>476</v>
-      </c>
-      <c r="H15" s="215"/>
+        <v>481</v>
+      </c>
+      <c r="H15" s="216"/>
       <c r="I15" s="51"/>
       <c r="J15" s="51"/>
       <c r="K15" s="51"/>
@@ -10629,16 +10671,16 @@
       <c r="X15" s="51"/>
       <c r="Y15" s="38"/>
       <c r="Z15" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA15" s="40" t="n">
         <v>3</v>
       </c>
-      <c r="AB15" s="243"/>
-      <c r="AC15" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD15" s="244" t="n">
+      <c r="AB15" s="244"/>
+      <c r="AC15" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD15" s="245" t="n">
         <v>5</v>
       </c>
       <c r="AE15" s="12"/>
@@ -10650,16 +10692,16 @@
       <c r="B16" s="29"/>
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
-      <c r="E16" s="237" t="s">
-        <v>478</v>
-      </c>
-      <c r="F16" s="237" t="s">
-        <v>479</v>
+      <c r="E16" s="238" t="s">
+        <v>483</v>
+      </c>
+      <c r="F16" s="238" t="s">
+        <v>484</v>
       </c>
       <c r="G16" s="71" t="s">
-        <v>480</v>
-      </c>
-      <c r="H16" s="215"/>
+        <v>485</v>
+      </c>
+      <c r="H16" s="216"/>
       <c r="I16" s="51"/>
       <c r="J16" s="51"/>
       <c r="K16" s="51"/>
@@ -10678,16 +10720,16 @@
       <c r="X16" s="51"/>
       <c r="Y16" s="38"/>
       <c r="Z16" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA16" s="40" t="n">
         <v>3.5</v>
       </c>
-      <c r="AB16" s="243"/>
-      <c r="AC16" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD16" s="244" t="n">
+      <c r="AB16" s="244"/>
+      <c r="AC16" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD16" s="245" t="n">
         <v>6</v>
       </c>
       <c r="AE16" s="12"/>
@@ -10700,43 +10742,43 @@
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
       <c r="E17" s="60" t="s">
-        <v>481</v>
+        <v>486</v>
       </c>
       <c r="F17" s="60" t="s">
-        <v>482</v>
+        <v>487</v>
       </c>
       <c r="G17" s="68" t="s">
-        <v>483</v>
-      </c>
-      <c r="H17" s="218"/>
-      <c r="I17" s="217"/>
-      <c r="J17" s="217"/>
-      <c r="K17" s="217"/>
-      <c r="L17" s="217"/>
-      <c r="M17" s="217"/>
-      <c r="N17" s="217"/>
-      <c r="O17" s="217"/>
-      <c r="P17" s="217"/>
-      <c r="Q17" s="217"/>
-      <c r="R17" s="217"/>
-      <c r="S17" s="217"/>
-      <c r="T17" s="217"/>
-      <c r="U17" s="217"/>
-      <c r="V17" s="217"/>
-      <c r="W17" s="217"/>
-      <c r="X17" s="217"/>
+        <v>488</v>
+      </c>
+      <c r="H17" s="219"/>
+      <c r="I17" s="218"/>
+      <c r="J17" s="218"/>
+      <c r="K17" s="218"/>
+      <c r="L17" s="218"/>
+      <c r="M17" s="218"/>
+      <c r="N17" s="218"/>
+      <c r="O17" s="218"/>
+      <c r="P17" s="218"/>
+      <c r="Q17" s="218"/>
+      <c r="R17" s="218"/>
+      <c r="S17" s="218"/>
+      <c r="T17" s="218"/>
+      <c r="U17" s="218"/>
+      <c r="V17" s="218"/>
+      <c r="W17" s="218"/>
+      <c r="X17" s="218"/>
       <c r="Y17" s="38"/>
       <c r="Z17" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA17" s="79" t="n">
         <v>4</v>
       </c>
       <c r="AB17" s="38"/>
-      <c r="AC17" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD17" s="244" t="n">
+      <c r="AC17" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD17" s="245" t="n">
         <v>7</v>
       </c>
       <c r="AE17" s="12"/>
@@ -10748,14 +10790,14 @@
       <c r="B18" s="29"/>
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
-      <c r="E18" s="245" t="s">
-        <v>484</v>
-      </c>
-      <c r="F18" s="245" t="s">
-        <v>485</v>
-      </c>
-      <c r="G18" s="246" t="s">
-        <v>486</v>
+      <c r="E18" s="246" t="s">
+        <v>489</v>
+      </c>
+      <c r="F18" s="246" t="s">
+        <v>490</v>
+      </c>
+      <c r="G18" s="247" t="s">
+        <v>491</v>
       </c>
       <c r="H18" s="149"/>
       <c r="I18" s="185"/>
@@ -10776,16 +10818,16 @@
       <c r="X18" s="185"/>
       <c r="Y18" s="38"/>
       <c r="Z18" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA18" s="79" t="n">
         <v>4.5</v>
       </c>
       <c r="AB18" s="80"/>
-      <c r="AC18" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD18" s="247" t="n">
+      <c r="AC18" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD18" s="248" t="n">
         <v>8</v>
       </c>
       <c r="AE18" s="12"/>
@@ -10798,13 +10840,13 @@
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="60" t="s">
-        <v>487</v>
+        <v>492</v>
       </c>
       <c r="F19" s="60" t="s">
-        <v>488</v>
+        <v>493</v>
       </c>
       <c r="G19" s="68" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="H19" s="149"/>
       <c r="I19" s="185"/>
@@ -10825,16 +10867,16 @@
       <c r="X19" s="185"/>
       <c r="Y19" s="38"/>
       <c r="Z19" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA19" s="79" t="n">
         <v>3</v>
       </c>
       <c r="AB19" s="82"/>
-      <c r="AC19" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD19" s="247" t="n">
+      <c r="AC19" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD19" s="248" t="n">
         <v>5</v>
       </c>
       <c r="AE19" s="12"/>
@@ -10846,14 +10888,14 @@
       <c r="B20" s="29"/>
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
-      <c r="E20" s="245" t="s">
-        <v>490</v>
-      </c>
-      <c r="F20" s="245" t="s">
-        <v>491</v>
+      <c r="E20" s="246" t="s">
+        <v>495</v>
+      </c>
+      <c r="F20" s="246" t="s">
+        <v>496</v>
       </c>
       <c r="G20" s="68" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="H20" s="149"/>
       <c r="I20" s="185"/>
@@ -10874,16 +10916,16 @@
       <c r="X20" s="185"/>
       <c r="Y20" s="38"/>
       <c r="Z20" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA20" s="79" t="n">
         <v>4</v>
       </c>
       <c r="AB20" s="41"/>
-      <c r="AC20" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD20" s="244" t="n">
+      <c r="AC20" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD20" s="245" t="n">
         <v>7</v>
       </c>
       <c r="AE20" s="12"/>
@@ -10896,13 +10938,13 @@
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
       <c r="E21" s="60" t="s">
-        <v>492</v>
+        <v>497</v>
       </c>
       <c r="F21" s="60" t="s">
-        <v>493</v>
+        <v>498</v>
       </c>
       <c r="G21" s="68" t="s">
-        <v>489</v>
+        <v>494</v>
       </c>
       <c r="H21" s="149"/>
       <c r="I21" s="185"/>
@@ -10923,16 +10965,16 @@
       <c r="X21" s="185"/>
       <c r="Y21" s="38"/>
       <c r="Z21" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA21" s="79" t="n">
         <v>4</v>
       </c>
       <c r="AB21" s="41"/>
-      <c r="AC21" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD21" s="244" t="n">
+      <c r="AC21" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD21" s="245" t="n">
         <v>7</v>
       </c>
       <c r="AE21" s="12"/>
@@ -10945,13 +10987,13 @@
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="60" t="s">
+        <v>499</v>
+      </c>
+      <c r="F22" s="60" t="s">
+        <v>500</v>
+      </c>
+      <c r="G22" s="51" t="s">
         <v>494</v>
-      </c>
-      <c r="F22" s="60" t="s">
-        <v>495</v>
-      </c>
-      <c r="G22" s="51" t="s">
-        <v>489</v>
       </c>
       <c r="H22" s="149"/>
       <c r="I22" s="185"/>
@@ -10972,16 +11014,16 @@
       <c r="X22" s="185"/>
       <c r="Y22" s="38"/>
       <c r="Z22" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA22" s="79" t="n">
         <v>5</v>
       </c>
       <c r="AB22" s="80"/>
-      <c r="AC22" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD22" s="236" t="n">
+      <c r="AC22" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD22" s="237" t="n">
         <v>8</v>
       </c>
       <c r="AE22" s="12"/>
@@ -10991,46 +11033,46 @@
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="73"/>
       <c r="B23" s="73"/>
-      <c r="C23" s="248"/>
-      <c r="D23" s="248"/>
-      <c r="E23" s="205" t="s">
-        <v>496</v>
-      </c>
-      <c r="F23" s="205" t="s">
-        <v>497</v>
+      <c r="C23" s="249"/>
+      <c r="D23" s="249"/>
+      <c r="E23" s="206" t="s">
+        <v>501</v>
+      </c>
+      <c r="F23" s="206" t="s">
+        <v>502</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>489</v>
-      </c>
-      <c r="H23" s="221"/>
-      <c r="I23" s="222"/>
-      <c r="J23" s="222"/>
-      <c r="K23" s="222"/>
-      <c r="L23" s="222"/>
-      <c r="M23" s="222"/>
-      <c r="N23" s="222"/>
-      <c r="O23" s="222"/>
-      <c r="P23" s="222"/>
-      <c r="Q23" s="222"/>
-      <c r="R23" s="222"/>
-      <c r="S23" s="222"/>
-      <c r="T23" s="222"/>
-      <c r="U23" s="222"/>
-      <c r="V23" s="222"/>
-      <c r="W23" s="222"/>
-      <c r="X23" s="222"/>
+        <v>494</v>
+      </c>
+      <c r="H23" s="222"/>
+      <c r="I23" s="223"/>
+      <c r="J23" s="223"/>
+      <c r="K23" s="223"/>
+      <c r="L23" s="223"/>
+      <c r="M23" s="223"/>
+      <c r="N23" s="223"/>
+      <c r="O23" s="223"/>
+      <c r="P23" s="223"/>
+      <c r="Q23" s="223"/>
+      <c r="R23" s="223"/>
+      <c r="S23" s="223"/>
+      <c r="T23" s="223"/>
+      <c r="U23" s="223"/>
+      <c r="V23" s="223"/>
+      <c r="W23" s="223"/>
+      <c r="X23" s="223"/>
       <c r="Y23" s="38"/>
       <c r="Z23" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA23" s="79" t="n">
         <v>5</v>
       </c>
       <c r="AB23" s="80"/>
-      <c r="AC23" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD23" s="236" t="n">
+      <c r="AC23" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD23" s="237" t="n">
         <v>8.5</v>
       </c>
       <c r="AE23" s="12"/>
@@ -11043,15 +11085,15 @@
       <c r="C24" s="90"/>
       <c r="D24" s="90"/>
       <c r="E24" s="85" t="s">
-        <v>498</v>
+        <v>503</v>
       </c>
       <c r="F24" s="85" t="s">
-        <v>499</v>
+        <v>504</v>
       </c>
       <c r="G24" s="35" t="s">
-        <v>500</v>
-      </c>
-      <c r="H24" s="197"/>
+        <v>505</v>
+      </c>
+      <c r="H24" s="198"/>
       <c r="I24" s="12"/>
       <c r="J24" s="12"/>
       <c r="K24" s="12"/>
@@ -11070,12 +11112,12 @@
       <c r="X24" s="12"/>
       <c r="Y24" s="38"/>
       <c r="Z24" s="39"/>
-      <c r="AA24" s="249"/>
+      <c r="AA24" s="250"/>
       <c r="AB24" s="35"/>
-      <c r="AC24" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD24" s="247" t="n">
+      <c r="AC24" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD24" s="248" t="n">
         <v>4.5</v>
       </c>
       <c r="AE24" s="12"/>
@@ -11088,15 +11130,15 @@
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="85" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="F25" s="85" t="s">
-        <v>502</v>
+        <v>507</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>503</v>
-      </c>
-      <c r="H25" s="197"/>
+        <v>508</v>
+      </c>
+      <c r="H25" s="198"/>
       <c r="I25" s="12"/>
       <c r="J25" s="12"/>
       <c r="K25" s="12"/>
@@ -11117,10 +11159,10 @@
       <c r="Z25" s="39"/>
       <c r="AA25" s="84"/>
       <c r="AB25" s="12"/>
-      <c r="AC25" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD25" s="247" t="n">
+      <c r="AC25" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD25" s="248" t="n">
         <v>4.5</v>
       </c>
       <c r="AE25" s="12"/>
@@ -11133,15 +11175,15 @@
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="85" t="s">
-        <v>504</v>
+        <v>509</v>
       </c>
       <c r="F26" s="85" t="s">
-        <v>505</v>
+        <v>510</v>
       </c>
       <c r="G26" s="35" t="s">
-        <v>506</v>
-      </c>
-      <c r="H26" s="197"/>
+        <v>511</v>
+      </c>
+      <c r="H26" s="198"/>
       <c r="I26" s="12"/>
       <c r="J26" s="12"/>
       <c r="K26" s="12"/>
@@ -11160,16 +11202,16 @@
       <c r="X26" s="12"/>
       <c r="Y26" s="12"/>
       <c r="Z26" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA26" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AB26" s="12"/>
-      <c r="AC26" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD26" s="250" t="n">
+      <c r="AC26" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD26" s="251" t="n">
         <v>4.5</v>
       </c>
       <c r="AE26" s="12"/>
@@ -11182,15 +11224,15 @@
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="85" t="s">
-        <v>507</v>
+        <v>512</v>
       </c>
       <c r="F27" s="85" t="s">
-        <v>508</v>
+        <v>513</v>
       </c>
       <c r="G27" s="35" t="s">
-        <v>506</v>
-      </c>
-      <c r="H27" s="197"/>
+        <v>511</v>
+      </c>
+      <c r="H27" s="198"/>
       <c r="I27" s="12"/>
       <c r="J27" s="12"/>
       <c r="K27" s="12"/>
@@ -11209,16 +11251,16 @@
       <c r="X27" s="12"/>
       <c r="Y27" s="12"/>
       <c r="Z27" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA27" s="84" t="n">
         <v>4.5</v>
       </c>
       <c r="AB27" s="12"/>
-      <c r="AC27" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD27" s="250" t="n">
+      <c r="AC27" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD27" s="251" t="n">
         <v>7.5</v>
       </c>
       <c r="AE27" s="12"/>
@@ -11231,15 +11273,15 @@
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="85" t="s">
-        <v>509</v>
+        <v>514</v>
       </c>
       <c r="F28" s="85" t="s">
-        <v>510</v>
+        <v>515</v>
       </c>
       <c r="G28" s="35" t="s">
-        <v>511</v>
-      </c>
-      <c r="H28" s="197"/>
+        <v>516</v>
+      </c>
+      <c r="H28" s="198"/>
       <c r="I28" s="12"/>
       <c r="J28" s="12"/>
       <c r="K28" s="12"/>
@@ -11258,16 +11300,16 @@
       <c r="X28" s="12"/>
       <c r="Y28" s="12"/>
       <c r="Z28" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA28" s="84" t="n">
         <v>4.5</v>
       </c>
       <c r="AB28" s="12"/>
-      <c r="AC28" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD28" s="250" t="n">
+      <c r="AC28" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD28" s="251" t="n">
         <v>7.5</v>
       </c>
       <c r="AE28" s="12"/>
@@ -11280,15 +11322,15 @@
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="85" t="s">
-        <v>512</v>
+        <v>517</v>
       </c>
       <c r="F29" s="85" t="s">
-        <v>513</v>
+        <v>518</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>514</v>
-      </c>
-      <c r="H29" s="197"/>
+        <v>519</v>
+      </c>
+      <c r="H29" s="198"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
@@ -11307,16 +11349,16 @@
       <c r="X29" s="12"/>
       <c r="Y29" s="12"/>
       <c r="Z29" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA29" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB29" s="12"/>
-      <c r="AC29" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD29" s="250" t="n">
+      <c r="AC29" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD29" s="251" t="n">
         <v>5</v>
       </c>
       <c r="AE29" s="12"/>
@@ -11329,15 +11371,15 @@
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="85" t="s">
-        <v>515</v>
+        <v>520</v>
       </c>
       <c r="F30" s="85" t="s">
-        <v>516</v>
+        <v>521</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>514</v>
-      </c>
-      <c r="H30" s="197"/>
+        <v>519</v>
+      </c>
+      <c r="H30" s="198"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
@@ -11356,16 +11398,16 @@
       <c r="X30" s="12"/>
       <c r="Y30" s="12"/>
       <c r="Z30" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA30" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB30" s="12"/>
-      <c r="AC30" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD30" s="250" t="n">
+      <c r="AC30" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD30" s="251" t="n">
         <v>5</v>
       </c>
       <c r="AE30" s="12"/>
@@ -11378,15 +11420,15 @@
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="85" t="s">
-        <v>517</v>
+        <v>522</v>
       </c>
       <c r="F31" s="85" t="s">
-        <v>518</v>
+        <v>523</v>
       </c>
       <c r="G31" s="35" t="s">
-        <v>519</v>
-      </c>
-      <c r="H31" s="197"/>
+        <v>524</v>
+      </c>
+      <c r="H31" s="198"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
@@ -11405,16 +11447,16 @@
       <c r="X31" s="12"/>
       <c r="Y31" s="12"/>
       <c r="Z31" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA31" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB31" s="12"/>
-      <c r="AC31" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD31" s="250" t="n">
+      <c r="AC31" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD31" s="251" t="n">
         <v>5</v>
       </c>
       <c r="AE31" s="12"/>
@@ -11427,15 +11469,15 @@
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="85" t="s">
-        <v>520</v>
+        <v>525</v>
       </c>
       <c r="F32" s="85" t="s">
-        <v>521</v>
+        <v>526</v>
       </c>
       <c r="G32" s="35" t="s">
-        <v>519</v>
-      </c>
-      <c r="H32" s="197"/>
+        <v>524</v>
+      </c>
+      <c r="H32" s="198"/>
       <c r="I32" s="12"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
@@ -11454,16 +11496,16 @@
       <c r="X32" s="12"/>
       <c r="Y32" s="12"/>
       <c r="Z32" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA32" s="84" t="n">
         <v>4</v>
       </c>
       <c r="AB32" s="12"/>
-      <c r="AC32" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD32" s="250" t="n">
+      <c r="AC32" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD32" s="251" t="n">
         <v>7</v>
       </c>
       <c r="AE32" s="12"/>
@@ -11476,15 +11518,15 @@
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="85" t="s">
-        <v>522</v>
+        <v>527</v>
       </c>
       <c r="F33" s="85" t="s">
-        <v>523</v>
+        <v>528</v>
       </c>
       <c r="G33" s="35" t="s">
-        <v>519</v>
-      </c>
-      <c r="H33" s="197"/>
+        <v>524</v>
+      </c>
+      <c r="H33" s="198"/>
       <c r="I33" s="12"/>
       <c r="J33" s="12"/>
       <c r="K33" s="12"/>
@@ -11503,16 +11545,16 @@
       <c r="X33" s="12"/>
       <c r="Y33" s="12"/>
       <c r="Z33" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA33" s="84" t="n">
         <v>4.5</v>
       </c>
       <c r="AB33" s="12"/>
-      <c r="AC33" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD33" s="250" t="n">
+      <c r="AC33" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD33" s="251" t="n">
         <v>8</v>
       </c>
       <c r="AE33" s="12"/>
@@ -11525,15 +11567,15 @@
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="85" t="s">
-        <v>524</v>
+        <v>529</v>
       </c>
       <c r="F34" s="85" t="s">
-        <v>525</v>
+        <v>530</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>526</v>
-      </c>
-      <c r="H34" s="197"/>
+        <v>531</v>
+      </c>
+      <c r="H34" s="198"/>
       <c r="I34" s="12"/>
       <c r="J34" s="12"/>
       <c r="K34" s="12"/>
@@ -11552,16 +11594,16 @@
       <c r="X34" s="12"/>
       <c r="Y34" s="12"/>
       <c r="Z34" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA34" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB34" s="12"/>
-      <c r="AC34" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD34" s="250" t="n">
+      <c r="AC34" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD34" s="251" t="n">
         <v>5</v>
       </c>
       <c r="AE34" s="12"/>
@@ -11574,15 +11616,15 @@
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="85" t="s">
-        <v>527</v>
+        <v>532</v>
       </c>
       <c r="F35" s="85" t="s">
-        <v>528</v>
+        <v>533</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>526</v>
-      </c>
-      <c r="H35" s="197"/>
+        <v>531</v>
+      </c>
+      <c r="H35" s="198"/>
       <c r="I35" s="12"/>
       <c r="J35" s="12"/>
       <c r="K35" s="12"/>
@@ -11601,16 +11643,16 @@
       <c r="X35" s="12"/>
       <c r="Y35" s="12"/>
       <c r="Z35" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA35" s="84" t="n">
         <v>6</v>
       </c>
       <c r="AB35" s="12"/>
-      <c r="AC35" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD35" s="250" t="n">
+      <c r="AC35" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD35" s="251" t="n">
         <v>9.5</v>
       </c>
       <c r="AE35" s="12"/>
@@ -11622,16 +11664,16 @@
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
-      <c r="E36" s="245" t="s">
-        <v>529</v>
+      <c r="E36" s="246" t="s">
+        <v>534</v>
       </c>
       <c r="F36" s="85" t="s">
-        <v>530</v>
+        <v>535</v>
       </c>
       <c r="G36" s="35" t="s">
-        <v>526</v>
-      </c>
-      <c r="H36" s="197"/>
+        <v>531</v>
+      </c>
+      <c r="H36" s="198"/>
       <c r="I36" s="12"/>
       <c r="J36" s="12"/>
       <c r="K36" s="12"/>
@@ -11650,16 +11692,16 @@
       <c r="X36" s="12"/>
       <c r="Y36" s="12"/>
       <c r="Z36" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA36" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB36" s="12"/>
-      <c r="AC36" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD36" s="250" t="n">
+      <c r="AC36" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD36" s="251" t="n">
         <v>5</v>
       </c>
       <c r="AE36" s="12"/>
@@ -11672,15 +11714,15 @@
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="85" t="s">
+        <v>536</v>
+      </c>
+      <c r="F37" s="85" t="s">
+        <v>537</v>
+      </c>
+      <c r="G37" s="35" t="s">
         <v>531</v>
       </c>
-      <c r="F37" s="85" t="s">
-        <v>532</v>
-      </c>
-      <c r="G37" s="35" t="s">
-        <v>526</v>
-      </c>
-      <c r="H37" s="197"/>
+      <c r="H37" s="198"/>
       <c r="I37" s="12"/>
       <c r="J37" s="12"/>
       <c r="K37" s="12"/>
@@ -11699,16 +11741,16 @@
       <c r="X37" s="12"/>
       <c r="Y37" s="12"/>
       <c r="Z37" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA37" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB37" s="12"/>
-      <c r="AC37" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD37" s="250" t="n">
+      <c r="AC37" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD37" s="251" t="n">
         <v>5</v>
       </c>
       <c r="AE37" s="12"/>
@@ -11721,15 +11763,15 @@
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="85" t="s">
-        <v>533</v>
+        <v>538</v>
       </c>
       <c r="F38" s="85" t="s">
-        <v>534</v>
+        <v>539</v>
       </c>
       <c r="G38" s="35" t="s">
-        <v>526</v>
-      </c>
-      <c r="H38" s="197"/>
+        <v>531</v>
+      </c>
+      <c r="H38" s="198"/>
       <c r="I38" s="12"/>
       <c r="J38" s="12"/>
       <c r="K38" s="12"/>
@@ -11748,16 +11790,16 @@
       <c r="X38" s="12"/>
       <c r="Y38" s="12"/>
       <c r="Z38" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA38" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB38" s="12"/>
-      <c r="AC38" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD38" s="250" t="n">
+      <c r="AC38" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD38" s="251" t="n">
         <v>5</v>
       </c>
       <c r="AE38" s="12"/>
@@ -11770,13 +11812,13 @@
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="85" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="F39" s="85" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="G39" s="35"/>
-      <c r="H39" s="197"/>
+      <c r="H39" s="198"/>
       <c r="I39" s="12"/>
       <c r="J39" s="12"/>
       <c r="K39" s="12"/>
@@ -11795,16 +11837,16 @@
       <c r="X39" s="12"/>
       <c r="Y39" s="12"/>
       <c r="Z39" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA39" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB39" s="12"/>
-      <c r="AC39" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD39" s="250" t="n">
+      <c r="AC39" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD39" s="251" t="n">
         <v>4.5</v>
       </c>
       <c r="AE39" s="12"/>
@@ -11817,13 +11859,13 @@
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="85" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="F40" s="85" t="s">
-        <v>538</v>
+        <v>543</v>
       </c>
       <c r="G40" s="35"/>
-      <c r="H40" s="197"/>
+      <c r="H40" s="198"/>
       <c r="I40" s="12"/>
       <c r="J40" s="12"/>
       <c r="K40" s="12"/>
@@ -11842,16 +11884,16 @@
       <c r="X40" s="12"/>
       <c r="Y40" s="12"/>
       <c r="Z40" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA40" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AB40" s="12"/>
-      <c r="AC40" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD40" s="250" t="n">
+      <c r="AC40" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD40" s="251" t="n">
         <v>4</v>
       </c>
       <c r="AE40" s="12"/>
@@ -11864,13 +11906,13 @@
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="85" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="F41" s="85" t="s">
-        <v>540</v>
+        <v>545</v>
       </c>
       <c r="G41" s="35"/>
-      <c r="H41" s="197"/>
+      <c r="H41" s="198"/>
       <c r="I41" s="12"/>
       <c r="J41" s="12"/>
       <c r="K41" s="12"/>
@@ -11889,16 +11931,16 @@
       <c r="X41" s="12"/>
       <c r="Y41" s="12"/>
       <c r="Z41" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA41" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AB41" s="12"/>
-      <c r="AC41" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD41" s="250" t="n">
+      <c r="AC41" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD41" s="251" t="n">
         <v>4</v>
       </c>
       <c r="AE41" s="12"/>
@@ -11911,13 +11953,13 @@
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="85" t="s">
-        <v>541</v>
+        <v>546</v>
       </c>
       <c r="F42" s="85" t="s">
-        <v>542</v>
+        <v>547</v>
       </c>
       <c r="G42" s="35"/>
-      <c r="H42" s="197"/>
+      <c r="H42" s="198"/>
       <c r="I42" s="12"/>
       <c r="J42" s="12"/>
       <c r="K42" s="12"/>
@@ -11936,16 +11978,16 @@
       <c r="X42" s="12"/>
       <c r="Y42" s="12"/>
       <c r="Z42" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA42" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AB42" s="12"/>
-      <c r="AC42" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD42" s="250" t="n">
+      <c r="AC42" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD42" s="251" t="n">
         <v>4</v>
       </c>
       <c r="AE42" s="12"/>
@@ -11955,14 +11997,14 @@
     <row r="43" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
-      <c r="C43" s="192" t="s">
-        <v>543</v>
-      </c>
-      <c r="D43" s="192"/>
+      <c r="C43" s="193" t="s">
+        <v>548</v>
+      </c>
+      <c r="D43" s="193"/>
       <c r="E43" s="85"/>
       <c r="F43" s="85"/>
       <c r="G43" s="35"/>
-      <c r="H43" s="197"/>
+      <c r="H43" s="198"/>
       <c r="I43" s="12"/>
       <c r="J43" s="12"/>
       <c r="K43" s="12"/>
@@ -11983,8 +12025,8 @@
       <c r="Z43" s="39"/>
       <c r="AA43" s="84"/>
       <c r="AB43" s="12"/>
-      <c r="AC43" s="240"/>
-      <c r="AD43" s="250"/>
+      <c r="AC43" s="241"/>
+      <c r="AD43" s="251"/>
       <c r="AE43" s="12"/>
       <c r="AF43" s="12"/>
       <c r="AG43" s="12"/>
@@ -11993,13 +12035,13 @@
       <c r="A44" s="12"/>
       <c r="B44" s="97"/>
       <c r="E44" s="85" t="s">
-        <v>544</v>
+        <v>549</v>
       </c>
       <c r="F44" s="85" t="s">
-        <v>545</v>
+        <v>550</v>
       </c>
       <c r="G44" s="12"/>
-      <c r="H44" s="197"/>
+      <c r="H44" s="198"/>
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
       <c r="K44" s="12"/>
@@ -12018,16 +12060,16 @@
       <c r="X44" s="12"/>
       <c r="Y44" s="12"/>
       <c r="Z44" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA44" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB44" s="12"/>
-      <c r="AC44" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD44" s="250" t="n">
+      <c r="AC44" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD44" s="251" t="n">
         <v>4.5</v>
       </c>
       <c r="AE44" s="12"/>
@@ -12040,13 +12082,13 @@
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="E45" s="85" t="s">
-        <v>546</v>
+        <v>551</v>
       </c>
       <c r="F45" s="85" t="s">
-        <v>547</v>
+        <v>552</v>
       </c>
       <c r="G45" s="12"/>
-      <c r="H45" s="197"/>
+      <c r="H45" s="198"/>
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
       <c r="K45" s="12"/>
@@ -12065,16 +12107,16 @@
       <c r="X45" s="12"/>
       <c r="Y45" s="12"/>
       <c r="Z45" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA45" s="84" t="n">
         <v>3.5</v>
       </c>
       <c r="AB45" s="12"/>
-      <c r="AC45" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD45" s="250" t="n">
+      <c r="AC45" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD45" s="251" t="n">
         <v>6</v>
       </c>
       <c r="AE45" s="12"/>
@@ -12087,13 +12129,13 @@
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="85" t="s">
-        <v>548</v>
+        <v>553</v>
       </c>
       <c r="F46" s="85" t="s">
-        <v>549</v>
+        <v>554</v>
       </c>
       <c r="G46" s="12"/>
-      <c r="H46" s="197"/>
+      <c r="H46" s="198"/>
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
       <c r="K46" s="12"/>
@@ -12112,16 +12154,16 @@
       <c r="X46" s="12"/>
       <c r="Y46" s="12"/>
       <c r="Z46" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA46" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB46" s="12"/>
-      <c r="AC46" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD46" s="250" t="n">
+      <c r="AC46" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD46" s="251" t="n">
         <v>4.5</v>
       </c>
       <c r="AE46" s="12"/>
@@ -12134,15 +12176,15 @@
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="85" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="F47" s="85" t="s">
-        <v>551</v>
+        <v>556</v>
       </c>
       <c r="G47" s="35" t="s">
-        <v>552</v>
-      </c>
-      <c r="H47" s="197"/>
+        <v>557</v>
+      </c>
+      <c r="H47" s="198"/>
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
       <c r="K47" s="12"/>
@@ -12161,16 +12203,16 @@
       <c r="X47" s="12"/>
       <c r="Y47" s="12"/>
       <c r="Z47" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA47" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB47" s="12"/>
-      <c r="AC47" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD47" s="250" t="n">
+      <c r="AC47" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD47" s="251" t="n">
         <v>4.5</v>
       </c>
       <c r="AE47" s="12"/>
@@ -12183,13 +12225,13 @@
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="85" t="s">
-        <v>553</v>
+        <v>558</v>
       </c>
       <c r="F48" s="85" t="s">
-        <v>554</v>
+        <v>559</v>
       </c>
       <c r="G48" s="12"/>
-      <c r="H48" s="197"/>
+      <c r="H48" s="198"/>
       <c r="I48" s="12"/>
       <c r="J48" s="12"/>
       <c r="K48" s="12"/>
@@ -12208,16 +12250,16 @@
       <c r="X48" s="12"/>
       <c r="Y48" s="12"/>
       <c r="Z48" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA48" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AB48" s="12"/>
-      <c r="AC48" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD48" s="250" t="n">
+      <c r="AC48" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD48" s="251" t="n">
         <v>4.5</v>
       </c>
       <c r="AE48" s="12"/>
@@ -12230,13 +12272,13 @@
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="85" t="s">
-        <v>555</v>
+        <v>560</v>
       </c>
       <c r="F49" s="85" t="s">
-        <v>556</v>
+        <v>561</v>
       </c>
       <c r="G49" s="12"/>
-      <c r="H49" s="197"/>
+      <c r="H49" s="198"/>
       <c r="I49" s="12"/>
       <c r="J49" s="12"/>
       <c r="K49" s="12"/>
@@ -12255,16 +12297,16 @@
       <c r="X49" s="12"/>
       <c r="Y49" s="12"/>
       <c r="Z49" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA49" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AB49" s="12"/>
-      <c r="AC49" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD49" s="250" t="n">
+      <c r="AC49" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD49" s="251" t="n">
         <v>4</v>
       </c>
       <c r="AE49" s="12"/>
@@ -12277,13 +12319,13 @@
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="85" t="s">
-        <v>557</v>
+        <v>562</v>
       </c>
       <c r="F50" s="85" t="s">
-        <v>558</v>
+        <v>563</v>
       </c>
       <c r="G50" s="12"/>
-      <c r="H50" s="197"/>
+      <c r="H50" s="198"/>
       <c r="I50" s="12"/>
       <c r="J50" s="12"/>
       <c r="K50" s="12"/>
@@ -12302,16 +12344,16 @@
       <c r="X50" s="12"/>
       <c r="Y50" s="12"/>
       <c r="Z50" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA50" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AB50" s="12"/>
-      <c r="AC50" s="240" t="s">
-        <v>469</v>
-      </c>
-      <c r="AD50" s="250" t="n">
+      <c r="AC50" s="241" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD50" s="251" t="n">
         <v>4</v>
       </c>
       <c r="AE50" s="12"/>
@@ -12321,14 +12363,14 @@
     <row r="51" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
-      <c r="C51" s="192" t="s">
-        <v>559</v>
-      </c>
-      <c r="D51" s="192"/>
+      <c r="C51" s="193" t="s">
+        <v>564</v>
+      </c>
+      <c r="D51" s="193"/>
       <c r="E51" s="85"/>
       <c r="F51" s="85"/>
       <c r="G51" s="12"/>
-      <c r="H51" s="197"/>
+      <c r="H51" s="198"/>
       <c r="I51" s="12"/>
       <c r="J51" s="12"/>
       <c r="K51" s="12"/>
@@ -12349,8 +12391,8 @@
       <c r="Z51" s="39"/>
       <c r="AA51" s="84"/>
       <c r="AB51" s="12"/>
-      <c r="AC51" s="240"/>
-      <c r="AD51" s="250"/>
+      <c r="AC51" s="241"/>
+      <c r="AD51" s="251"/>
       <c r="AE51" s="12"/>
       <c r="AF51" s="12"/>
       <c r="AG51" s="12"/>
@@ -12360,13 +12402,13 @@
       <c r="B52" s="97"/>
       <c r="C52" s="12"/>
       <c r="E52" s="85" t="s">
-        <v>560</v>
+        <v>565</v>
       </c>
       <c r="F52" s="85" t="s">
-        <v>561</v>
+        <v>566</v>
       </c>
       <c r="G52" s="12"/>
-      <c r="H52" s="197"/>
+      <c r="H52" s="198"/>
       <c r="I52" s="12"/>
       <c r="J52" s="12"/>
       <c r="K52" s="12"/>
@@ -12385,14 +12427,14 @@
       <c r="X52" s="12"/>
       <c r="Y52" s="12"/>
       <c r="Z52" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA52" s="84" t="n">
         <v>3.5</v>
       </c>
       <c r="AB52" s="12"/>
       <c r="AC52" s="12"/>
-      <c r="AD52" s="250"/>
+      <c r="AD52" s="251"/>
       <c r="AE52" s="12"/>
       <c r="AF52" s="12"/>
       <c r="AG52" s="12"/>
@@ -12403,15 +12445,15 @@
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="85" t="s">
-        <v>562</v>
+        <v>567</v>
       </c>
       <c r="F53" s="85" t="s">
-        <v>563</v>
+        <v>568</v>
       </c>
       <c r="G53" s="35" t="s">
-        <v>564</v>
-      </c>
-      <c r="H53" s="197"/>
+        <v>569</v>
+      </c>
+      <c r="H53" s="198"/>
       <c r="I53" s="12"/>
       <c r="J53" s="12"/>
       <c r="K53" s="12"/>
@@ -12432,14 +12474,14 @@
       <c r="X53" s="12"/>
       <c r="Y53" s="12"/>
       <c r="Z53" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA53" s="84" t="n">
         <v>3.5</v>
       </c>
       <c r="AB53" s="12"/>
       <c r="AC53" s="12"/>
-      <c r="AD53" s="250"/>
+      <c r="AD53" s="251"/>
       <c r="AE53" s="12"/>
       <c r="AF53" s="12"/>
       <c r="AG53" s="12"/>
@@ -12450,15 +12492,15 @@
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="85" t="s">
-        <v>565</v>
+        <v>570</v>
       </c>
       <c r="F54" s="85" t="s">
-        <v>566</v>
+        <v>571</v>
       </c>
       <c r="G54" s="35" t="s">
-        <v>567</v>
-      </c>
-      <c r="H54" s="197"/>
+        <v>572</v>
+      </c>
+      <c r="H54" s="198"/>
       <c r="I54" s="12"/>
       <c r="J54" s="12"/>
       <c r="K54" s="12"/>
@@ -12479,14 +12521,14 @@
       <c r="X54" s="12"/>
       <c r="Y54" s="12"/>
       <c r="Z54" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA54" s="84" t="n">
         <v>4</v>
       </c>
       <c r="AB54" s="12"/>
       <c r="AC54" s="12"/>
-      <c r="AD54" s="250"/>
+      <c r="AD54" s="251"/>
       <c r="AE54" s="12"/>
       <c r="AF54" s="12"/>
       <c r="AG54" s="12"/>
@@ -12497,15 +12539,15 @@
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="85" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="F55" s="85" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="G55" s="35" t="s">
-        <v>570</v>
-      </c>
-      <c r="H55" s="197"/>
+        <v>575</v>
+      </c>
+      <c r="H55" s="198"/>
       <c r="I55" s="12"/>
       <c r="J55" s="12"/>
       <c r="K55" s="12"/>
@@ -12526,14 +12568,14 @@
       <c r="X55" s="12"/>
       <c r="Y55" s="12"/>
       <c r="Z55" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA55" s="84" t="n">
         <v>3.5</v>
       </c>
       <c r="AB55" s="12"/>
       <c r="AC55" s="12"/>
-      <c r="AD55" s="250"/>
+      <c r="AD55" s="251"/>
       <c r="AE55" s="12"/>
       <c r="AF55" s="12"/>
       <c r="AG55" s="12"/>
@@ -12544,15 +12586,15 @@
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
       <c r="E56" s="61" t="s">
-        <v>571</v>
+        <v>576</v>
       </c>
       <c r="F56" s="61" t="s">
-        <v>572</v>
+        <v>577</v>
       </c>
       <c r="G56" s="51" t="s">
-        <v>573</v>
-      </c>
-      <c r="H56" s="197"/>
+        <v>578</v>
+      </c>
+      <c r="H56" s="198"/>
       <c r="I56" s="12"/>
       <c r="J56" s="12"/>
       <c r="K56" s="12"/>
@@ -12573,14 +12615,14 @@
       <c r="X56" s="12"/>
       <c r="Y56" s="12"/>
       <c r="Z56" s="39" t="s">
-        <v>477</v>
+        <v>482</v>
       </c>
       <c r="AA56" s="44" t="n">
         <v>4</v>
       </c>
       <c r="AB56" s="12"/>
       <c r="AC56" s="12"/>
-      <c r="AD56" s="250"/>
+      <c r="AD56" s="251"/>
       <c r="AE56" s="12"/>
       <c r="AF56" s="12"/>
       <c r="AG56" s="12"/>

</xml_diff>

<commit_message>
Supporto hidden per items
</commit_message>
<xml_diff>
--- a/excel/DATABASE_MENU_VENDITA.xlsx
+++ b/excel/DATABASE_MENU_VENDITA.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="580">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="583">
   <si>
     <t xml:space="preserve">macro-category:</t>
   </si>
@@ -387,6 +387,15 @@
   </si>
   <si>
     <t xml:space="preserve">heink_bot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SIDRO MAGNERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">magners</t>
+  </si>
+  <si>
+    <t xml:space="preserve">magn_me</t>
   </si>
   <si>
     <t xml:space="preserve">Macro-category:</t>
@@ -3212,8 +3221,8 @@
   </sheetPr>
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y6" activeCellId="0" sqref="Y6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AA25" activeCellId="0" sqref="AA25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3224,7 +3233,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="28.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="63.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="8.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="7.15"/>
@@ -3846,7 +3855,9 @@
       <c r="V12" s="35"/>
       <c r="W12" s="35"/>
       <c r="X12" s="37"/>
-      <c r="Y12" s="37"/>
+      <c r="Y12" s="37" t="n">
+        <v>1</v>
+      </c>
       <c r="Z12" s="61" t="s">
         <v>76</v>
       </c>
@@ -4002,7 +4013,9 @@
       <c r="V15" s="35"/>
       <c r="W15" s="35"/>
       <c r="X15" s="37"/>
-      <c r="Y15" s="37"/>
+      <c r="Y15" s="37" t="n">
+        <v>1</v>
+      </c>
       <c r="Z15" s="61"/>
       <c r="AA15" s="53"/>
       <c r="AB15" s="62"/>
@@ -4106,7 +4119,9 @@
       <c r="V17" s="35"/>
       <c r="W17" s="35"/>
       <c r="X17" s="37"/>
-      <c r="Y17" s="37"/>
+      <c r="Y17" s="37" t="n">
+        <v>1</v>
+      </c>
       <c r="Z17" s="61" t="s">
         <v>99</v>
       </c>
@@ -4258,7 +4273,9 @@
       <c r="V20" s="12"/>
       <c r="W20" s="12"/>
       <c r="X20" s="12"/>
-      <c r="Y20" s="12"/>
+      <c r="Y20" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="Z20" s="85" t="s">
         <v>111</v>
       </c>
@@ -4306,7 +4323,9 @@
       <c r="V21" s="35"/>
       <c r="W21" s="35"/>
       <c r="X21" s="46"/>
-      <c r="Y21" s="46"/>
+      <c r="Y21" s="46" t="n">
+        <v>1</v>
+      </c>
       <c r="Z21" s="82" t="s">
         <v>116</v>
       </c>
@@ -4354,7 +4373,9 @@
       <c r="V22" s="35"/>
       <c r="W22" s="35"/>
       <c r="X22" s="37"/>
-      <c r="Y22" s="37"/>
+      <c r="Y22" s="37" t="n">
+        <v>1</v>
+      </c>
       <c r="Z22" s="38" t="s">
         <v>120</v>
       </c>
@@ -4370,12 +4391,56 @@
       <c r="AH22" s="91"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="F23" s="0"/>
-      <c r="AA23" s="0"/>
-      <c r="AB23" s="0"/>
-      <c r="AC23" s="0"/>
-      <c r="AD23" s="0"/>
-      <c r="AE23" s="0"/>
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="85" t="s">
+        <v>121</v>
+      </c>
+      <c r="F23" s="82" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="H23" s="86"/>
+      <c r="I23" s="12"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="12"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="12"/>
+      <c r="N23" s="12"/>
+      <c r="O23" s="12"/>
+      <c r="P23" s="12"/>
+      <c r="Q23" s="12"/>
+      <c r="R23" s="12"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="83" t="n">
+        <v>1</v>
+      </c>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+      <c r="Y23" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="Z23" s="85" t="s">
+        <v>123</v>
+      </c>
+      <c r="AA23" s="87" t="s">
+        <v>56</v>
+      </c>
+      <c r="AB23" s="88" t="n">
+        <v>6</v>
+      </c>
+      <c r="AC23" s="89"/>
+      <c r="AD23" s="87"/>
+      <c r="AE23" s="88"/>
+      <c r="AF23" s="12"/>
+      <c r="AG23" s="12"/>
+      <c r="AH23" s="12"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AC25" s="92"/>
@@ -4498,10 +4563,10 @@
   </sheetPr>
   <dimension ref="A1:AH47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="Y20" activeCellId="0" sqref="Y20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="Y51" activeCellId="0" sqref="Y51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4510,7 +4575,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="100" width="42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="101" width="35.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="101" width="31.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="64.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="102" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="103" width="11.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="103" width="8"/>
@@ -4535,23 +4600,23 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="104" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B1" s="105"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="106" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B2" s="106" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D2" s="107"/>
       <c r="E2" s="108" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F2" s="108"/>
       <c r="G2" s="109"/>
@@ -4580,28 +4645,28 @@
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="112" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="112" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="46" t="s">
         <v>125</v>
-      </c>
-      <c r="B3" s="112" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="46" t="s">
-        <v>122</v>
       </c>
       <c r="D3" s="113" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="113" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="114" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H3" s="106" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I3" s="115"/>
       <c r="J3" s="115"/>
@@ -4623,25 +4688,25 @@
         <v>10</v>
       </c>
       <c r="Z3" s="46" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AA3" s="46" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AB3" s="46" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="12"/>
       <c r="B4" s="12" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="C4" s="117" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="D4" s="118" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="E4" s="46"/>
       <c r="F4" s="119"/>
@@ -4708,13 +4773,13 @@
       <c r="C5" s="117"/>
       <c r="D5" s="116"/>
       <c r="E5" s="124" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="F5" s="125" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="G5" s="126" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H5" s="127"/>
       <c r="I5" s="128"/>
@@ -4735,9 +4800,11 @@
       <c r="V5" s="128"/>
       <c r="W5" s="128"/>
       <c r="X5" s="128"/>
-      <c r="Y5" s="128"/>
+      <c r="Y5" s="128" t="n">
+        <v>1</v>
+      </c>
       <c r="Z5" s="125" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AA5" s="32"/>
       <c r="AB5" s="129" t="n">
@@ -4750,13 +4817,13 @@
       <c r="C6" s="128"/>
       <c r="D6" s="131"/>
       <c r="E6" s="132" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="F6" s="133" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="G6" s="134" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H6" s="127"/>
       <c r="I6" s="128"/>
@@ -4781,7 +4848,7 @@
       <c r="X6" s="128"/>
       <c r="Y6" s="128"/>
       <c r="Z6" s="133" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="AA6" s="38"/>
       <c r="AB6" s="129" t="n">
@@ -4794,13 +4861,13 @@
       <c r="C7" s="117"/>
       <c r="D7" s="116"/>
       <c r="E7" s="132" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F7" s="132" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G7" s="135" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H7" s="127"/>
       <c r="I7" s="128"/>
@@ -4827,7 +4894,7 @@
       <c r="X7" s="128"/>
       <c r="Y7" s="128"/>
       <c r="Z7" s="132" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="AA7" s="38"/>
       <c r="AB7" s="129" t="n">
@@ -4840,13 +4907,13 @@
       <c r="C8" s="117"/>
       <c r="D8" s="116"/>
       <c r="E8" s="132" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F8" s="132" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G8" s="135" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H8" s="136"/>
       <c r="I8" s="137"/>
@@ -4869,9 +4936,11 @@
       <c r="V8" s="137"/>
       <c r="W8" s="137"/>
       <c r="X8" s="137"/>
-      <c r="Y8" s="137"/>
+      <c r="Y8" s="137" t="n">
+        <v>1</v>
+      </c>
       <c r="Z8" s="132" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="AA8" s="38"/>
       <c r="AB8" s="129" t="n">
@@ -4889,13 +4958,13 @@
       <c r="C9" s="117"/>
       <c r="D9" s="116"/>
       <c r="E9" s="132" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="F9" s="132" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="G9" s="135" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H9" s="136"/>
       <c r="I9" s="137" t="n">
@@ -4920,9 +4989,11 @@
       <c r="V9" s="137"/>
       <c r="W9" s="137"/>
       <c r="X9" s="137"/>
-      <c r="Y9" s="137"/>
+      <c r="Y9" s="137" t="n">
+        <v>1</v>
+      </c>
       <c r="Z9" s="132" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="AA9" s="38"/>
       <c r="AB9" s="129" t="n">
@@ -4938,10 +5009,10 @@
       <c r="A10" s="130"/>
       <c r="B10" s="130"/>
       <c r="C10" s="117" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="D10" s="140" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="E10" s="132"/>
       <c r="F10" s="132"/>
@@ -4979,13 +5050,13 @@
       <c r="C11" s="117"/>
       <c r="D11" s="116"/>
       <c r="E11" s="132" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="F11" s="132" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="G11" s="135" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H11" s="142"/>
       <c r="I11" s="43"/>
@@ -5012,7 +5083,7 @@
       <c r="X11" s="43"/>
       <c r="Y11" s="43"/>
       <c r="Z11" s="132" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="AA11" s="38"/>
       <c r="AB11" s="129" t="n">
@@ -5025,13 +5096,13 @@
       <c r="C12" s="117"/>
       <c r="D12" s="116"/>
       <c r="E12" s="132" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="F12" s="133" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="G12" s="134" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H12" s="143"/>
       <c r="I12" s="144" t="n">
@@ -5056,9 +5127,11 @@
       <c r="V12" s="43"/>
       <c r="W12" s="43"/>
       <c r="X12" s="43"/>
-      <c r="Y12" s="43"/>
+      <c r="Y12" s="43" t="n">
+        <v>1</v>
+      </c>
       <c r="Z12" s="133" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="AA12" s="38"/>
       <c r="AB12" s="129" t="n">
@@ -5071,13 +5144,13 @@
       <c r="C13" s="117"/>
       <c r="D13" s="116"/>
       <c r="E13" s="132" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="F13" s="132" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="G13" s="135" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H13" s="142"/>
       <c r="I13" s="43"/>
@@ -5100,9 +5173,11 @@
       <c r="V13" s="43"/>
       <c r="W13" s="43"/>
       <c r="X13" s="43"/>
-      <c r="Y13" s="43"/>
+      <c r="Y13" s="43" t="n">
+        <v>1</v>
+      </c>
       <c r="Z13" s="132" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="AA13" s="38"/>
       <c r="AB13" s="129" t="n">
@@ -5115,13 +5190,13 @@
       <c r="C14" s="117"/>
       <c r="D14" s="116"/>
       <c r="E14" s="132" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="F14" s="133" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="G14" s="134" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H14" s="142"/>
       <c r="I14" s="43" t="n">
@@ -5144,9 +5219,11 @@
       <c r="V14" s="43"/>
       <c r="W14" s="43"/>
       <c r="X14" s="43"/>
-      <c r="Y14" s="43"/>
+      <c r="Y14" s="43" t="n">
+        <v>1</v>
+      </c>
       <c r="Z14" s="133" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="AA14" s="38"/>
       <c r="AB14" s="129" t="n">
@@ -5159,13 +5236,13 @@
       <c r="C15" s="117"/>
       <c r="D15" s="116"/>
       <c r="E15" s="132" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F15" s="132" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="G15" s="145" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H15" s="143"/>
       <c r="I15" s="144"/>
@@ -5190,7 +5267,7 @@
       <c r="X15" s="43"/>
       <c r="Y15" s="43"/>
       <c r="Z15" s="132" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="AA15" s="38"/>
       <c r="AB15" s="129" t="n">
@@ -5203,13 +5280,13 @@
       <c r="C16" s="117"/>
       <c r="D16" s="116"/>
       <c r="E16" s="132" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="F16" s="133" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="G16" s="134" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H16" s="142"/>
       <c r="I16" s="43"/>
@@ -5234,9 +5311,11 @@
       <c r="V16" s="43"/>
       <c r="W16" s="43"/>
       <c r="X16" s="43"/>
-      <c r="Y16" s="43"/>
+      <c r="Y16" s="43" t="n">
+        <v>1</v>
+      </c>
       <c r="Z16" s="133" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="AA16" s="38"/>
       <c r="AB16" s="129" t="n">
@@ -5249,13 +5328,13 @@
       <c r="C17" s="117"/>
       <c r="D17" s="116"/>
       <c r="E17" s="132" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="F17" s="132" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G17" s="146" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H17" s="147"/>
       <c r="I17" s="148"/>
@@ -5284,7 +5363,7 @@
       <c r="X17" s="148"/>
       <c r="Y17" s="148"/>
       <c r="Z17" s="132" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="AA17" s="38"/>
       <c r="AB17" s="129" t="n">
@@ -5297,13 +5376,13 @@
       <c r="C18" s="117"/>
       <c r="D18" s="116"/>
       <c r="E18" s="132" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="F18" s="132" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="G18" s="135" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H18" s="143"/>
       <c r="I18" s="144" t="n">
@@ -5328,7 +5407,7 @@
       <c r="X18" s="144"/>
       <c r="Y18" s="144"/>
       <c r="Z18" s="132" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="AA18" s="38"/>
       <c r="AB18" s="129" t="n">
@@ -5341,13 +5420,13 @@
       <c r="C19" s="117"/>
       <c r="D19" s="116"/>
       <c r="E19" s="132" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F19" s="132" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G19" s="135" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="H19" s="143"/>
       <c r="I19" s="144" t="n">
@@ -5374,9 +5453,11 @@
       <c r="V19" s="144"/>
       <c r="W19" s="144"/>
       <c r="X19" s="144"/>
-      <c r="Y19" s="144"/>
+      <c r="Y19" s="144" t="n">
+        <v>1</v>
+      </c>
       <c r="Z19" s="132" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="AA19" s="38"/>
       <c r="AB19" s="129" t="n">
@@ -5387,10 +5468,10 @@
       <c r="A20" s="12"/>
       <c r="B20" s="12"/>
       <c r="C20" s="117" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="D20" s="82" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
@@ -5425,10 +5506,10 @@
       <c r="C21" s="117"/>
       <c r="D21" s="82"/>
       <c r="E21" s="38" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="F21" s="38" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="G21" s="83"/>
       <c r="H21" s="149"/>
@@ -5451,7 +5532,7 @@
       <c r="Y21" s="117"/>
       <c r="Z21" s="83"/>
       <c r="AA21" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB21" s="150" t="n">
         <v>2</v>
@@ -5463,10 +5544,10 @@
       <c r="C22" s="117"/>
       <c r="D22" s="82"/>
       <c r="E22" s="38" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="F22" s="38" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="G22" s="83"/>
       <c r="H22" s="149"/>
@@ -5489,7 +5570,7 @@
       <c r="Y22" s="117"/>
       <c r="Z22" s="83"/>
       <c r="AA22" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB22" s="150" t="n">
         <v>1.5</v>
@@ -5501,10 +5582,10 @@
       <c r="C23" s="117"/>
       <c r="D23" s="82"/>
       <c r="E23" s="38" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="F23" s="38" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="G23" s="83"/>
       <c r="H23" s="149"/>
@@ -5535,10 +5616,10 @@
       <c r="C24" s="117"/>
       <c r="D24" s="82"/>
       <c r="E24" s="38" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F24" s="38" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G24" s="83"/>
       <c r="H24" s="149"/>
@@ -5569,10 +5650,10 @@
       <c r="C25" s="117"/>
       <c r="D25" s="82"/>
       <c r="E25" s="38" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="F25" s="38" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="G25" s="83"/>
       <c r="H25" s="149"/>
@@ -5603,10 +5684,10 @@
       <c r="C26" s="117"/>
       <c r="D26" s="82"/>
       <c r="E26" s="38" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="F26" s="38" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="G26" s="83"/>
       <c r="H26" s="149"/>
@@ -5637,10 +5718,10 @@
       <c r="C27" s="117"/>
       <c r="D27" s="82"/>
       <c r="E27" s="38" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F27" s="38" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G27" s="83"/>
       <c r="H27" s="149"/>
@@ -5671,10 +5752,10 @@
       <c r="C28" s="117"/>
       <c r="D28" s="82"/>
       <c r="E28" s="38" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="F28" s="38" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="G28" s="83"/>
       <c r="H28" s="149"/>
@@ -5705,10 +5786,10 @@
       <c r="C29" s="117"/>
       <c r="D29" s="117"/>
       <c r="E29" s="38" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="G29" s="151"/>
       <c r="H29" s="149"/>
@@ -5731,7 +5812,7 @@
       <c r="Y29" s="117"/>
       <c r="Z29" s="83"/>
       <c r="AA29" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB29" s="150" t="n">
         <v>0.5</v>
@@ -5743,10 +5824,10 @@
       <c r="C30" s="117"/>
       <c r="D30" s="117"/>
       <c r="E30" s="38" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="G30" s="151"/>
       <c r="H30" s="149"/>
@@ -5771,7 +5852,7 @@
       <c r="Y30" s="117"/>
       <c r="Z30" s="83"/>
       <c r="AA30" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB30" s="150" t="n">
         <v>0.5</v>
@@ -5783,10 +5864,10 @@
       <c r="C31" s="117"/>
       <c r="D31" s="117"/>
       <c r="E31" s="38" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="F31" s="38" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="G31" s="151"/>
       <c r="H31" s="149"/>
@@ -5811,7 +5892,7 @@
       <c r="Y31" s="117"/>
       <c r="Z31" s="83"/>
       <c r="AA31" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB31" s="150" t="n">
         <v>1</v>
@@ -5823,10 +5904,10 @@
       <c r="C32" s="117"/>
       <c r="D32" s="117"/>
       <c r="E32" s="38" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="F32" s="38" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="G32" s="151"/>
       <c r="H32" s="149"/>
@@ -5851,7 +5932,7 @@
       <c r="Y32" s="117"/>
       <c r="Z32" s="83"/>
       <c r="AA32" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB32" s="150" t="n">
         <v>0.5</v>
@@ -5863,10 +5944,10 @@
       <c r="C33" s="117"/>
       <c r="D33" s="117"/>
       <c r="E33" s="38" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F33" s="38" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="G33" s="151"/>
       <c r="H33" s="149"/>
@@ -5889,7 +5970,7 @@
       <c r="Y33" s="117"/>
       <c r="Z33" s="83"/>
       <c r="AA33" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB33" s="150" t="n">
         <v>0.5</v>
@@ -5901,10 +5982,10 @@
       <c r="C34" s="117"/>
       <c r="D34" s="117"/>
       <c r="E34" s="38" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="F34" s="38" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="G34" s="151"/>
       <c r="H34" s="149"/>
@@ -5927,7 +6008,7 @@
       <c r="Y34" s="117"/>
       <c r="Z34" s="83"/>
       <c r="AA34" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB34" s="150" t="n">
         <v>0.5</v>
@@ -5939,10 +6020,10 @@
       <c r="C35" s="117"/>
       <c r="D35" s="117"/>
       <c r="E35" s="38" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="F35" s="38" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="G35" s="151"/>
       <c r="H35" s="149"/>
@@ -5965,7 +6046,7 @@
       <c r="Y35" s="117"/>
       <c r="Z35" s="83"/>
       <c r="AA35" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB35" s="150" t="n">
         <v>0.5</v>
@@ -5977,10 +6058,10 @@
       <c r="C36" s="117"/>
       <c r="D36" s="117"/>
       <c r="E36" s="38" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F36" s="38" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="G36" s="151"/>
       <c r="H36" s="149"/>
@@ -6003,7 +6084,7 @@
       <c r="Y36" s="117"/>
       <c r="Z36" s="83"/>
       <c r="AA36" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB36" s="150" t="n">
         <v>0.5</v>
@@ -6015,10 +6096,10 @@
       <c r="C37" s="117"/>
       <c r="D37" s="117"/>
       <c r="E37" s="38" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="F37" s="38" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="G37" s="151"/>
       <c r="H37" s="149"/>
@@ -6041,7 +6122,7 @@
       <c r="Y37" s="117"/>
       <c r="Z37" s="83"/>
       <c r="AA37" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB37" s="150" t="n">
         <v>0.5</v>
@@ -6053,10 +6134,10 @@
       <c r="C38" s="117"/>
       <c r="D38" s="117"/>
       <c r="E38" s="38" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="F38" s="38" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="G38" s="152"/>
       <c r="H38" s="149"/>
@@ -6079,7 +6160,7 @@
       <c r="Y38" s="117"/>
       <c r="Z38" s="83"/>
       <c r="AA38" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB38" s="150" t="n">
         <v>0.5</v>
@@ -6091,10 +6172,10 @@
       <c r="C39" s="117"/>
       <c r="D39" s="117"/>
       <c r="E39" s="38" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F39" s="38" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G39" s="152"/>
       <c r="H39" s="149"/>
@@ -6125,10 +6206,10 @@
       <c r="C40" s="117"/>
       <c r="D40" s="117"/>
       <c r="E40" s="38" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="F40" s="38" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="G40" s="151"/>
       <c r="H40" s="149"/>
@@ -6155,7 +6236,7 @@
       <c r="Y40" s="117"/>
       <c r="Z40" s="83"/>
       <c r="AA40" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB40" s="150" t="n">
         <v>0.5</v>
@@ -6167,10 +6248,10 @@
       <c r="C41" s="117"/>
       <c r="D41" s="117"/>
       <c r="E41" s="38" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="F41" s="38" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="G41" s="151"/>
       <c r="H41" s="149"/>
@@ -6195,7 +6276,7 @@
       <c r="Y41" s="117"/>
       <c r="Z41" s="83"/>
       <c r="AA41" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB41" s="150" t="n">
         <v>0.5</v>
@@ -6207,10 +6288,10 @@
       <c r="C42" s="117"/>
       <c r="D42" s="117"/>
       <c r="E42" s="38" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="F42" s="38" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="G42" s="151"/>
       <c r="H42" s="149"/>
@@ -6235,7 +6316,7 @@
       <c r="Y42" s="117"/>
       <c r="Z42" s="83"/>
       <c r="AA42" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB42" s="150" t="n">
         <v>0.5</v>
@@ -6247,10 +6328,10 @@
       <c r="C43" s="117"/>
       <c r="D43" s="117"/>
       <c r="E43" s="38" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="F43" s="38" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="G43" s="151"/>
       <c r="H43" s="149"/>
@@ -6275,7 +6356,7 @@
       <c r="Y43" s="117"/>
       <c r="Z43" s="83"/>
       <c r="AA43" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB43" s="150" t="n">
         <v>0.5</v>
@@ -6287,10 +6368,10 @@
       <c r="C44" s="117"/>
       <c r="D44" s="117"/>
       <c r="E44" s="38" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="F44" s="38" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="G44" s="151"/>
       <c r="H44" s="149"/>
@@ -6317,7 +6398,7 @@
       <c r="Y44" s="117"/>
       <c r="Z44" s="83"/>
       <c r="AA44" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB44" s="150" t="n">
         <v>0.5</v>
@@ -6329,10 +6410,10 @@
       <c r="C45" s="117"/>
       <c r="D45" s="117"/>
       <c r="E45" s="38" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="F45" s="38" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="G45" s="83"/>
       <c r="H45" s="149"/>
@@ -6357,7 +6438,7 @@
       <c r="Y45" s="117"/>
       <c r="Z45" s="83"/>
       <c r="AA45" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB45" s="150" t="n">
         <v>0.5</v>
@@ -6369,10 +6450,10 @@
       <c r="C46" s="117"/>
       <c r="D46" s="117"/>
       <c r="E46" s="38" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="F46" s="38" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="G46" s="83"/>
       <c r="H46" s="149"/>
@@ -6397,7 +6478,7 @@
       <c r="Y46" s="117"/>
       <c r="Z46" s="83"/>
       <c r="AA46" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB46" s="150" t="n">
         <v>0.5</v>
@@ -6409,10 +6490,10 @@
       <c r="C47" s="156"/>
       <c r="D47" s="117"/>
       <c r="E47" s="38" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="F47" s="38" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="G47" s="83"/>
       <c r="H47" s="149"/>
@@ -6437,7 +6518,7 @@
       <c r="Y47" s="117"/>
       <c r="Z47" s="83"/>
       <c r="AA47" s="83" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="AB47" s="150" t="n">
         <v>0.5</v>
@@ -6462,8 +6543,8 @@
   </sheetPr>
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H14" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="X37" activeCellId="0" sqref="X37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y31" activeCellId="0" sqref="Y31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6496,23 +6577,23 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="104" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B1" s="105"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="106" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B2" s="106" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="D2" s="107"/>
       <c r="E2" s="108" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F2" s="108"/>
       <c r="G2" s="109"/>
@@ -6541,28 +6622,28 @@
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="112" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="B3" s="112" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="D3" s="113" t="s">
         <v>3</v>
       </c>
       <c r="E3" s="113" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F3" s="18" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="114" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="H3" s="106" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="I3" s="115"/>
       <c r="J3" s="115"/>
@@ -6584,13 +6665,13 @@
         <v>10</v>
       </c>
       <c r="Z3" s="46" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="AA3" s="46" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="AB3" s="46" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6599,10 +6680,10 @@
       </c>
       <c r="B4" s="157"/>
       <c r="C4" s="158" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="D4" s="89" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="E4" s="113"/>
       <c r="F4" s="18"/>
@@ -6671,13 +6752,13 @@
       <c r="C5" s="12"/>
       <c r="D5" s="0"/>
       <c r="E5" s="32" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="G5" s="160" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="H5" s="23"/>
       <c r="I5" s="117"/>
@@ -6715,13 +6796,13 @@
       <c r="C6" s="46"/>
       <c r="D6" s="46"/>
       <c r="E6" s="32" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="F6" s="32" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="G6" s="160" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="H6" s="23"/>
       <c r="I6" s="117" t="n">
@@ -6761,13 +6842,13 @@
       <c r="C7" s="46"/>
       <c r="D7" s="46"/>
       <c r="E7" s="32" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="F7" s="32" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="G7" s="160" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="H7" s="23"/>
       <c r="I7" s="117"/>
@@ -6805,13 +6886,13 @@
       <c r="C8" s="46"/>
       <c r="D8" s="46"/>
       <c r="E8" s="32" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="F8" s="32" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="G8" s="160" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="H8" s="23"/>
       <c r="I8" s="117"/>
@@ -6849,13 +6930,13 @@
       <c r="C9" s="46"/>
       <c r="D9" s="46"/>
       <c r="E9" s="32" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="F9" s="32" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="G9" s="160" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="H9" s="23"/>
       <c r="I9" s="117" t="n">
@@ -6895,13 +6976,13 @@
       <c r="C10" s="46"/>
       <c r="D10" s="46"/>
       <c r="E10" s="32" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="F10" s="32" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="G10" s="160" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="H10" s="23"/>
       <c r="I10" s="117"/>
@@ -6939,13 +7020,13 @@
       <c r="C11" s="46"/>
       <c r="D11" s="46"/>
       <c r="E11" s="32" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="F11" s="32" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="G11" s="160" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="H11" s="23"/>
       <c r="I11" s="117"/>
@@ -6989,13 +7070,13 @@
       <c r="C12" s="46"/>
       <c r="D12" s="46"/>
       <c r="E12" s="32" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="F12" s="32" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="G12" s="160" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="H12" s="23"/>
       <c r="I12" s="117" t="n">
@@ -7041,13 +7122,13 @@
       <c r="C13" s="46"/>
       <c r="D13" s="46"/>
       <c r="E13" s="32" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F13" s="32" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G13" s="160" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="H13" s="23"/>
       <c r="I13" s="117"/>
@@ -7089,10 +7170,10 @@
       <c r="A14" s="162"/>
       <c r="B14" s="162"/>
       <c r="C14" s="163" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="D14" s="164" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="E14" s="38"/>
       <c r="F14" s="38"/>
@@ -7125,13 +7206,13 @@
       <c r="C15" s="117"/>
       <c r="D15" s="116"/>
       <c r="E15" s="132" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="F15" s="132" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="G15" s="33" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="H15" s="166"/>
       <c r="I15" s="117"/>
@@ -7167,13 +7248,13 @@
       <c r="C16" s="117"/>
       <c r="D16" s="116"/>
       <c r="E16" s="132" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="F16" s="132" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="G16" s="160" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
       <c r="H16" s="166"/>
       <c r="I16" s="43" t="n">
@@ -7213,13 +7294,13 @@
       <c r="C17" s="117"/>
       <c r="D17" s="116"/>
       <c r="E17" s="132" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
       <c r="F17" s="132" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="G17" s="70" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="H17" s="166"/>
       <c r="I17" s="117"/>
@@ -7257,13 +7338,13 @@
       <c r="C18" s="117"/>
       <c r="D18" s="116"/>
       <c r="E18" s="132" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="F18" s="132" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="G18" s="51" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="H18" s="168"/>
       <c r="I18" s="117"/>
@@ -7297,10 +7378,10 @@
       <c r="A19" s="165"/>
       <c r="B19" s="165"/>
       <c r="C19" s="169" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="D19" s="170" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="E19" s="132"/>
       <c r="F19" s="132"/>
@@ -7333,10 +7414,10 @@
       <c r="C20" s="117"/>
       <c r="D20" s="117"/>
       <c r="E20" s="82" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="F20" s="173" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="G20" s="174"/>
       <c r="H20" s="175"/>
@@ -7371,10 +7452,10 @@
       <c r="C21" s="117"/>
       <c r="D21" s="116"/>
       <c r="E21" s="132" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F21" s="132" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="G21" s="35"/>
       <c r="H21" s="178"/>
@@ -7411,10 +7492,10 @@
       <c r="C22" s="117"/>
       <c r="D22" s="116"/>
       <c r="E22" s="132" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="F22" s="132" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="G22" s="35"/>
       <c r="H22" s="178"/>
@@ -7451,10 +7532,10 @@
       <c r="C23" s="117"/>
       <c r="D23" s="116"/>
       <c r="E23" s="132" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="F23" s="132" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="G23" s="35"/>
       <c r="H23" s="178"/>
@@ -7491,10 +7572,10 @@
       <c r="C24" s="117"/>
       <c r="D24" s="116"/>
       <c r="E24" s="132" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="F24" s="132" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="G24" s="35"/>
       <c r="H24" s="178"/>
@@ -7535,13 +7616,13 @@
       <c r="C25" s="117"/>
       <c r="D25" s="116"/>
       <c r="E25" s="132" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="F25" s="132" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="H25" s="178"/>
       <c r="I25" s="39" t="n">
@@ -7583,13 +7664,13 @@
       <c r="C26" s="117"/>
       <c r="D26" s="116"/>
       <c r="E26" s="132" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="F26" s="132" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="G26" s="179" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
       <c r="H26" s="178"/>
       <c r="I26" s="39" t="n">
@@ -7633,10 +7714,10 @@
       <c r="A27" s="162"/>
       <c r="B27" s="162"/>
       <c r="C27" s="180" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="D27" s="164" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="H27" s="166"/>
       <c r="I27" s="117"/>
@@ -7666,13 +7747,13 @@
       <c r="C28" s="117"/>
       <c r="D28" s="117"/>
       <c r="E28" s="32" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="F28" s="32" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="G28" s="181" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="H28" s="182"/>
       <c r="I28" s="39"/>
@@ -7712,13 +7793,13 @@
       <c r="C29" s="117"/>
       <c r="D29" s="117"/>
       <c r="E29" s="38" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="F29" s="38" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="G29" s="181" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="H29" s="183"/>
       <c r="I29" s="117"/>
@@ -7758,13 +7839,13 @@
       <c r="C30" s="117"/>
       <c r="D30" s="117"/>
       <c r="E30" s="38" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="F30" s="38" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="G30" s="184" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="H30" s="185"/>
       <c r="I30" s="117"/>
@@ -7796,10 +7877,10 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C31" s="180" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="D31" s="100" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="Y31" s="103" t="n">
         <v>1</v>
@@ -7807,13 +7888,13 @@
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E32" s="101" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="F32" s="101" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="AB32" s="186" t="n">
         <v>30</v>
@@ -7949,10 +8030,10 @@
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="112" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="B3" s="112" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>2</v>
@@ -7970,7 +8051,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -8019,10 +8100,10 @@
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="193" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="D4" s="194" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="H4" s="121" t="s">
         <v>20</v>
@@ -8092,13 +8173,13 @@
       <c r="C5" s="151"/>
       <c r="D5" s="151"/>
       <c r="E5" s="196" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="F5" s="196" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="G5" s="197" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="H5" s="198"/>
       <c r="I5" s="12"/>
@@ -8136,13 +8217,13 @@
       <c r="C6" s="151"/>
       <c r="D6" s="151"/>
       <c r="E6" s="196" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="F6" s="196" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="G6" s="197" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="H6" s="198"/>
       <c r="I6" s="12"/>
@@ -8180,13 +8261,13 @@
       <c r="C7" s="151"/>
       <c r="D7" s="151"/>
       <c r="E7" s="196" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="F7" s="196" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="G7" s="197" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="H7" s="198"/>
       <c r="I7" s="12"/>
@@ -8224,13 +8305,13 @@
       <c r="C8" s="151"/>
       <c r="D8" s="151"/>
       <c r="E8" s="196" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="F8" s="196" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="G8" s="160" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="H8" s="198"/>
       <c r="I8" s="12"/>
@@ -8268,13 +8349,13 @@
       <c r="C9" s="151"/>
       <c r="D9" s="151"/>
       <c r="E9" s="196" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="F9" s="196" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="G9" s="160" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="H9" s="198"/>
       <c r="I9" s="12"/>
@@ -8312,13 +8393,13 @@
       <c r="C10" s="151"/>
       <c r="D10" s="151"/>
       <c r="E10" s="196" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
       <c r="F10" s="196" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="G10" s="197" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="H10" s="198"/>
       <c r="I10" s="12"/>
@@ -8356,10 +8437,10 @@
       <c r="C11" s="151"/>
       <c r="D11" s="151"/>
       <c r="E11" s="196" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F11" s="196" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="G11" s="160"/>
       <c r="H11" s="198"/>
@@ -8382,21 +8463,21 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="23"/>
       <c r="AA11" s="201" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="AB11" s="42" t="n">
         <v>7</v>
       </c>
       <c r="AC11" s="23"/>
       <c r="AD11" s="201" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="AE11" s="65" t="n">
         <v>9</v>
       </c>
       <c r="AF11" s="23"/>
       <c r="AG11" s="160" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="AH11" s="65" t="n">
         <v>10</v>
@@ -8408,10 +8489,10 @@
       <c r="C12" s="151"/>
       <c r="D12" s="151"/>
       <c r="E12" s="196" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="F12" s="196" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="G12" s="160"/>
       <c r="H12" s="198"/>
@@ -8434,14 +8515,14 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="23"/>
       <c r="AA12" s="201" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="AB12" s="42" t="n">
         <v>6</v>
       </c>
       <c r="AC12" s="23"/>
       <c r="AD12" s="201" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="AE12" s="65" t="n">
         <v>11</v>
@@ -8456,13 +8537,13 @@
       <c r="C13" s="151"/>
       <c r="D13" s="151"/>
       <c r="E13" s="196" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="F13" s="196" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
       <c r="G13" s="160" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="H13" s="198"/>
       <c r="I13" s="12"/>
@@ -8498,13 +8579,13 @@
       <c r="A14" s="23"/>
       <c r="B14" s="105"/>
       <c r="E14" s="196" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="F14" s="196" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="G14" s="197" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="H14" s="198"/>
       <c r="I14" s="12"/>
@@ -8542,13 +8623,13 @@
       <c r="C15" s="151"/>
       <c r="D15" s="151"/>
       <c r="E15" s="196" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="F15" s="196" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="G15" s="197" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="H15" s="198"/>
       <c r="I15" s="12"/>
@@ -8586,13 +8667,13 @@
       <c r="C16" s="151"/>
       <c r="D16" s="151"/>
       <c r="E16" s="196" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="F16" s="196" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="G16" s="197" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="H16" s="198"/>
       <c r="I16" s="12"/>
@@ -8630,13 +8711,13 @@
       <c r="C17" s="151"/>
       <c r="D17" s="151"/>
       <c r="E17" s="196" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="F17" s="196" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="G17" s="197" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="H17" s="198"/>
       <c r="I17" s="12"/>
@@ -8674,13 +8755,13 @@
       <c r="C18" s="151"/>
       <c r="D18" s="202"/>
       <c r="E18" s="196" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="F18" s="196" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="G18" s="160" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="H18" s="198"/>
       <c r="I18" s="12"/>
@@ -8718,13 +8799,13 @@
       <c r="C19" s="151"/>
       <c r="D19" s="151"/>
       <c r="E19" s="196" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="F19" s="196" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="G19" s="203" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="H19" s="198"/>
       <c r="I19" s="12"/>
@@ -8762,13 +8843,13 @@
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
       <c r="E20" s="196" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="F20" s="196" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="G20" s="203" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="H20" s="198"/>
       <c r="I20" s="12"/>
@@ -8806,13 +8887,13 @@
       <c r="C21" s="12"/>
       <c r="D21" s="12"/>
       <c r="E21" s="196" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="F21" s="196" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="G21" s="203" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="H21" s="198"/>
       <c r="I21" s="12"/>
@@ -8848,10 +8929,10 @@
       <c r="A22" s="112"/>
       <c r="B22" s="112"/>
       <c r="C22" s="36" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="D22" s="204" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="10"/>
@@ -8890,13 +8971,13 @@
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
       <c r="E23" s="31" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="H23" s="205"/>
       <c r="I23" s="33"/>
@@ -8925,7 +9006,7 @@
       </c>
       <c r="AC23" s="209"/>
       <c r="AD23" s="209" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="AE23" s="208" t="n">
         <v>2</v>
@@ -8940,13 +9021,13 @@
       <c r="C24" s="12"/>
       <c r="D24" s="12"/>
       <c r="E24" s="31" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="F24" s="31" t="s">
+        <v>392</v>
+      </c>
+      <c r="G24" s="33" t="s">
         <v>389</v>
-      </c>
-      <c r="G24" s="33" t="s">
-        <v>386</v>
       </c>
       <c r="H24" s="205"/>
       <c r="I24" s="33"/>
@@ -8982,13 +9063,13 @@
       <c r="C25" s="12"/>
       <c r="D25" s="12"/>
       <c r="E25" s="31" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="F25" s="31" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="G25" s="33" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="H25" s="205"/>
       <c r="I25" s="33"/>
@@ -9017,7 +9098,7 @@
       </c>
       <c r="AC25" s="209"/>
       <c r="AD25" s="209" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="AE25" s="208" t="n">
         <v>4</v>
@@ -9032,13 +9113,13 @@
       <c r="C26" s="35"/>
       <c r="D26" s="35"/>
       <c r="E26" s="85" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="F26" s="85" t="s">
+        <v>398</v>
+      </c>
+      <c r="G26" s="33" t="s">
         <v>395</v>
-      </c>
-      <c r="G26" s="33" t="s">
-        <v>392</v>
       </c>
       <c r="H26" s="205"/>
       <c r="I26" s="33"/>
@@ -9078,13 +9159,13 @@
       <c r="C27" s="35"/>
       <c r="D27" s="35"/>
       <c r="E27" s="85" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="F27" s="85" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="G27" s="33" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="H27" s="205"/>
       <c r="I27" s="33"/>
@@ -9124,13 +9205,13 @@
       <c r="C28" s="35"/>
       <c r="D28" s="35"/>
       <c r="E28" s="85" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="F28" s="85" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="G28" s="33" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H28" s="205"/>
       <c r="I28" s="33"/>
@@ -9168,10 +9249,10 @@
       <c r="C29" s="35"/>
       <c r="D29" s="35"/>
       <c r="E29" s="85" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="F29" s="85" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="G29" s="33"/>
       <c r="H29" s="205"/>
@@ -9210,13 +9291,13 @@
       <c r="C30" s="35"/>
       <c r="D30" s="35"/>
       <c r="E30" s="60" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="F30" s="60" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="G30" s="33" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="H30" s="205"/>
       <c r="I30" s="33"/>
@@ -9254,13 +9335,13 @@
       <c r="C31" s="35"/>
       <c r="D31" s="35"/>
       <c r="E31" s="31" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="F31" s="31" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="G31" s="33" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H31" s="205"/>
       <c r="I31" s="33"/>
@@ -9298,13 +9379,13 @@
       <c r="C32" s="210"/>
       <c r="D32" s="210"/>
       <c r="E32" s="211" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="F32" s="61" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="G32" s="33" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H32" s="205"/>
       <c r="I32" s="33"/>
@@ -9342,13 +9423,13 @@
       <c r="C33" s="210"/>
       <c r="D33" s="210"/>
       <c r="E33" s="211" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="F33" s="61" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="G33" s="33" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="H33" s="205"/>
       <c r="I33" s="33"/>
@@ -9386,13 +9467,13 @@
       <c r="C34" s="35"/>
       <c r="D34" s="35"/>
       <c r="E34" s="31" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="F34" s="31" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="G34" s="33" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="H34" s="205"/>
       <c r="I34" s="33"/>
@@ -9430,13 +9511,13 @@
       <c r="C35" s="35"/>
       <c r="D35" s="35"/>
       <c r="E35" s="31" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="F35" s="31" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="G35" s="33" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="H35" s="205"/>
       <c r="I35" s="33"/>
@@ -9474,13 +9555,13 @@
       <c r="C36" s="35"/>
       <c r="D36" s="35"/>
       <c r="E36" s="31" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="F36" s="31" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="G36" s="33" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="H36" s="205"/>
       <c r="I36" s="33"/>
@@ -9518,13 +9599,13 @@
       <c r="C37" s="35"/>
       <c r="D37" s="35"/>
       <c r="E37" s="31" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="F37" s="31" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="G37" s="33" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="H37" s="205"/>
       <c r="I37" s="33"/>
@@ -9562,13 +9643,13 @@
       <c r="C38" s="35"/>
       <c r="D38" s="35"/>
       <c r="E38" s="31" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="G38" s="33" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="H38" s="205"/>
       <c r="I38" s="33"/>
@@ -9604,10 +9685,10 @@
       <c r="A39" s="29"/>
       <c r="B39" s="29"/>
       <c r="C39" s="212" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="D39" s="213" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="E39" s="12"/>
       <c r="G39" s="12"/>
@@ -9645,10 +9726,10 @@
       <c r="C40" s="12"/>
       <c r="D40" s="165"/>
       <c r="E40" s="215" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="F40" s="215" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="G40" s="51"/>
       <c r="H40" s="216"/>
@@ -9687,10 +9768,10 @@
       <c r="C41" s="12"/>
       <c r="D41" s="165"/>
       <c r="E41" s="215" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="F41" s="215" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="G41" s="51"/>
       <c r="H41" s="216"/>
@@ -9729,10 +9810,10 @@
       <c r="C42" s="12"/>
       <c r="D42" s="165"/>
       <c r="E42" s="215" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="F42" s="215" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="G42" s="51"/>
       <c r="H42" s="216"/>
@@ -9771,10 +9852,10 @@
       <c r="C43" s="12"/>
       <c r="D43" s="165"/>
       <c r="E43" s="215" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="F43" s="215" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="G43" s="218"/>
       <c r="H43" s="219"/>
@@ -9813,10 +9894,10 @@
       <c r="C44" s="12"/>
       <c r="D44" s="165"/>
       <c r="E44" s="215" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="F44" s="215" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="G44" s="185"/>
       <c r="H44" s="149"/>
@@ -9855,10 +9936,10 @@
       <c r="C45" s="12"/>
       <c r="D45" s="165"/>
       <c r="E45" s="215" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="F45" s="215" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="G45" s="185"/>
       <c r="H45" s="149"/>
@@ -9897,10 +9978,10 @@
       <c r="C46" s="12"/>
       <c r="D46" s="165"/>
       <c r="E46" s="215" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="F46" s="215" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="G46" s="185"/>
       <c r="H46" s="149"/>
@@ -9939,10 +10020,10 @@
       <c r="C47" s="12"/>
       <c r="D47" s="165"/>
       <c r="E47" s="215" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="F47" s="215" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="G47" s="185"/>
       <c r="H47" s="149"/>
@@ -9981,10 +10062,10 @@
       <c r="C48" s="12"/>
       <c r="D48" s="165"/>
       <c r="E48" s="215" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="F48" s="215" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="G48" s="185"/>
       <c r="H48" s="149"/>
@@ -10023,10 +10104,10 @@
       <c r="C49" s="12"/>
       <c r="D49" s="165"/>
       <c r="E49" s="215" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="F49" s="215" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="G49" s="185"/>
       <c r="H49" s="149"/>
@@ -10065,13 +10146,13 @@
       <c r="C50" s="12"/>
       <c r="D50" s="165"/>
       <c r="E50" s="215" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="F50" s="215" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="G50" s="221" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="H50" s="222"/>
       <c r="I50" s="223"/>
@@ -10236,10 +10317,10 @@
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="112" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="B3" s="83" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C3" s="228" t="s">
         <v>2</v>
@@ -10257,7 +10338,7 @@
         <v>7</v>
       </c>
       <c r="H3" s="85" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -10299,13 +10380,13 @@
         <v>16</v>
       </c>
       <c r="AF3" s="46" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="AG3" s="46" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="AH3" s="233" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10314,10 +10395,10 @@
       </c>
       <c r="B4" s="23"/>
       <c r="C4" s="193" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="D4" s="193" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="H4" s="121" t="s">
         <v>20</v>
@@ -10377,10 +10458,10 @@
       <c r="B5" s="105"/>
       <c r="C5" s="12"/>
       <c r="E5" s="234" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="F5" s="234" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="G5" s="235"/>
       <c r="H5" s="205"/>
@@ -10405,14 +10486,14 @@
       <c r="Y5" s="33"/>
       <c r="Z5" s="206"/>
       <c r="AA5" s="87" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="AB5" s="81" t="n">
         <v>5</v>
       </c>
       <c r="AC5" s="206"/>
       <c r="AD5" s="87" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="AE5" s="237" t="n">
         <v>15</v>
@@ -10427,10 +10508,10 @@
       <c r="C6" s="36"/>
       <c r="D6" s="36"/>
       <c r="E6" s="238" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="F6" s="238" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="G6" s="71"/>
       <c r="H6" s="205"/>
@@ -10455,14 +10536,14 @@
       <c r="Y6" s="33"/>
       <c r="Z6" s="23"/>
       <c r="AA6" s="87" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="AB6" s="81" t="n">
         <v>4</v>
       </c>
       <c r="AC6" s="23"/>
       <c r="AD6" s="87" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="AE6" s="237" t="n">
         <v>12</v>
@@ -10477,10 +10558,10 @@
       <c r="C7" s="36"/>
       <c r="D7" s="36"/>
       <c r="E7" s="60" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="F7" s="60" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="G7" s="51"/>
       <c r="H7" s="205"/>
@@ -10505,14 +10586,14 @@
       <c r="Y7" s="33"/>
       <c r="Z7" s="23"/>
       <c r="AA7" s="87" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="AB7" s="81" t="n">
         <v>4</v>
       </c>
       <c r="AC7" s="23"/>
       <c r="AD7" s="87" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="AE7" s="237" t="n">
         <v>12</v>
@@ -10527,10 +10608,10 @@
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
       <c r="E8" s="238" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="F8" s="238" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="G8" s="51"/>
       <c r="H8" s="205"/>
@@ -10555,14 +10636,14 @@
       <c r="Y8" s="33"/>
       <c r="Z8" s="23"/>
       <c r="AA8" s="87" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="AB8" s="81" t="n">
         <v>4</v>
       </c>
       <c r="AC8" s="23"/>
       <c r="AD8" s="87" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="AE8" s="237" t="n">
         <v>12</v>
@@ -10577,10 +10658,10 @@
       <c r="C9" s="35"/>
       <c r="D9" s="35"/>
       <c r="E9" s="238" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="F9" s="238" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="G9" s="71"/>
       <c r="H9" s="205"/>
@@ -10605,14 +10686,14 @@
       <c r="Y9" s="33"/>
       <c r="Z9" s="23"/>
       <c r="AA9" s="87" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="AB9" s="81" t="n">
         <v>4.5</v>
       </c>
       <c r="AC9" s="23"/>
       <c r="AD9" s="87" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="AE9" s="237" t="n">
         <v>14</v>
@@ -10625,10 +10706,10 @@
       <c r="A10" s="23"/>
       <c r="B10" s="23"/>
       <c r="C10" s="193" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="D10" s="194" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="H10" s="205"/>
       <c r="I10" s="33"/>
@@ -10659,10 +10740,10 @@
       <c r="C11" s="193"/>
       <c r="D11" s="193"/>
       <c r="E11" s="60" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="F11" s="60" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="G11" s="51"/>
       <c r="H11" s="205"/>
@@ -10685,7 +10766,7 @@
       <c r="Y11" s="33"/>
       <c r="Z11" s="23"/>
       <c r="AA11" s="87" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="AB11" s="81" t="n">
         <v>4</v>
@@ -10703,13 +10784,13 @@
       <c r="C12" s="36"/>
       <c r="D12" s="36"/>
       <c r="E12" s="238" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="F12" s="238" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="G12" s="71" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="H12" s="205"/>
       <c r="I12" s="33"/>
@@ -10731,7 +10812,7 @@
       <c r="Y12" s="33"/>
       <c r="Z12" s="23"/>
       <c r="AA12" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AB12" s="81" t="n">
         <v>5</v>
@@ -10749,13 +10830,13 @@
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
       <c r="E13" s="60" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="F13" s="60" t="s">
+        <v>480</v>
+      </c>
+      <c r="G13" s="51" t="s">
         <v>477</v>
-      </c>
-      <c r="G13" s="51" t="s">
-        <v>474</v>
       </c>
       <c r="H13" s="205"/>
       <c r="I13" s="33"/>
@@ -10777,7 +10858,7 @@
       <c r="Y13" s="33"/>
       <c r="Z13" s="23"/>
       <c r="AA13" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AB13" s="81" t="n">
         <v>5</v>
@@ -10793,10 +10874,10 @@
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="193" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="D14" s="193" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="E14" s="60"/>
       <c r="F14" s="60"/>
@@ -10833,13 +10914,13 @@
       <c r="A15" s="29"/>
       <c r="B15" s="243"/>
       <c r="E15" s="238" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="F15" s="238" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="G15" s="71" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="H15" s="216"/>
       <c r="I15" s="51"/>
@@ -10861,14 +10942,14 @@
       <c r="Y15" s="51"/>
       <c r="Z15" s="38"/>
       <c r="AA15" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB15" s="40" t="n">
         <v>3</v>
       </c>
       <c r="AC15" s="244"/>
       <c r="AD15" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE15" s="245" t="n">
         <v>5</v>
@@ -10883,13 +10964,13 @@
       <c r="C16" s="30"/>
       <c r="D16" s="30"/>
       <c r="E16" s="238" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="F16" s="238" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="G16" s="71" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="H16" s="216"/>
       <c r="I16" s="51"/>
@@ -10911,14 +10992,14 @@
       <c r="Y16" s="51"/>
       <c r="Z16" s="38"/>
       <c r="AA16" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB16" s="40" t="n">
         <v>3.5</v>
       </c>
       <c r="AC16" s="244"/>
       <c r="AD16" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE16" s="245" t="n">
         <v>6</v>
@@ -10933,13 +11014,13 @@
       <c r="C17" s="30"/>
       <c r="D17" s="30"/>
       <c r="E17" s="60" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="F17" s="60" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="G17" s="68" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="H17" s="219"/>
       <c r="I17" s="218"/>
@@ -10961,14 +11042,14 @@
       <c r="Y17" s="218"/>
       <c r="Z17" s="38"/>
       <c r="AA17" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB17" s="79" t="n">
         <v>4</v>
       </c>
       <c r="AC17" s="38"/>
       <c r="AD17" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE17" s="245" t="n">
         <v>7</v>
@@ -10983,13 +11064,13 @@
       <c r="C18" s="30"/>
       <c r="D18" s="30"/>
       <c r="E18" s="246" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="F18" s="246" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="G18" s="247" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="H18" s="149"/>
       <c r="I18" s="185"/>
@@ -11011,14 +11092,14 @@
       <c r="Y18" s="185"/>
       <c r="Z18" s="38"/>
       <c r="AA18" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB18" s="79" t="n">
         <v>4.5</v>
       </c>
       <c r="AC18" s="80"/>
       <c r="AD18" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE18" s="248" t="n">
         <v>8</v>
@@ -11033,13 +11114,13 @@
       <c r="C19" s="30"/>
       <c r="D19" s="30"/>
       <c r="E19" s="60" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="F19" s="60" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="G19" s="68" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="H19" s="149"/>
       <c r="I19" s="185"/>
@@ -11061,14 +11142,14 @@
       <c r="Y19" s="185"/>
       <c r="Z19" s="38"/>
       <c r="AA19" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB19" s="79" t="n">
         <v>3</v>
       </c>
       <c r="AC19" s="82"/>
       <c r="AD19" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE19" s="248" t="n">
         <v>5</v>
@@ -11083,13 +11164,13 @@
       <c r="C20" s="30"/>
       <c r="D20" s="30"/>
       <c r="E20" s="246" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="F20" s="246" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="G20" s="68" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="H20" s="149"/>
       <c r="I20" s="185"/>
@@ -11111,14 +11192,14 @@
       <c r="Y20" s="185"/>
       <c r="Z20" s="38"/>
       <c r="AA20" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB20" s="79" t="n">
         <v>4</v>
       </c>
       <c r="AC20" s="41"/>
       <c r="AD20" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE20" s="245" t="n">
         <v>7</v>
@@ -11133,13 +11214,13 @@
       <c r="C21" s="30"/>
       <c r="D21" s="30"/>
       <c r="E21" s="60" t="s">
+        <v>501</v>
+      </c>
+      <c r="F21" s="60" t="s">
+        <v>502</v>
+      </c>
+      <c r="G21" s="68" t="s">
         <v>498</v>
-      </c>
-      <c r="F21" s="60" t="s">
-        <v>499</v>
-      </c>
-      <c r="G21" s="68" t="s">
-        <v>495</v>
       </c>
       <c r="H21" s="149"/>
       <c r="I21" s="185"/>
@@ -11161,14 +11242,14 @@
       <c r="Y21" s="185"/>
       <c r="Z21" s="38"/>
       <c r="AA21" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB21" s="79" t="n">
         <v>4</v>
       </c>
       <c r="AC21" s="41"/>
       <c r="AD21" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE21" s="245" t="n">
         <v>7</v>
@@ -11183,13 +11264,13 @@
       <c r="C22" s="30"/>
       <c r="D22" s="30"/>
       <c r="E22" s="60" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="F22" s="60" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="G22" s="51" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="H22" s="149"/>
       <c r="I22" s="185"/>
@@ -11211,14 +11292,14 @@
       <c r="Y22" s="185"/>
       <c r="Z22" s="38"/>
       <c r="AA22" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB22" s="79" t="n">
         <v>5</v>
       </c>
       <c r="AC22" s="80"/>
       <c r="AD22" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE22" s="237" t="n">
         <v>8</v>
@@ -11233,13 +11314,13 @@
       <c r="C23" s="249"/>
       <c r="D23" s="249"/>
       <c r="E23" s="206" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="F23" s="206" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="G23" s="35" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="H23" s="222"/>
       <c r="I23" s="223"/>
@@ -11261,14 +11342,14 @@
       <c r="Y23" s="223"/>
       <c r="Z23" s="38"/>
       <c r="AA23" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB23" s="79" t="n">
         <v>5</v>
       </c>
       <c r="AC23" s="80"/>
       <c r="AD23" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE23" s="237" t="n">
         <v>8.5</v>
@@ -11283,13 +11364,13 @@
       <c r="C24" s="90"/>
       <c r="D24" s="90"/>
       <c r="E24" s="85" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="F24" s="85" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="G24" s="35" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="H24" s="198"/>
       <c r="I24" s="12"/>
@@ -11314,7 +11395,7 @@
       <c r="AB24" s="250"/>
       <c r="AC24" s="35"/>
       <c r="AD24" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE24" s="248" t="n">
         <v>4.5</v>
@@ -11329,13 +11410,13 @@
       <c r="C25" s="29"/>
       <c r="D25" s="29"/>
       <c r="E25" s="85" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="F25" s="85" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="G25" s="35" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="H25" s="198"/>
       <c r="I25" s="12"/>
@@ -11360,7 +11441,7 @@
       <c r="AB25" s="84"/>
       <c r="AC25" s="12"/>
       <c r="AD25" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE25" s="248" t="n">
         <v>4.5</v>
@@ -11375,13 +11456,13 @@
       <c r="C26" s="12"/>
       <c r="D26" s="12"/>
       <c r="E26" s="85" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="F26" s="85" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="G26" s="35" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="H26" s="198"/>
       <c r="I26" s="12"/>
@@ -11403,14 +11484,14 @@
       <c r="Y26" s="12"/>
       <c r="Z26" s="12"/>
       <c r="AA26" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB26" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AC26" s="12"/>
       <c r="AD26" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE26" s="251" t="n">
         <v>4.5</v>
@@ -11425,13 +11506,13 @@
       <c r="C27" s="12"/>
       <c r="D27" s="12"/>
       <c r="E27" s="85" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="F27" s="85" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="G27" s="35" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="H27" s="198"/>
       <c r="I27" s="12"/>
@@ -11453,14 +11534,14 @@
       <c r="Y27" s="12"/>
       <c r="Z27" s="12"/>
       <c r="AA27" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB27" s="84" t="n">
         <v>4.5</v>
       </c>
       <c r="AC27" s="12"/>
       <c r="AD27" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE27" s="251" t="n">
         <v>7.5</v>
@@ -11475,13 +11556,13 @@
       <c r="C28" s="12"/>
       <c r="D28" s="12"/>
       <c r="E28" s="85" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="F28" s="85" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="G28" s="35" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="H28" s="198"/>
       <c r="I28" s="12"/>
@@ -11503,14 +11584,14 @@
       <c r="Y28" s="12"/>
       <c r="Z28" s="12"/>
       <c r="AA28" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB28" s="84" t="n">
         <v>4.5</v>
       </c>
       <c r="AC28" s="12"/>
       <c r="AD28" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE28" s="251" t="n">
         <v>7.5</v>
@@ -11525,13 +11606,13 @@
       <c r="C29" s="12"/>
       <c r="D29" s="12"/>
       <c r="E29" s="85" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="F29" s="85" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="G29" s="35" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="H29" s="198"/>
       <c r="I29" s="12"/>
@@ -11553,14 +11634,14 @@
       <c r="Y29" s="12"/>
       <c r="Z29" s="12"/>
       <c r="AA29" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB29" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC29" s="12"/>
       <c r="AD29" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE29" s="251" t="n">
         <v>5</v>
@@ -11575,13 +11656,13 @@
       <c r="C30" s="12"/>
       <c r="D30" s="12"/>
       <c r="E30" s="85" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="F30" s="85" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="G30" s="35" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="H30" s="198"/>
       <c r="I30" s="12"/>
@@ -11603,14 +11684,14 @@
       <c r="Y30" s="12"/>
       <c r="Z30" s="12"/>
       <c r="AA30" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB30" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC30" s="12"/>
       <c r="AD30" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE30" s="251" t="n">
         <v>5</v>
@@ -11625,13 +11706,13 @@
       <c r="C31" s="12"/>
       <c r="D31" s="12"/>
       <c r="E31" s="85" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="F31" s="85" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="G31" s="35" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="H31" s="198"/>
       <c r="I31" s="12"/>
@@ -11653,14 +11734,14 @@
       <c r="Y31" s="12"/>
       <c r="Z31" s="12"/>
       <c r="AA31" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB31" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC31" s="12"/>
       <c r="AD31" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE31" s="251" t="n">
         <v>5</v>
@@ -11675,13 +11756,13 @@
       <c r="C32" s="12"/>
       <c r="D32" s="12"/>
       <c r="E32" s="85" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="F32" s="85" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="G32" s="35" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="H32" s="198"/>
       <c r="I32" s="12"/>
@@ -11703,14 +11784,14 @@
       <c r="Y32" s="12"/>
       <c r="Z32" s="12"/>
       <c r="AA32" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB32" s="84" t="n">
         <v>4</v>
       </c>
       <c r="AC32" s="12"/>
       <c r="AD32" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE32" s="251" t="n">
         <v>7</v>
@@ -11725,13 +11806,13 @@
       <c r="C33" s="12"/>
       <c r="D33" s="12"/>
       <c r="E33" s="85" t="s">
+        <v>531</v>
+      </c>
+      <c r="F33" s="85" t="s">
+        <v>532</v>
+      </c>
+      <c r="G33" s="35" t="s">
         <v>528</v>
-      </c>
-      <c r="F33" s="85" t="s">
-        <v>529</v>
-      </c>
-      <c r="G33" s="35" t="s">
-        <v>525</v>
       </c>
       <c r="H33" s="198"/>
       <c r="I33" s="12"/>
@@ -11753,14 +11834,14 @@
       <c r="Y33" s="12"/>
       <c r="Z33" s="12"/>
       <c r="AA33" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB33" s="84" t="n">
         <v>4.5</v>
       </c>
       <c r="AC33" s="12"/>
       <c r="AD33" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE33" s="251" t="n">
         <v>8</v>
@@ -11775,13 +11856,13 @@
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
       <c r="E34" s="85" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="F34" s="85" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="G34" s="35" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="H34" s="198"/>
       <c r="I34" s="12"/>
@@ -11803,14 +11884,14 @@
       <c r="Y34" s="12"/>
       <c r="Z34" s="12"/>
       <c r="AA34" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB34" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC34" s="12"/>
       <c r="AD34" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE34" s="251" t="n">
         <v>5</v>
@@ -11825,13 +11906,13 @@
       <c r="C35" s="12"/>
       <c r="D35" s="12"/>
       <c r="E35" s="85" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="F35" s="85" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="G35" s="35" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="H35" s="198"/>
       <c r="I35" s="12"/>
@@ -11853,14 +11934,14 @@
       <c r="Y35" s="12"/>
       <c r="Z35" s="12"/>
       <c r="AA35" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB35" s="84" t="n">
         <v>6</v>
       </c>
       <c r="AC35" s="12"/>
       <c r="AD35" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE35" s="251" t="n">
         <v>9.5</v>
@@ -11875,13 +11956,13 @@
       <c r="C36" s="12"/>
       <c r="D36" s="12"/>
       <c r="E36" s="246" t="s">
+        <v>538</v>
+      </c>
+      <c r="F36" s="85" t="s">
+        <v>539</v>
+      </c>
+      <c r="G36" s="35" t="s">
         <v>535</v>
-      </c>
-      <c r="F36" s="85" t="s">
-        <v>536</v>
-      </c>
-      <c r="G36" s="35" t="s">
-        <v>532</v>
       </c>
       <c r="H36" s="198"/>
       <c r="I36" s="12"/>
@@ -11903,14 +11984,14 @@
       <c r="Y36" s="12"/>
       <c r="Z36" s="12"/>
       <c r="AA36" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB36" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC36" s="12"/>
       <c r="AD36" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE36" s="251" t="n">
         <v>5</v>
@@ -11925,13 +12006,13 @@
       <c r="C37" s="12"/>
       <c r="D37" s="12"/>
       <c r="E37" s="85" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="F37" s="85" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="G37" s="35" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="H37" s="198"/>
       <c r="I37" s="12"/>
@@ -11953,14 +12034,14 @@
       <c r="Y37" s="12"/>
       <c r="Z37" s="12"/>
       <c r="AA37" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB37" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC37" s="12"/>
       <c r="AD37" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE37" s="251" t="n">
         <v>5</v>
@@ -11975,13 +12056,13 @@
       <c r="C38" s="12"/>
       <c r="D38" s="12"/>
       <c r="E38" s="85" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="F38" s="85" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="G38" s="35" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="H38" s="198"/>
       <c r="I38" s="12"/>
@@ -12003,14 +12084,14 @@
       <c r="Y38" s="12"/>
       <c r="Z38" s="12"/>
       <c r="AA38" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB38" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC38" s="12"/>
       <c r="AD38" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE38" s="251" t="n">
         <v>5</v>
@@ -12025,10 +12106,10 @@
       <c r="C39" s="12"/>
       <c r="D39" s="12"/>
       <c r="E39" s="85" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="F39" s="85" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="G39" s="35"/>
       <c r="H39" s="198"/>
@@ -12051,14 +12132,14 @@
       <c r="Y39" s="12"/>
       <c r="Z39" s="12"/>
       <c r="AA39" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB39" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC39" s="12"/>
       <c r="AD39" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE39" s="251" t="n">
         <v>4.5</v>
@@ -12073,10 +12154,10 @@
       <c r="C40" s="12"/>
       <c r="D40" s="12"/>
       <c r="E40" s="85" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="F40" s="85" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="G40" s="35"/>
       <c r="H40" s="198"/>
@@ -12099,14 +12180,14 @@
       <c r="Y40" s="12"/>
       <c r="Z40" s="12"/>
       <c r="AA40" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB40" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AC40" s="12"/>
       <c r="AD40" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE40" s="251" t="n">
         <v>4</v>
@@ -12121,10 +12202,10 @@
       <c r="C41" s="12"/>
       <c r="D41" s="12"/>
       <c r="E41" s="85" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="F41" s="85" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="G41" s="35"/>
       <c r="H41" s="198"/>
@@ -12147,14 +12228,14 @@
       <c r="Y41" s="12"/>
       <c r="Z41" s="12"/>
       <c r="AA41" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB41" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AC41" s="12"/>
       <c r="AD41" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE41" s="251" t="n">
         <v>4</v>
@@ -12169,10 +12250,10 @@
       <c r="C42" s="12"/>
       <c r="D42" s="12"/>
       <c r="E42" s="85" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="F42" s="85" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="G42" s="35"/>
       <c r="H42" s="198"/>
@@ -12195,14 +12276,14 @@
       <c r="Y42" s="12"/>
       <c r="Z42" s="12"/>
       <c r="AA42" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB42" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AC42" s="12"/>
       <c r="AD42" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE42" s="251" t="n">
         <v>4</v>
@@ -12215,7 +12296,7 @@
       <c r="A43" s="12"/>
       <c r="B43" s="12"/>
       <c r="C43" s="193" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="D43" s="193"/>
       <c r="E43" s="85"/>
@@ -12253,10 +12334,10 @@
       <c r="A44" s="12"/>
       <c r="B44" s="97"/>
       <c r="E44" s="85" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="F44" s="85" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="G44" s="12"/>
       <c r="H44" s="198"/>
@@ -12279,14 +12360,14 @@
       <c r="Y44" s="12"/>
       <c r="Z44" s="12"/>
       <c r="AA44" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB44" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC44" s="12"/>
       <c r="AD44" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE44" s="251" t="n">
         <v>4.5</v>
@@ -12301,10 +12382,10 @@
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
       <c r="E45" s="85" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="F45" s="85" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="G45" s="12"/>
       <c r="H45" s="198"/>
@@ -12327,14 +12408,14 @@
       <c r="Y45" s="12"/>
       <c r="Z45" s="12"/>
       <c r="AA45" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB45" s="84" t="n">
         <v>3.5</v>
       </c>
       <c r="AC45" s="12"/>
       <c r="AD45" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE45" s="251" t="n">
         <v>6</v>
@@ -12349,10 +12430,10 @@
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
       <c r="E46" s="85" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="F46" s="85" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="G46" s="12"/>
       <c r="H46" s="198"/>
@@ -12375,14 +12456,14 @@
       <c r="Y46" s="12"/>
       <c r="Z46" s="12"/>
       <c r="AA46" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB46" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC46" s="12"/>
       <c r="AD46" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE46" s="251" t="n">
         <v>4.5</v>
@@ -12397,13 +12478,13 @@
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
       <c r="E47" s="85" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="F47" s="85" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="G47" s="35" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="H47" s="198"/>
       <c r="I47" s="12"/>
@@ -12425,14 +12506,14 @@
       <c r="Y47" s="12"/>
       <c r="Z47" s="12"/>
       <c r="AA47" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB47" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC47" s="12"/>
       <c r="AD47" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE47" s="251" t="n">
         <v>4.5</v>
@@ -12447,10 +12528,10 @@
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>
       <c r="E48" s="85" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="F48" s="85" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="G48" s="12"/>
       <c r="H48" s="198"/>
@@ -12473,14 +12554,14 @@
       <c r="Y48" s="12"/>
       <c r="Z48" s="12"/>
       <c r="AA48" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB48" s="84" t="n">
         <v>3</v>
       </c>
       <c r="AC48" s="12"/>
       <c r="AD48" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE48" s="251" t="n">
         <v>4.5</v>
@@ -12495,10 +12576,10 @@
       <c r="C49" s="12"/>
       <c r="D49" s="12"/>
       <c r="E49" s="85" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="F49" s="85" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="G49" s="12"/>
       <c r="H49" s="198"/>
@@ -12521,14 +12602,14 @@
       <c r="Y49" s="12"/>
       <c r="Z49" s="12"/>
       <c r="AA49" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB49" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AC49" s="12"/>
       <c r="AD49" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE49" s="251" t="n">
         <v>4</v>
@@ -12543,10 +12624,10 @@
       <c r="C50" s="12"/>
       <c r="D50" s="12"/>
       <c r="E50" s="85" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="F50" s="85" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="G50" s="12"/>
       <c r="H50" s="198"/>
@@ -12569,14 +12650,14 @@
       <c r="Y50" s="12"/>
       <c r="Z50" s="12"/>
       <c r="AA50" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB50" s="84" t="n">
         <v>2.5</v>
       </c>
       <c r="AC50" s="12"/>
       <c r="AD50" s="241" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="AE50" s="251" t="n">
         <v>4</v>
@@ -12589,7 +12670,7 @@
       <c r="A51" s="12"/>
       <c r="B51" s="12"/>
       <c r="C51" s="193" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="D51" s="193"/>
       <c r="E51" s="85"/>
@@ -12628,10 +12709,10 @@
       <c r="B52" s="97"/>
       <c r="C52" s="12"/>
       <c r="E52" s="85" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="F52" s="85" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="G52" s="12"/>
       <c r="H52" s="198"/>
@@ -12654,7 +12735,7 @@
       <c r="Y52" s="12"/>
       <c r="Z52" s="12"/>
       <c r="AA52" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB52" s="84" t="n">
         <v>3.5</v>
@@ -12672,13 +12753,13 @@
       <c r="C53" s="12"/>
       <c r="D53" s="12"/>
       <c r="E53" s="85" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="F53" s="85" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="G53" s="35" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="H53" s="198"/>
       <c r="I53" s="12"/>
@@ -12702,7 +12783,7 @@
       <c r="Y53" s="12"/>
       <c r="Z53" s="12"/>
       <c r="AA53" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB53" s="84" t="n">
         <v>3.5</v>
@@ -12720,13 +12801,13 @@
       <c r="C54" s="12"/>
       <c r="D54" s="12"/>
       <c r="E54" s="85" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="F54" s="85" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="G54" s="35" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="H54" s="198"/>
       <c r="I54" s="12"/>
@@ -12750,7 +12831,7 @@
       <c r="Y54" s="12"/>
       <c r="Z54" s="12"/>
       <c r="AA54" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB54" s="84" t="n">
         <v>4</v>
@@ -12768,13 +12849,13 @@
       <c r="C55" s="12"/>
       <c r="D55" s="12"/>
       <c r="E55" s="85" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="F55" s="85" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="G55" s="35" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="H55" s="198"/>
       <c r="I55" s="12"/>
@@ -12798,7 +12879,7 @@
       <c r="Y55" s="12"/>
       <c r="Z55" s="12"/>
       <c r="AA55" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB55" s="84" t="n">
         <v>3.5</v>
@@ -12816,13 +12897,13 @@
       <c r="C56" s="12"/>
       <c r="D56" s="12"/>
       <c r="E56" s="61" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="F56" s="61" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="G56" s="51" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="H56" s="198"/>
       <c r="I56" s="12"/>
@@ -12846,7 +12927,7 @@
       <c r="Y56" s="12"/>
       <c r="Z56" s="12"/>
       <c r="AA56" s="39" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="AB56" s="44" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
Supporto hidden per items e subsection
</commit_message>
<xml_diff>
--- a/excel/DATABASE_MENU_VENDITA.xlsx
+++ b/excel/DATABASE_MENU_VENDITA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LE NOSTRE BIRRE" sheetId="1" state="visible" r:id="rId2"/>
@@ -3221,8 +3221,8 @@
   </sheetPr>
   <dimension ref="A1:AH45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AA25" activeCellId="0" sqref="AA25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y15" activeCellId="0" sqref="Y15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4563,10 +4563,10 @@
   </sheetPr>
   <dimension ref="A1:AH47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="Y51" activeCellId="0" sqref="Y51"/>
+      <selection pane="bottomLeft" activeCell="Y8" activeCellId="0" sqref="Y8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6543,8 +6543,8 @@
   </sheetPr>
   <dimension ref="A1:AC32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y31" activeCellId="0" sqref="Y31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y19" activeCellId="0" sqref="Y19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7235,7 +7235,9 @@
       <c r="V15" s="117"/>
       <c r="W15" s="117"/>
       <c r="X15" s="117"/>
-      <c r="Y15" s="117"/>
+      <c r="Y15" s="117" t="n">
+        <v>1</v>
+      </c>
       <c r="Z15" s="83"/>
       <c r="AA15" s="83"/>
       <c r="AB15" s="167" t="n">
@@ -7367,7 +7369,9 @@
       <c r="V18" s="117"/>
       <c r="W18" s="117"/>
       <c r="X18" s="117"/>
-      <c r="Y18" s="117"/>
+      <c r="Y18" s="117" t="n">
+        <v>1</v>
+      </c>
       <c r="Z18" s="83"/>
       <c r="AA18" s="83"/>
       <c r="AB18" s="167" t="n">
@@ -7519,7 +7523,9 @@
       <c r="V22" s="39"/>
       <c r="W22" s="39"/>
       <c r="X22" s="39"/>
-      <c r="Y22" s="39"/>
+      <c r="Y22" s="39" t="n">
+        <v>1</v>
+      </c>
       <c r="Z22" s="35"/>
       <c r="AA22" s="35"/>
       <c r="AB22" s="129" t="n">
@@ -7919,8 +7925,8 @@
   </sheetPr>
   <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="P1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y3" activeCellId="0" sqref="Y3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F10" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y49" activeCellId="0" sqref="Y49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8046875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9088,7 +9094,9 @@
       <c r="V25" s="33"/>
       <c r="W25" s="33"/>
       <c r="X25" s="33"/>
-      <c r="Y25" s="33"/>
+      <c r="Y25" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="Z25" s="206"/>
       <c r="AA25" s="207" t="s">
         <v>77</v>
@@ -9138,7 +9146,9 @@
       <c r="V26" s="33"/>
       <c r="W26" s="33"/>
       <c r="X26" s="33"/>
-      <c r="Y26" s="33"/>
+      <c r="Y26" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="Z26" s="206"/>
       <c r="AA26" s="207" t="s">
         <v>77</v>
@@ -9184,7 +9194,9 @@
       <c r="V27" s="33"/>
       <c r="W27" s="33"/>
       <c r="X27" s="33"/>
-      <c r="Y27" s="33"/>
+      <c r="Y27" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="Z27" s="206"/>
       <c r="AA27" s="207" t="s">
         <v>77</v>
@@ -9404,7 +9416,9 @@
       <c r="V32" s="33"/>
       <c r="W32" s="33"/>
       <c r="X32" s="33"/>
-      <c r="Y32" s="33"/>
+      <c r="Y32" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="Z32" s="206"/>
       <c r="AA32" s="207"/>
       <c r="AB32" s="208" t="n">
@@ -9448,7 +9462,9 @@
       <c r="V33" s="33"/>
       <c r="W33" s="33"/>
       <c r="X33" s="33"/>
-      <c r="Y33" s="33"/>
+      <c r="Y33" s="33" t="n">
+        <v>1</v>
+      </c>
       <c r="Z33" s="206"/>
       <c r="AA33" s="207"/>
       <c r="AB33" s="208" t="n">
@@ -9709,7 +9725,9 @@
       <c r="V39" s="12"/>
       <c r="W39" s="12"/>
       <c r="X39" s="12"/>
-      <c r="Y39" s="12"/>
+      <c r="Y39" s="12" t="n">
+        <v>1</v>
+      </c>
       <c r="Z39" s="12"/>
       <c r="AA39" s="12"/>
       <c r="AB39" s="214"/>
@@ -10205,7 +10223,7 @@
   </sheetPr>
   <dimension ref="A1:AH56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Z6" activeCellId="0" sqref="Z6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update menu e edit label
</commit_message>
<xml_diff>
--- a/excel/DATABASE_MENU_VENDITA.xlsx
+++ b/excel/DATABASE_MENU_VENDITA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LA BIRRERIA" sheetId="1" state="visible" r:id="rId2"/>
@@ -3374,11 +3374,11 @@
   </sheetPr>
   <dimension ref="A1:AH50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F31" activeCellId="0" sqref="F31"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D13" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y18" activeCellId="0" sqref="Y18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.99"/>
@@ -4269,7 +4269,9 @@
       <c r="V17" s="35"/>
       <c r="W17" s="35"/>
       <c r="X17" s="37"/>
-      <c r="Y17" s="37"/>
+      <c r="Y17" s="37" t="n">
+        <v>1</v>
+      </c>
       <c r="Z17" s="38" t="s">
         <v>94</v>
       </c>
@@ -4292,7 +4294,7 @@
       <c r="AG17" s="66"/>
       <c r="AH17" s="67"/>
     </row>
-    <row r="18" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29"/>
       <c r="B18" s="29"/>
       <c r="C18" s="30"/>
@@ -4323,9 +4325,7 @@
       <c r="V18" s="35"/>
       <c r="W18" s="35"/>
       <c r="X18" s="37"/>
-      <c r="Y18" s="37" t="n">
-        <v>1</v>
-      </c>
+      <c r="Y18" s="37"/>
       <c r="Z18" s="38" t="s">
         <v>99</v>
       </c>
@@ -4991,7 +4991,7 @@
       <selection pane="topLeft" activeCell="K22" activeCellId="0" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="100" width="42"/>
@@ -6747,13 +6747,13 @@
   </sheetPr>
   <dimension ref="A1:AH48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="4" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="37.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="100" width="42"/>
@@ -8769,7 +8769,7 @@
       <selection pane="topLeft" activeCell="E16" activeCellId="0" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="46.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="24.29"/>
@@ -11618,7 +11618,7 @@
       <selection pane="topLeft" activeCell="AH52" activeCellId="0" sqref="AH52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.03125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.0390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="41.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="19.42"/>

</xml_diff>

<commit_message>
piatti bavaresi e thumbs piadine
</commit_message>
<xml_diff>
--- a/excel/DATABASE_MENU_VENDITA.xlsx
+++ b/excel/DATABASE_MENU_VENDITA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="BIRRE" sheetId="1" state="visible" r:id="rId2"/>
@@ -229,13 +229,13 @@
     <t xml:space="preserve">33 cl</t>
   </si>
   <si>
-    <t xml:space="preserve">MASTINO - MONACO AMBER LAGER</t>
+    <t xml:space="preserve">BIRRIFICIO MASTINO - MONACO</t>
   </si>
   <si>
     <t xml:space="preserve">mastino_amber</t>
   </si>
   <si>
-    <t xml:space="preserve">Birra fresca e beverina dal colore rosso ambra, con profumi fruttati e leggermente tostati. Al palato sono i malti Monaco e il caramello a farsi sentire con finale secco e bilanciato. Gradazione 5,6°.</t>
+    <t xml:space="preserve">Amber lager fresca e beverina dal colore rosso ambra, con profumi fruttati e leggermente tostati. Al palato sono i malti Monaco e il caramello a farsi sentire con finale secco e bilanciato. Gradazione 5,6°.</t>
   </si>
   <si>
     <t xml:space="preserve">mastino_amber_p</t>
@@ -256,7 +256,7 @@
     <t xml:space="preserve">leffe_m</t>
   </si>
   <si>
-    <t xml:space="preserve">MASTIO - LITHA BLANCHE</t>
+    <t xml:space="preserve">IL MASTIO - LITHA BLANCHE</t>
   </si>
   <si>
     <t xml:space="preserve">blanche</t>
@@ -3391,8 +3391,8 @@
   </sheetPr>
   <dimension ref="A1:AH1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D7" activeCellId="0" sqref="D7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D8" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3867,7 +3867,7 @@
       <c r="AG8" s="57"/>
       <c r="AH8" s="58"/>
     </row>
-    <row r="9" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="127.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="59"/>
       <c r="B9" s="59"/>
       <c r="C9" s="13"/>
@@ -5172,8 +5172,8 @@
   </sheetPr>
   <dimension ref="A1:AC1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Menu update via menuPublish script
</commit_message>
<xml_diff>
--- a/excel/DATABASE_MENU_VENDITA.xlsx
+++ b/excel/DATABASE_MENU_VENDITA.xlsx
@@ -3624,8 +3624,8 @@
   </sheetPr>
   <dimension ref="A1:AH58"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D9" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y17" activeCellId="0" sqref="Y17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.06640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>